<commit_message>
Update 6845 CRTC timing spreadsheet with new adjustments
</commit_message>
<xml_diff>
--- a/6845_crtc_timing.xlsx
+++ b/6845_crtc_timing.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\iCloudDrive\Documents\Developer\BBC_Micro\Programs\Game_01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\iCloudDrive\Documents\Developer\BBC_Micro\Programs\Game_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1793971B-F411-4F02-81DC-28A033748BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7601B7DB-33C7-4F82-A7DC-05BB19A242AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{E881977C-AD55-4380-9786-6EB6D25147A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{E881977C-AD55-4380-9786-6EB6D25147A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="98">
   <si>
     <t>6845 CRTC Vertical Rupture Worksheet</t>
   </si>
@@ -256,6 +280,81 @@
   </si>
   <si>
     <t>Screen Layout</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Repeat</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Start Address (Hex)</t>
+  </si>
+  <si>
+    <t>Banks</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Bytes</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>2C00</t>
+  </si>
+  <si>
+    <t>V.Sync</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Scroll Offset</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Speed</t>
   </si>
 </sst>
 </file>
@@ -265,7 +364,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,8 +395,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -379,6 +484,84 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,7 +747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="215">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -703,12 +886,457 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="24" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="24" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="25" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="25" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="25" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="25" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="25" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="24" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="25" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="24" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="25" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="24" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FF33"/>
+      <color rgb="FF99FF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1040,29 +1668,29 @@
   <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="Q4" sqref="Q4:Q28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="4"/>
-    <col min="2" max="2" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="6.81640625" customWidth="1"/>
-    <col min="5" max="5" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="6.81640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="6.81640625" customWidth="1"/>
-    <col min="11" max="13" width="6.81640625" style="4" customWidth="1"/>
-    <col min="14" max="15" width="6.81640625" customWidth="1"/>
-    <col min="16" max="16" width="6.81640625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="10.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.81640625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="13.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="23" width="7.81640625" customWidth="1"/>
-    <col min="24" max="26" width="6.81640625" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="6.77734375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="6.77734375" customWidth="1"/>
+    <col min="11" max="13" width="6.77734375" style="4" customWidth="1"/>
+    <col min="14" max="15" width="6.77734375" customWidth="1"/>
+    <col min="16" max="16" width="6.77734375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="10.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.77734375" style="4" customWidth="1"/>
+    <col min="19" max="19" width="13.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="7.77734375" customWidth="1"/>
+    <col min="24" max="26" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:23" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1708,7 @@
       <c r="R1" s="3"/>
       <c r="S1" s="12"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="I2" s="3" t="s">
         <v>32</v>
       </c>
@@ -1107,7 +1735,7 @@
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1139,7 +1767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
@@ -1202,7 +1830,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>28</v>
       </c>
@@ -1250,7 +1878,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1289,7 +1917,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
@@ -1328,7 +1956,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="I8" s="22" t="s">
         <v>34</v>
       </c>
@@ -1365,7 +1993,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
@@ -1405,7 +2033,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>0</v>
       </c>
@@ -1454,7 +2082,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -1494,7 +2122,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>2</v>
       </c>
@@ -1543,7 +2171,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>3</v>
       </c>
@@ -1583,7 +2211,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -1629,7 +2257,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>4</v>
       </c>
@@ -1669,7 +2297,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>5</v>
       </c>
@@ -1718,7 +2346,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>6</v>
       </c>
@@ -1758,7 +2386,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>7</v>
       </c>
@@ -1807,7 +2435,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>8</v>
       </c>
@@ -1847,7 +2475,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -1893,7 +2521,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>16</v>
       </c>
@@ -1930,7 +2558,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>9</v>
       </c>
@@ -1979,7 +2607,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>10</v>
       </c>
@@ -2019,7 +2647,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>18</v>
       </c>
@@ -2065,7 +2693,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>19</v>
       </c>
@@ -2102,7 +2730,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>11</v>
       </c>
@@ -2151,7 +2779,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>12</v>
       </c>
@@ -2205,7 +2833,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>13</v>
       </c>
@@ -2258,18 +2886,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC23565D-C8C0-41CF-B4FA-F791AA87DEFC}">
   <dimension ref="A1:BQ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="5" width="5.6328125" style="4" customWidth="1"/>
-    <col min="6" max="69" width="4.7265625" customWidth="1"/>
-    <col min="70" max="133" width="8.7265625" customWidth="1"/>
+    <col min="4" max="5" width="5.6640625" style="4" customWidth="1"/>
+    <col min="6" max="69" width="4.77734375" customWidth="1"/>
+    <col min="70" max="133" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:69" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>72</v>
       </c>
@@ -2530,7 +3158,7 @@
         <v>7E</v>
       </c>
     </row>
-    <row r="2" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D2" s="26"/>
       <c r="E2" s="27"/>
       <c r="F2" s="37">
@@ -2789,7 +3417,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D3" s="23" t="str">
         <f>DEC2HEX(E3,2)</f>
         <v>00</v>
@@ -2862,7 +3490,7 @@
       <c r="BP3" s="54"/>
       <c r="BQ3" s="57"/>
     </row>
-    <row r="4" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D4" s="8" t="str">
         <f t="shared" ref="D4:D41" si="2">DEC2HEX(E4,2)</f>
         <v>01</v>
@@ -2936,7 +3564,7 @@
       <c r="BP4" s="56"/>
       <c r="BQ4" s="58"/>
     </row>
-    <row r="5" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D5" s="8" t="str">
         <f t="shared" si="2"/>
         <v>02</v>
@@ -3010,7 +3638,7 @@
       <c r="BP5" s="56"/>
       <c r="BQ5" s="58"/>
     </row>
-    <row r="6" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D6" s="8" t="str">
         <f t="shared" si="2"/>
         <v>03</v>
@@ -3084,7 +3712,7 @@
       <c r="BP6" s="56"/>
       <c r="BQ6" s="58"/>
     </row>
-    <row r="7" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="8" t="str">
         <f t="shared" si="2"/>
         <v>04</v>
@@ -3158,7 +3786,7 @@
       <c r="BP7" s="56"/>
       <c r="BQ7" s="58"/>
     </row>
-    <row r="8" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="8" t="str">
         <f t="shared" si="2"/>
         <v>05</v>
@@ -3232,7 +3860,7 @@
       <c r="BP8" s="56"/>
       <c r="BQ8" s="58"/>
     </row>
-    <row r="9" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D9" s="8" t="str">
         <f t="shared" si="2"/>
         <v>06</v>
@@ -3306,7 +3934,7 @@
       <c r="BP9" s="56"/>
       <c r="BQ9" s="58"/>
     </row>
-    <row r="10" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D10" s="8" t="str">
         <f t="shared" si="2"/>
         <v>07</v>
@@ -3380,7 +4008,7 @@
       <c r="BP10" s="56"/>
       <c r="BQ10" s="58"/>
     </row>
-    <row r="11" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D11" s="8" t="str">
         <f t="shared" si="2"/>
         <v>08</v>
@@ -3454,7 +4082,7 @@
       <c r="BP11" s="56"/>
       <c r="BQ11" s="58"/>
     </row>
-    <row r="12" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D12" s="8" t="str">
         <f t="shared" si="2"/>
         <v>09</v>
@@ -3528,7 +4156,7 @@
       <c r="BP12" s="56"/>
       <c r="BQ12" s="58"/>
     </row>
-    <row r="13" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D13" s="8" t="str">
         <f t="shared" si="2"/>
         <v>0A</v>
@@ -3602,7 +4230,7 @@
       <c r="BP13" s="56"/>
       <c r="BQ13" s="58"/>
     </row>
-    <row r="14" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="8" t="str">
         <f t="shared" si="2"/>
         <v>0B</v>
@@ -3676,7 +4304,7 @@
       <c r="BP14" s="56"/>
       <c r="BQ14" s="58"/>
     </row>
-    <row r="15" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D15" s="8" t="str">
         <f t="shared" si="2"/>
         <v>0C</v>
@@ -3750,7 +4378,7 @@
       <c r="BP15" s="56"/>
       <c r="BQ15" s="58"/>
     </row>
-    <row r="16" spans="1:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16" s="8" t="str">
         <f t="shared" si="2"/>
         <v>0D</v>
@@ -3824,7 +4452,7 @@
       <c r="BP16" s="56"/>
       <c r="BQ16" s="58"/>
     </row>
-    <row r="17" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="8" t="str">
         <f t="shared" si="2"/>
         <v>0E</v>
@@ -3898,7 +4526,7 @@
       <c r="BP17" s="56"/>
       <c r="BQ17" s="58"/>
     </row>
-    <row r="18" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D18" s="8" t="str">
         <f t="shared" si="2"/>
         <v>0F</v>
@@ -3972,7 +4600,7 @@
       <c r="BP18" s="56"/>
       <c r="BQ18" s="58"/>
     </row>
-    <row r="19" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D19" s="8" t="str">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -4046,7 +4674,7 @@
       <c r="BP19" s="56"/>
       <c r="BQ19" s="58"/>
     </row>
-    <row r="20" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D20" s="8" t="str">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -4120,7 +4748,7 @@
       <c r="BP20" s="56"/>
       <c r="BQ20" s="58"/>
     </row>
-    <row r="21" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="8" t="str">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -4194,7 +4822,7 @@
       <c r="BP21" s="56"/>
       <c r="BQ21" s="58"/>
     </row>
-    <row r="22" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D22" s="8" t="str">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -4268,7 +4896,7 @@
       <c r="BP22" s="56"/>
       <c r="BQ22" s="58"/>
     </row>
-    <row r="23" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D23" s="8" t="str">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -4342,7 +4970,7 @@
       <c r="BP23" s="56"/>
       <c r="BQ23" s="58"/>
     </row>
-    <row r="24" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="8" t="str">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -4416,7 +5044,7 @@
       <c r="BP24" s="56"/>
       <c r="BQ24" s="58"/>
     </row>
-    <row r="25" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D25" s="8" t="str">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -4490,7 +5118,7 @@
       <c r="BP25" s="56"/>
       <c r="BQ25" s="58"/>
     </row>
-    <row r="26" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D26" s="8" t="str">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -4564,7 +5192,7 @@
       <c r="BP26" s="56"/>
       <c r="BQ26" s="58"/>
     </row>
-    <row r="27" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D27" s="23" t="str">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -4638,7 +5266,7 @@
       <c r="BP27" s="54"/>
       <c r="BQ27" s="57"/>
     </row>
-    <row r="28" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D28" s="8" t="str">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -4712,7 +5340,7 @@
       <c r="BP28" s="56"/>
       <c r="BQ28" s="58"/>
     </row>
-    <row r="29" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D29" s="8" t="str">
         <f t="shared" si="2"/>
         <v>1A</v>
@@ -4786,7 +5414,7 @@
       <c r="BP29" s="56"/>
       <c r="BQ29" s="58"/>
     </row>
-    <row r="30" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D30" s="8" t="str">
         <f t="shared" si="2"/>
         <v>1B</v>
@@ -4860,7 +5488,7 @@
       <c r="BP30" s="56"/>
       <c r="BQ30" s="58"/>
     </row>
-    <row r="31" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D31" s="8" t="str">
         <f t="shared" si="2"/>
         <v>1C</v>
@@ -4934,7 +5562,7 @@
       <c r="BP31" s="56"/>
       <c r="BQ31" s="58"/>
     </row>
-    <row r="32" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D32" s="8" t="str">
         <f t="shared" si="2"/>
         <v>1D</v>
@@ -5008,7 +5636,7 @@
       <c r="BP32" s="56"/>
       <c r="BQ32" s="58"/>
     </row>
-    <row r="33" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D33" s="8" t="str">
         <f t="shared" si="2"/>
         <v>1E</v>
@@ -5082,7 +5710,7 @@
       <c r="BP33" s="56"/>
       <c r="BQ33" s="58"/>
     </row>
-    <row r="34" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D34" s="49" t="str">
         <f t="shared" si="2"/>
         <v>1F</v>
@@ -5156,7 +5784,7 @@
       <c r="BP34" s="29"/>
       <c r="BQ34" s="30"/>
     </row>
-    <row r="35" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D35" s="50" t="str">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -5230,7 +5858,7 @@
       <c r="BP35" s="32"/>
       <c r="BQ35" s="33"/>
     </row>
-    <row r="36" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D36" s="51" t="str">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -5304,7 +5932,7 @@
       <c r="BP36" s="35"/>
       <c r="BQ36" s="36"/>
     </row>
-    <row r="37" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D37" s="8" t="str">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -5378,7 +6006,7 @@
       <c r="BP37" s="56"/>
       <c r="BQ37" s="58"/>
     </row>
-    <row r="38" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D38" s="8" t="str">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -5452,7 +6080,7 @@
       <c r="BP38" s="56"/>
       <c r="BQ38" s="58"/>
     </row>
-    <row r="39" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D39" s="8" t="str">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -5526,7 +6154,7 @@
       <c r="BP39" s="56"/>
       <c r="BQ39" s="58"/>
     </row>
-    <row r="40" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D40" s="8" t="str">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -5600,7 +6228,7 @@
       <c r="BP40" s="56"/>
       <c r="BQ40" s="58"/>
     </row>
-    <row r="41" spans="4:69" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D41" s="8" t="str">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -5677,4 +6305,3132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9990A00-F3D8-4E56-9C95-A4A5E0390716}">
+  <dimension ref="A1:Q42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="4"/>
+    <col min="4" max="4" width="10.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="17" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K1" s="168" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="169" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="180" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="154" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="155" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="155" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="155" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="155" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="155" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="155" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="167" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="154" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="155" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="83" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="82">
+        <v>0</v>
+      </c>
+      <c r="D3" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="84" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="84">
+        <v>32</v>
+      </c>
+      <c r="G3" s="85">
+        <v>0</v>
+      </c>
+      <c r="H3" s="86">
+        <v>1</v>
+      </c>
+      <c r="I3" s="80">
+        <f>C3</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="80" t="str">
+        <f>DEC2HEX(IF(G3=0,H3*F3*16,0),4)</f>
+        <v>0200</v>
+      </c>
+      <c r="K3" s="93" t="str" cm="1">
+        <f t="array" aca="1" ref="K3" ca="1">IF(G3=0,DEC2HEX(HEX2DEC($A$3)),INDIRECT("K"&amp;(G3+3)))</f>
+        <v>2C00</v>
+      </c>
+      <c r="L3" s="156" t="str">
+        <f ca="1">DEC2HEX(HEX2DEC(K3)+HEX2DEC(J3)-1)</f>
+        <v>2DFF</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C4" s="157">
+        <f>C3+1</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="99" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="96" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="96">
+        <v>32</v>
+      </c>
+      <c r="G4" s="75">
+        <v>0</v>
+      </c>
+      <c r="H4" s="77">
+        <v>1</v>
+      </c>
+      <c r="I4" s="87">
+        <f>I3+HEX2DEC(J3)/512</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="87" t="str">
+        <f t="shared" ref="J4:J26" si="0">DEC2HEX(IF(G4=0,H4*F4*16,0),4)</f>
+        <v>0200</v>
+      </c>
+      <c r="K4" s="91" t="str" cm="1">
+        <f t="array" aca="1" ref="K4" ca="1">IF(G4=0,DEC2HEX(HEX2DEC($A$3)+I4*512,4),INDIRECT("K"&amp;(G4+3)))</f>
+        <v>2E00</v>
+      </c>
+      <c r="L4" s="158" t="str">
+        <f t="shared" ref="L4:L26" ca="1" si="1">DEC2HEX(HEX2DEC(K4)+HEX2DEC(J4)-1)</f>
+        <v>2FFF</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C5" s="159">
+        <f>C4+1</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="97" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="97">
+        <v>32</v>
+      </c>
+      <c r="G5" s="76">
+        <v>0</v>
+      </c>
+      <c r="H5" s="78">
+        <v>1</v>
+      </c>
+      <c r="I5" s="82">
+        <f t="shared" ref="I5:I26" si="2">I4+HEX2DEC(J4)/512</f>
+        <v>2</v>
+      </c>
+      <c r="J5" s="82" t="str">
+        <f t="shared" si="0"/>
+        <v>0200</v>
+      </c>
+      <c r="K5" s="94" t="str" cm="1">
+        <f t="array" aca="1" ref="K5" ca="1">IF(G5=0,DEC2HEX(HEX2DEC($A$3)+I5*512,4),INDIRECT("K"&amp;(G5+3)))</f>
+        <v>3000</v>
+      </c>
+      <c r="L5" s="160" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>31FF</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C6" s="161">
+        <f>C5+1</f>
+        <v>3</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="98">
+        <v>32</v>
+      </c>
+      <c r="G6" s="88">
+        <v>0</v>
+      </c>
+      <c r="H6" s="79">
+        <v>1</v>
+      </c>
+      <c r="I6" s="89">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J6" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v>0200</v>
+      </c>
+      <c r="K6" s="92" t="str" cm="1">
+        <f t="array" aca="1" ref="K6" ca="1">IF(G6=0,DEC2HEX(HEX2DEC($A$3)+I6*512,4),INDIRECT("K"&amp;(G6+3)))</f>
+        <v>3200</v>
+      </c>
+      <c r="L6" s="162" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>33FF</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C7" s="80">
+        <f>C6+1</f>
+        <v>4</v>
+      </c>
+      <c r="D7" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="84">
+        <v>32</v>
+      </c>
+      <c r="G7" s="85">
+        <v>0</v>
+      </c>
+      <c r="H7" s="86">
+        <v>4</v>
+      </c>
+      <c r="I7" s="80">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J7" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>0800</v>
+      </c>
+      <c r="K7" s="95" t="str" cm="1">
+        <f t="array" aca="1" ref="K7" ca="1">IF(G7=0,DEC2HEX(HEX2DEC($A$3)+I7*512,4),INDIRECT("K"&amp;(G7+3)))</f>
+        <v>3400</v>
+      </c>
+      <c r="L7" s="163" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>3BFF</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C8" s="89">
+        <f>C7+1</f>
+        <v>5</v>
+      </c>
+      <c r="D8" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="74">
+        <v>32</v>
+      </c>
+      <c r="G8" s="88">
+        <v>0</v>
+      </c>
+      <c r="H8" s="79">
+        <v>4</v>
+      </c>
+      <c r="I8" s="89">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J8" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v>0800</v>
+      </c>
+      <c r="K8" s="92" t="str" cm="1">
+        <f t="array" aca="1" ref="K8" ca="1">IF(G8=0,DEC2HEX(HEX2DEC($A$3)+I8*512,4),INDIRECT("K"&amp;(G8+3)))</f>
+        <v>3C00</v>
+      </c>
+      <c r="L8" s="164" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>43FF</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C9" s="80">
+        <f>C8+1</f>
+        <v>6</v>
+      </c>
+      <c r="D9" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="84">
+        <v>32</v>
+      </c>
+      <c r="G9" s="85">
+        <v>0</v>
+      </c>
+      <c r="H9" s="86">
+        <v>4</v>
+      </c>
+      <c r="I9" s="80">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="J9" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>0800</v>
+      </c>
+      <c r="K9" s="95" t="str" cm="1">
+        <f t="array" aca="1" ref="K9" ca="1">IF(G9=0,DEC2HEX(HEX2DEC($A$3)+I9*512,4),INDIRECT("K"&amp;(G9+3)))</f>
+        <v>4400</v>
+      </c>
+      <c r="L9" s="163" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>4BFF</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C10" s="89">
+        <f>C9+1</f>
+        <v>7</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="74">
+        <v>32</v>
+      </c>
+      <c r="G10" s="88">
+        <v>0</v>
+      </c>
+      <c r="H10" s="79">
+        <v>4</v>
+      </c>
+      <c r="I10" s="89">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="J10" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v>0800</v>
+      </c>
+      <c r="K10" s="92" t="str" cm="1">
+        <f t="array" aca="1" ref="K10" ca="1">IF(G10=0,DEC2HEX(HEX2DEC($A$3)+I10*512,4),INDIRECT("K"&amp;(G10+3)))</f>
+        <v>4C00</v>
+      </c>
+      <c r="L10" s="164" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>53FF</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C11" s="80">
+        <f>C10+1</f>
+        <v>8</v>
+      </c>
+      <c r="D11" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="84">
+        <v>32</v>
+      </c>
+      <c r="G11" s="85">
+        <v>4</v>
+      </c>
+      <c r="H11" s="86">
+        <v>4</v>
+      </c>
+      <c r="I11" s="80">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J11" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="K11" s="95" t="str" cm="1">
+        <f t="array" aca="1" ref="K11" ca="1">IF(G11=0,DEC2HEX(HEX2DEC($A$3)+I11*512,4),INDIRECT("K"&amp;(G11+3)))</f>
+        <v>3400</v>
+      </c>
+      <c r="L11" s="165" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>33FF</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C12" s="89">
+        <f>C11+1</f>
+        <v>9</v>
+      </c>
+      <c r="D12" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="74">
+        <v>32</v>
+      </c>
+      <c r="G12" s="88">
+        <v>5</v>
+      </c>
+      <c r="H12" s="79">
+        <v>4</v>
+      </c>
+      <c r="I12" s="89">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J12" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="K12" s="92" t="str" cm="1">
+        <f t="array" aca="1" ref="K12" ca="1">IF(G12=0,DEC2HEX(HEX2DEC($A$3)+I12*512,4),INDIRECT("K"&amp;(G12+3)))</f>
+        <v>3C00</v>
+      </c>
+      <c r="L12" s="166" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>3BFF</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C13" s="80">
+        <f>C12+1</f>
+        <v>10</v>
+      </c>
+      <c r="D13" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="84">
+        <v>32</v>
+      </c>
+      <c r="G13" s="85">
+        <v>6</v>
+      </c>
+      <c r="H13" s="86">
+        <v>4</v>
+      </c>
+      <c r="I13" s="80">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J13" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="K13" s="95" t="str" cm="1">
+        <f t="array" aca="1" ref="K13" ca="1">IF(G13=0,DEC2HEX(HEX2DEC($A$3)+I13*512,4),INDIRECT("K"&amp;(G13+3)))</f>
+        <v>4400</v>
+      </c>
+      <c r="L13" s="165" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>43FF</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C14" s="89">
+        <f>C13+1</f>
+        <v>11</v>
+      </c>
+      <c r="D14" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="74">
+        <v>32</v>
+      </c>
+      <c r="G14" s="88">
+        <v>7</v>
+      </c>
+      <c r="H14" s="79">
+        <v>4</v>
+      </c>
+      <c r="I14" s="89">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J14" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="K14" s="92" t="str" cm="1">
+        <f t="array" aca="1" ref="K14" ca="1">IF(G14=0,DEC2HEX(HEX2DEC($A$3)+I14*512,4),INDIRECT("K"&amp;(G14+3)))</f>
+        <v>4C00</v>
+      </c>
+      <c r="L14" s="166" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>4BFF</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C15" s="80">
+        <f>C14+1</f>
+        <v>12</v>
+      </c>
+      <c r="D15" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="84" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="84">
+        <v>32</v>
+      </c>
+      <c r="G15" s="85">
+        <v>0</v>
+      </c>
+      <c r="H15" s="86">
+        <v>1</v>
+      </c>
+      <c r="I15" s="80">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J15" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>0200</v>
+      </c>
+      <c r="K15" s="95" t="str" cm="1">
+        <f t="array" aca="1" ref="K15" ca="1">IF(G15=0,DEC2HEX(HEX2DEC($A$3)+I15*512,4),INDIRECT("K"&amp;(G15+3)))</f>
+        <v>5400</v>
+      </c>
+      <c r="L15" s="163" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>55FF</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C16" s="89">
+        <f>C15+1</f>
+        <v>13</v>
+      </c>
+      <c r="D16" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="74">
+        <v>32</v>
+      </c>
+      <c r="G16" s="88">
+        <v>0</v>
+      </c>
+      <c r="H16" s="79">
+        <v>1</v>
+      </c>
+      <c r="I16" s="89">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="J16" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v>0200</v>
+      </c>
+      <c r="K16" s="92" t="str" cm="1">
+        <f t="array" aca="1" ref="K16" ca="1">IF(G16=0,DEC2HEX(HEX2DEC($A$3)+I16*512,4),INDIRECT("K"&amp;(G16+3)))</f>
+        <v>5600</v>
+      </c>
+      <c r="L16" s="164" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>57FF</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="80">
+        <f>C16+1</f>
+        <v>14</v>
+      </c>
+      <c r="D17" s="71" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="84">
+        <v>32</v>
+      </c>
+      <c r="G17" s="85">
+        <v>0</v>
+      </c>
+      <c r="H17" s="86">
+        <v>4</v>
+      </c>
+      <c r="I17" s="80">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="J17" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>0800</v>
+      </c>
+      <c r="K17" s="95" t="str" cm="1">
+        <f t="array" aca="1" ref="K17" ca="1">IF(G17=0,DEC2HEX(HEX2DEC($A$3)+I17*512,4),INDIRECT("K"&amp;(G17+3)))</f>
+        <v>5800</v>
+      </c>
+      <c r="L17" s="156" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>5FFF</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="89">
+        <f>C17+1</f>
+        <v>15</v>
+      </c>
+      <c r="D18" s="73" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="74">
+        <v>32</v>
+      </c>
+      <c r="G18" s="88">
+        <v>0</v>
+      </c>
+      <c r="H18" s="79">
+        <v>4</v>
+      </c>
+      <c r="I18" s="89">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="J18" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v>0800</v>
+      </c>
+      <c r="K18" s="92" t="str" cm="1">
+        <f t="array" aca="1" ref="K18" ca="1">IF(G18=0,DEC2HEX(HEX2DEC($A$3)+I18*512,4),INDIRECT("K"&amp;(G18+3)))</f>
+        <v>6000</v>
+      </c>
+      <c r="L18" s="162" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>67FF</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="80">
+        <f>C18+1</f>
+        <v>16</v>
+      </c>
+      <c r="D19" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="84">
+        <v>32</v>
+      </c>
+      <c r="G19" s="85">
+        <v>0</v>
+      </c>
+      <c r="H19" s="86">
+        <v>2</v>
+      </c>
+      <c r="I19" s="80">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="J19" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>0400</v>
+      </c>
+      <c r="K19" s="95" t="str" cm="1">
+        <f t="array" aca="1" ref="K19" ca="1">IF(G19=0,DEC2HEX(HEX2DEC($A$3)+I19*512,4),INDIRECT("K"&amp;(G19+3)))</f>
+        <v>6800</v>
+      </c>
+      <c r="L19" s="156" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>6BFF</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" s="89">
+        <f>C19+1</f>
+        <v>17</v>
+      </c>
+      <c r="D20" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="74">
+        <v>32</v>
+      </c>
+      <c r="G20" s="88">
+        <v>0</v>
+      </c>
+      <c r="H20" s="79">
+        <v>2</v>
+      </c>
+      <c r="I20" s="89">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="J20" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v>0400</v>
+      </c>
+      <c r="K20" s="92" t="str" cm="1">
+        <f t="array" aca="1" ref="K20" ca="1">IF(G20=0,DEC2HEX(HEX2DEC($A$3)+I20*512,4),INDIRECT("K"&amp;(G20+3)))</f>
+        <v>6C00</v>
+      </c>
+      <c r="L20" s="166" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>6FFF</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="80">
+        <f>C20+1</f>
+        <v>18</v>
+      </c>
+      <c r="D21" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="84">
+        <v>32</v>
+      </c>
+      <c r="G21" s="85">
+        <v>16</v>
+      </c>
+      <c r="H21" s="86">
+        <v>2</v>
+      </c>
+      <c r="I21" s="80">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J21" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="K21" s="95" t="str" cm="1">
+        <f t="array" aca="1" ref="K21" ca="1">IF(G21=0,DEC2HEX(HEX2DEC($A$3)+I21*512,4),INDIRECT("K"&amp;(G21+3)))</f>
+        <v>6800</v>
+      </c>
+      <c r="L21" s="165" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>67FF</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" s="89">
+        <f>C21+1</f>
+        <v>19</v>
+      </c>
+      <c r="D22" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="74">
+        <v>32</v>
+      </c>
+      <c r="G22" s="88">
+        <v>17</v>
+      </c>
+      <c r="H22" s="79">
+        <v>2</v>
+      </c>
+      <c r="I22" s="89">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J22" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="K22" s="92" t="str" cm="1">
+        <f t="array" aca="1" ref="K22" ca="1">IF(G22=0,DEC2HEX(HEX2DEC($A$3)+I22*512,4),INDIRECT("K"&amp;(G22+3)))</f>
+        <v>6C00</v>
+      </c>
+      <c r="L22" s="166" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>6BFF</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" s="80">
+        <f>C22+1</f>
+        <v>20</v>
+      </c>
+      <c r="D23" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="84">
+        <v>32</v>
+      </c>
+      <c r="G23" s="85">
+        <v>0</v>
+      </c>
+      <c r="H23" s="86">
+        <v>4</v>
+      </c>
+      <c r="I23" s="80">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J23" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>0800</v>
+      </c>
+      <c r="K23" s="95" t="str" cm="1">
+        <f t="array" aca="1" ref="K23" ca="1">IF(G23=0,DEC2HEX(HEX2DEC($A$3)+I23*512,4),INDIRECT("K"&amp;(G23+3)))</f>
+        <v>7000</v>
+      </c>
+      <c r="L23" s="165" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>77FF</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C24" s="89">
+        <f>C23+1</f>
+        <v>21</v>
+      </c>
+      <c r="D24" s="73" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="74">
+        <v>32</v>
+      </c>
+      <c r="G24" s="88">
+        <v>0</v>
+      </c>
+      <c r="H24" s="79">
+        <v>4</v>
+      </c>
+      <c r="I24" s="89">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="J24" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v>0800</v>
+      </c>
+      <c r="K24" s="92" t="str" cm="1">
+        <f t="array" aca="1" ref="K24" ca="1">IF(G24=0,DEC2HEX(HEX2DEC($A$3)+I24*512,4),INDIRECT("K"&amp;(G24+3)))</f>
+        <v>7800</v>
+      </c>
+      <c r="L24" s="166" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>7FFF</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C25" s="80">
+        <f>C24+1</f>
+        <v>22</v>
+      </c>
+      <c r="D25" s="71" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="84" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="84">
+        <v>32</v>
+      </c>
+      <c r="G25" s="85">
+        <v>12</v>
+      </c>
+      <c r="H25" s="86">
+        <v>1</v>
+      </c>
+      <c r="I25" s="80">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="J25" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="K25" s="95" t="str" cm="1">
+        <f t="array" aca="1" ref="K25" ca="1">IF(G25=0,DEC2HEX(HEX2DEC($A$3)+I25*512,4),INDIRECT("K"&amp;(G25+3)))</f>
+        <v>5400</v>
+      </c>
+      <c r="L25" s="165" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>53FF</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C26" s="81">
+        <f>C25+1</f>
+        <v>23</v>
+      </c>
+      <c r="D26" s="73" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="74">
+        <v>32</v>
+      </c>
+      <c r="G26" s="88">
+        <v>13</v>
+      </c>
+      <c r="H26" s="79">
+        <v>1</v>
+      </c>
+      <c r="I26" s="89">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="J26" s="89" t="str">
+        <f t="shared" si="0"/>
+        <v>0000</v>
+      </c>
+      <c r="K26" s="92" t="str" cm="1">
+        <f t="array" aca="1" ref="K26" ca="1">IF(G26=0,DEC2HEX(HEX2DEC($A$3)+I26*512,4),INDIRECT("K"&amp;(G26+3)))</f>
+        <v>5600</v>
+      </c>
+      <c r="L26" s="166" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>55FF</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C27" s="80">
+        <f>C26+1</f>
+        <v>24</v>
+      </c>
+      <c r="D27" s="179" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="171"/>
+      <c r="F27" s="171"/>
+      <c r="G27" s="171"/>
+      <c r="H27" s="171"/>
+      <c r="I27" s="171"/>
+      <c r="J27" s="171"/>
+      <c r="K27" s="171"/>
+      <c r="L27" s="103"/>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C28" s="81">
+        <f>C27+1</f>
+        <v>25</v>
+      </c>
+      <c r="D28" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="104"/>
+      <c r="F28" s="104"/>
+      <c r="G28" s="104"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="104"/>
+      <c r="J28" s="172"/>
+      <c r="K28" s="104"/>
+      <c r="L28" s="68"/>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C29" s="82">
+        <f>C28+1</f>
+        <v>26</v>
+      </c>
+      <c r="D29" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="104"/>
+      <c r="F29" s="104"/>
+      <c r="G29" s="104"/>
+      <c r="H29" s="104"/>
+      <c r="I29" s="104"/>
+      <c r="J29" s="104"/>
+      <c r="K29" s="104"/>
+      <c r="L29" s="68"/>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C30" s="81">
+        <f>C29+1</f>
+        <v>27</v>
+      </c>
+      <c r="D30" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="104"/>
+      <c r="F30" s="104"/>
+      <c r="G30" s="104"/>
+      <c r="H30" s="104"/>
+      <c r="I30" s="104"/>
+      <c r="J30" s="104"/>
+      <c r="K30" s="104"/>
+      <c r="L30" s="68"/>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C31" s="82">
+        <f>C30+1</f>
+        <v>28</v>
+      </c>
+      <c r="D31" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="104"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="104"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="104"/>
+      <c r="K31" s="104"/>
+      <c r="L31" s="68"/>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C32" s="81">
+        <f>C31+1</f>
+        <v>29</v>
+      </c>
+      <c r="D32" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="104"/>
+      <c r="F32" s="104"/>
+      <c r="G32" s="104"/>
+      <c r="H32" s="104"/>
+      <c r="I32" s="104"/>
+      <c r="J32" s="104"/>
+      <c r="K32" s="104"/>
+      <c r="L32" s="68"/>
+    </row>
+    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C33" s="82">
+        <f>C32+1</f>
+        <v>30</v>
+      </c>
+      <c r="D33" s="106" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="105"/>
+      <c r="F33" s="105"/>
+      <c r="G33" s="105"/>
+      <c r="H33" s="105"/>
+      <c r="I33" s="105"/>
+      <c r="J33" s="105"/>
+      <c r="K33" s="105"/>
+      <c r="L33" s="106"/>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C34" s="87">
+        <f>C33+1</f>
+        <v>31</v>
+      </c>
+      <c r="D34" s="174" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="173"/>
+      <c r="F34" s="173"/>
+      <c r="G34" s="173"/>
+      <c r="H34" s="173"/>
+      <c r="I34" s="173"/>
+      <c r="J34" s="173"/>
+      <c r="K34" s="173"/>
+      <c r="L34" s="174"/>
+    </row>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C35" s="82">
+        <f>C34+1</f>
+        <v>32</v>
+      </c>
+      <c r="D35" s="176" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="175"/>
+      <c r="F35" s="175"/>
+      <c r="G35" s="175"/>
+      <c r="H35" s="175"/>
+      <c r="I35" s="175"/>
+      <c r="J35" s="175"/>
+      <c r="K35" s="175"/>
+      <c r="L35" s="176"/>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="89">
+        <f>C35+1</f>
+        <v>33</v>
+      </c>
+      <c r="D36" s="178" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" s="177"/>
+      <c r="F36" s="177"/>
+      <c r="G36" s="177"/>
+      <c r="H36" s="177"/>
+      <c r="I36" s="177"/>
+      <c r="J36" s="177"/>
+      <c r="K36" s="177"/>
+      <c r="L36" s="178"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="82">
+        <f>C36+1</f>
+        <v>34</v>
+      </c>
+      <c r="D37" s="103" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="102"/>
+      <c r="F37" s="102"/>
+      <c r="G37" s="102"/>
+      <c r="H37" s="102"/>
+      <c r="I37" s="102"/>
+      <c r="J37" s="102"/>
+      <c r="K37" s="102"/>
+      <c r="L37" s="103"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C38" s="81">
+        <f>C37+1</f>
+        <v>35</v>
+      </c>
+      <c r="D38" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="104"/>
+      <c r="F38" s="104"/>
+      <c r="G38" s="104"/>
+      <c r="H38" s="104"/>
+      <c r="I38" s="104"/>
+      <c r="J38" s="104"/>
+      <c r="K38" s="104"/>
+      <c r="L38" s="68"/>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C39" s="82">
+        <f>C38+1</f>
+        <v>36</v>
+      </c>
+      <c r="D39" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="104"/>
+      <c r="F39" s="104"/>
+      <c r="G39" s="104"/>
+      <c r="H39" s="104"/>
+      <c r="I39" s="104"/>
+      <c r="J39" s="104"/>
+      <c r="K39" s="104"/>
+      <c r="L39" s="68"/>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C40" s="81">
+        <f>C39+1</f>
+        <v>37</v>
+      </c>
+      <c r="D40" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="104"/>
+      <c r="F40" s="104"/>
+      <c r="G40" s="104"/>
+      <c r="H40" s="104"/>
+      <c r="I40" s="104"/>
+      <c r="J40" s="104"/>
+      <c r="K40" s="104"/>
+      <c r="L40" s="68"/>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C41" s="90">
+        <f>C40+1</f>
+        <v>38</v>
+      </c>
+      <c r="D41" s="106" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="105"/>
+      <c r="F41" s="105"/>
+      <c r="G41" s="105"/>
+      <c r="H41" s="105"/>
+      <c r="I41" s="105"/>
+      <c r="J41" s="105"/>
+      <c r="K41" s="105"/>
+      <c r="L41" s="106"/>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C42" s="170"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F481C70-9657-4394-93E6-4755D8687536}">
+  <dimension ref="B1:AT28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AV16" sqref="AV16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="10.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="35" width="3.77734375" customWidth="1"/>
+    <col min="36" max="39" width="8.88671875" style="4" customWidth="1"/>
+    <col min="41" max="41" width="8.88671875" style="9"/>
+    <col min="42" max="42" width="8.88671875" style="4"/>
+    <col min="44" max="45" width="8.88671875" style="9"/>
+    <col min="46" max="46" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="AO1" s="186" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP1" s="188" t="s">
+        <v>93</v>
+      </c>
+      <c r="AQ1" s="189"/>
+      <c r="AR1" s="183" t="s">
+        <v>94</v>
+      </c>
+      <c r="AS1" s="184"/>
+      <c r="AT1" s="193" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="2:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="100" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="101" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="204">
+        <v>0</v>
+      </c>
+      <c r="E2" s="204">
+        <f>D2+1</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="204">
+        <f t="shared" ref="F2:AI2" si="0">E2+1</f>
+        <v>2</v>
+      </c>
+      <c r="G2" s="204">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H2" s="204">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I2" s="204">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J2" s="204">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K2" s="204">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L2" s="204">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M2" s="204">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="N2" s="204">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="O2" s="204">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="P2" s="204">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Q2" s="204">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="R2" s="204">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="S2" s="204">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="T2" s="204">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="U2" s="204">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="V2" s="204">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="W2" s="204">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="X2" s="203">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="Y2" s="203">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="Z2" s="203">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="AA2" s="203">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="AB2" s="203">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="AC2" s="203">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AD2" s="203">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AE2" s="203">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AF2" s="204">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AG2" s="204">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AH2" s="204">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AI2" s="204">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AO2" s="185" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP2" s="194" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ2" s="194" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR2" s="187" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS2" s="185" t="s">
+        <v>96</v>
+      </c>
+      <c r="AT2" s="190" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="107">
+        <v>0</v>
+      </c>
+      <c r="C3" s="108" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="114" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="110" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="110" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="110"/>
+      <c r="J3" s="110" t="s">
+        <v>88</v>
+      </c>
+      <c r="K3" s="110" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="110" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" s="110" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="110" t="s">
+        <v>87</v>
+      </c>
+      <c r="O3" s="110" t="s">
+        <v>90</v>
+      </c>
+      <c r="P3" s="110">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="110">
+        <v>0</v>
+      </c>
+      <c r="R3" s="110">
+        <v>0</v>
+      </c>
+      <c r="S3" s="110">
+        <v>0</v>
+      </c>
+      <c r="T3" s="110">
+        <v>0</v>
+      </c>
+      <c r="U3" s="110">
+        <v>0</v>
+      </c>
+      <c r="V3" s="110"/>
+      <c r="W3" s="110"/>
+      <c r="X3" s="205"/>
+      <c r="Y3" s="206"/>
+      <c r="Z3" s="206"/>
+      <c r="AA3" s="206"/>
+      <c r="AB3" s="206"/>
+      <c r="AC3" s="206"/>
+      <c r="AD3" s="206"/>
+      <c r="AE3" s="207"/>
+      <c r="AF3" s="110" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG3" s="110" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH3" s="110" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI3" s="111" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ3" s="208">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="116" t="str">
+        <f>DEC2HEX(AJ3*2+44,2)</f>
+        <v>2C</v>
+      </c>
+      <c r="AP3" s="191">
+        <v>-1</v>
+      </c>
+      <c r="AQ3" s="192">
+        <v>-1</v>
+      </c>
+      <c r="AR3" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AS3" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AT3" s="109">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="112">
+        <f>B3+1</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="113" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="130"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="132"/>
+      <c r="H4" s="132"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="131"/>
+      <c r="L4" s="131"/>
+      <c r="M4" s="132"/>
+      <c r="N4" s="132"/>
+      <c r="O4" s="131"/>
+      <c r="P4" s="131"/>
+      <c r="Q4" s="131"/>
+      <c r="R4" s="131"/>
+      <c r="S4" s="132"/>
+      <c r="T4" s="132"/>
+      <c r="U4" s="131"/>
+      <c r="V4" s="131"/>
+      <c r="W4" s="131"/>
+      <c r="X4" s="131"/>
+      <c r="Y4" s="132"/>
+      <c r="Z4" s="132"/>
+      <c r="AA4" s="131"/>
+      <c r="AB4" s="131"/>
+      <c r="AC4" s="131"/>
+      <c r="AD4" s="131"/>
+      <c r="AE4" s="132"/>
+      <c r="AF4" s="132"/>
+      <c r="AG4" s="131"/>
+      <c r="AH4" s="131"/>
+      <c r="AI4" s="133"/>
+      <c r="AJ4" s="209">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="116" t="str">
+        <f t="shared" ref="AO4:AO26" si="1">DEC2HEX(AJ4*2+44,2)</f>
+        <v>2E</v>
+      </c>
+      <c r="AP4" s="191">
+        <v>-1</v>
+      </c>
+      <c r="AQ4" s="192">
+        <v>-1</v>
+      </c>
+      <c r="AR4" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AS4" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AT4" s="114">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="117">
+        <f>B4+1</f>
+        <v>2</v>
+      </c>
+      <c r="C5" s="108" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="123"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="137"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="124"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="134"/>
+      <c r="N5" s="137"/>
+      <c r="O5" s="124"/>
+      <c r="P5" s="124"/>
+      <c r="Q5" s="124"/>
+      <c r="R5" s="124"/>
+      <c r="S5" s="134"/>
+      <c r="T5" s="137"/>
+      <c r="U5" s="124"/>
+      <c r="V5" s="124"/>
+      <c r="W5" s="124"/>
+      <c r="X5" s="124"/>
+      <c r="Y5" s="134"/>
+      <c r="Z5" s="137"/>
+      <c r="AA5" s="124"/>
+      <c r="AB5" s="124"/>
+      <c r="AC5" s="124"/>
+      <c r="AD5" s="124"/>
+      <c r="AE5" s="134"/>
+      <c r="AF5" s="137"/>
+      <c r="AG5" s="124"/>
+      <c r="AH5" s="124"/>
+      <c r="AI5" s="125"/>
+      <c r="AJ5" s="210">
+        <v>2</v>
+      </c>
+      <c r="AO5" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="AP5" s="191">
+        <v>-1</v>
+      </c>
+      <c r="AQ5" s="192">
+        <v>-1</v>
+      </c>
+      <c r="AR5" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AS5" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AT5" s="114">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="118">
+        <f>B5+1</f>
+        <v>3</v>
+      </c>
+      <c r="C6" s="119" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="127"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="138"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="128"/>
+      <c r="K6" s="128"/>
+      <c r="L6" s="128"/>
+      <c r="M6" s="136"/>
+      <c r="N6" s="138"/>
+      <c r="O6" s="128"/>
+      <c r="P6" s="128"/>
+      <c r="Q6" s="128"/>
+      <c r="R6" s="128"/>
+      <c r="S6" s="136"/>
+      <c r="T6" s="138"/>
+      <c r="U6" s="128"/>
+      <c r="V6" s="128"/>
+      <c r="W6" s="128"/>
+      <c r="X6" s="128"/>
+      <c r="Y6" s="136"/>
+      <c r="Z6" s="138"/>
+      <c r="AA6" s="128"/>
+      <c r="AB6" s="128"/>
+      <c r="AC6" s="128"/>
+      <c r="AD6" s="128"/>
+      <c r="AE6" s="136"/>
+      <c r="AF6" s="138"/>
+      <c r="AG6" s="128"/>
+      <c r="AH6" s="128"/>
+      <c r="AI6" s="129"/>
+      <c r="AJ6" s="211">
+        <v>3</v>
+      </c>
+      <c r="AO6" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="AP6" s="191">
+        <v>-1</v>
+      </c>
+      <c r="AQ6" s="192">
+        <v>-1</v>
+      </c>
+      <c r="AR6" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AS6" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AT6" s="114">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="120">
+        <f>B6+1</f>
+        <v>4</v>
+      </c>
+      <c r="C7" s="121" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="136"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="126"/>
+      <c r="I7" s="126"/>
+      <c r="J7" s="126"/>
+      <c r="K7" s="126"/>
+      <c r="L7" s="126"/>
+      <c r="M7" s="126"/>
+      <c r="N7" s="126"/>
+      <c r="O7" s="126"/>
+      <c r="P7" s="126"/>
+      <c r="Q7" s="126"/>
+      <c r="R7" s="126"/>
+      <c r="S7" s="126"/>
+      <c r="T7" s="126"/>
+      <c r="U7" s="126"/>
+      <c r="V7" s="126"/>
+      <c r="W7" s="126"/>
+      <c r="X7" s="126"/>
+      <c r="Y7" s="126"/>
+      <c r="Z7" s="126"/>
+      <c r="AA7" s="126"/>
+      <c r="AB7" s="126"/>
+      <c r="AC7" s="126"/>
+      <c r="AD7" s="126"/>
+      <c r="AE7" s="126"/>
+      <c r="AF7" s="126"/>
+      <c r="AG7" s="126"/>
+      <c r="AH7" s="126"/>
+      <c r="AI7" s="126"/>
+      <c r="AJ7" s="134">
+        <v>4</v>
+      </c>
+      <c r="AK7" s="135">
+        <v>5</v>
+      </c>
+      <c r="AL7" s="135">
+        <v>6</v>
+      </c>
+      <c r="AM7" s="137">
+        <v>7</v>
+      </c>
+      <c r="AO7" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="AP7" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="116">
+        <v>3</v>
+      </c>
+      <c r="AR7" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT7" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="122">
+        <f>B7+1</f>
+        <v>5</v>
+      </c>
+      <c r="C8" s="119" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="136"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="126"/>
+      <c r="J8" s="126"/>
+      <c r="K8" s="126"/>
+      <c r="L8" s="126"/>
+      <c r="M8" s="126"/>
+      <c r="N8" s="126"/>
+      <c r="O8" s="126"/>
+      <c r="P8" s="126"/>
+      <c r="Q8" s="126"/>
+      <c r="R8" s="126"/>
+      <c r="S8" s="126"/>
+      <c r="T8" s="126"/>
+      <c r="U8" s="126"/>
+      <c r="V8" s="126"/>
+      <c r="W8" s="126"/>
+      <c r="X8" s="126"/>
+      <c r="Y8" s="126"/>
+      <c r="Z8" s="126"/>
+      <c r="AA8" s="126"/>
+      <c r="AB8" s="126"/>
+      <c r="AC8" s="126"/>
+      <c r="AD8" s="126"/>
+      <c r="AE8" s="126"/>
+      <c r="AF8" s="126"/>
+      <c r="AG8" s="126"/>
+      <c r="AH8" s="126"/>
+      <c r="AI8" s="126"/>
+      <c r="AJ8" s="151">
+        <v>8</v>
+      </c>
+      <c r="AK8" s="152">
+        <v>9</v>
+      </c>
+      <c r="AL8" s="152">
+        <v>10</v>
+      </c>
+      <c r="AM8" s="153">
+        <v>11</v>
+      </c>
+      <c r="AO8" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>3C</v>
+      </c>
+      <c r="AP8" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="116">
+        <v>3</v>
+      </c>
+      <c r="AR8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT8" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="120">
+        <f>B8+1</f>
+        <v>6</v>
+      </c>
+      <c r="C9" s="121" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="136"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="126"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="126"/>
+      <c r="J9" s="126"/>
+      <c r="K9" s="126"/>
+      <c r="L9" s="126"/>
+      <c r="M9" s="126"/>
+      <c r="N9" s="126"/>
+      <c r="O9" s="126"/>
+      <c r="P9" s="126"/>
+      <c r="Q9" s="126"/>
+      <c r="R9" s="126"/>
+      <c r="S9" s="126"/>
+      <c r="T9" s="126"/>
+      <c r="U9" s="126"/>
+      <c r="V9" s="126"/>
+      <c r="W9" s="126"/>
+      <c r="X9" s="126"/>
+      <c r="Y9" s="126"/>
+      <c r="Z9" s="126"/>
+      <c r="AA9" s="126"/>
+      <c r="AB9" s="126"/>
+      <c r="AC9" s="126"/>
+      <c r="AD9" s="126"/>
+      <c r="AE9" s="126"/>
+      <c r="AF9" s="126"/>
+      <c r="AG9" s="126"/>
+      <c r="AH9" s="126"/>
+      <c r="AI9" s="126"/>
+      <c r="AJ9" s="134">
+        <v>12</v>
+      </c>
+      <c r="AK9" s="135">
+        <v>13</v>
+      </c>
+      <c r="AL9" s="135">
+        <v>14</v>
+      </c>
+      <c r="AM9" s="137">
+        <v>15</v>
+      </c>
+      <c r="AO9" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="AP9" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="116">
+        <v>3</v>
+      </c>
+      <c r="AR9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT9" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="122">
+        <f>B9+1</f>
+        <v>7</v>
+      </c>
+      <c r="C10" s="119" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="136"/>
+      <c r="E10" s="126"/>
+      <c r="F10" s="126"/>
+      <c r="G10" s="126"/>
+      <c r="H10" s="126"/>
+      <c r="I10" s="126"/>
+      <c r="J10" s="126"/>
+      <c r="K10" s="126"/>
+      <c r="L10" s="126"/>
+      <c r="M10" s="126"/>
+      <c r="N10" s="126"/>
+      <c r="O10" s="126"/>
+      <c r="P10" s="126"/>
+      <c r="Q10" s="126"/>
+      <c r="R10" s="126"/>
+      <c r="S10" s="126"/>
+      <c r="T10" s="126"/>
+      <c r="U10" s="126"/>
+      <c r="V10" s="126"/>
+      <c r="W10" s="126"/>
+      <c r="X10" s="126"/>
+      <c r="Y10" s="126"/>
+      <c r="Z10" s="126"/>
+      <c r="AA10" s="126"/>
+      <c r="AB10" s="126"/>
+      <c r="AC10" s="126"/>
+      <c r="AD10" s="126"/>
+      <c r="AE10" s="126"/>
+      <c r="AF10" s="126"/>
+      <c r="AG10" s="126"/>
+      <c r="AH10" s="126"/>
+      <c r="AI10" s="126"/>
+      <c r="AJ10" s="151">
+        <v>16</v>
+      </c>
+      <c r="AK10" s="152">
+        <v>17</v>
+      </c>
+      <c r="AL10" s="152">
+        <v>18</v>
+      </c>
+      <c r="AM10" s="153">
+        <v>19</v>
+      </c>
+      <c r="AO10" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>4C</v>
+      </c>
+      <c r="AP10" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="116">
+        <v>3</v>
+      </c>
+      <c r="AR10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT10" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="120">
+        <f>B10+1</f>
+        <v>8</v>
+      </c>
+      <c r="C11" s="121" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="136"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="126"/>
+      <c r="H11" s="126"/>
+      <c r="I11" s="126"/>
+      <c r="J11" s="126"/>
+      <c r="K11" s="126"/>
+      <c r="L11" s="126"/>
+      <c r="M11" s="126"/>
+      <c r="N11" s="126"/>
+      <c r="O11" s="126"/>
+      <c r="P11" s="126"/>
+      <c r="Q11" s="126"/>
+      <c r="R11" s="126"/>
+      <c r="S11" s="126"/>
+      <c r="T11" s="126"/>
+      <c r="U11" s="126"/>
+      <c r="V11" s="126"/>
+      <c r="W11" s="126"/>
+      <c r="X11" s="126"/>
+      <c r="Y11" s="126"/>
+      <c r="Z11" s="126"/>
+      <c r="AA11" s="126"/>
+      <c r="AB11" s="126"/>
+      <c r="AC11" s="126"/>
+      <c r="AD11" s="126"/>
+      <c r="AE11" s="126"/>
+      <c r="AF11" s="126"/>
+      <c r="AG11" s="126"/>
+      <c r="AH11" s="126"/>
+      <c r="AI11" s="126"/>
+      <c r="AJ11" s="134">
+        <v>4</v>
+      </c>
+      <c r="AK11" s="135">
+        <v>5</v>
+      </c>
+      <c r="AL11" s="135">
+        <v>6</v>
+      </c>
+      <c r="AM11" s="137">
+        <v>7</v>
+      </c>
+      <c r="AO11" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="AP11" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="116">
+        <v>3</v>
+      </c>
+      <c r="AR11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT11" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="122">
+        <f>B11+1</f>
+        <v>9</v>
+      </c>
+      <c r="C12" s="119" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="136"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="126"/>
+      <c r="H12" s="126"/>
+      <c r="I12" s="126"/>
+      <c r="J12" s="126"/>
+      <c r="K12" s="126"/>
+      <c r="L12" s="126"/>
+      <c r="M12" s="126"/>
+      <c r="N12" s="126"/>
+      <c r="O12" s="126"/>
+      <c r="P12" s="126"/>
+      <c r="Q12" s="126"/>
+      <c r="R12" s="126"/>
+      <c r="S12" s="126"/>
+      <c r="T12" s="126"/>
+      <c r="U12" s="126"/>
+      <c r="V12" s="126"/>
+      <c r="W12" s="126"/>
+      <c r="X12" s="126"/>
+      <c r="Y12" s="126"/>
+      <c r="Z12" s="126"/>
+      <c r="AA12" s="126"/>
+      <c r="AB12" s="126"/>
+      <c r="AC12" s="126"/>
+      <c r="AD12" s="126"/>
+      <c r="AE12" s="126"/>
+      <c r="AF12" s="126"/>
+      <c r="AG12" s="126"/>
+      <c r="AH12" s="126"/>
+      <c r="AI12" s="126"/>
+      <c r="AJ12" s="151">
+        <v>8</v>
+      </c>
+      <c r="AK12" s="152">
+        <v>9</v>
+      </c>
+      <c r="AL12" s="152">
+        <v>10</v>
+      </c>
+      <c r="AM12" s="153">
+        <v>11</v>
+      </c>
+      <c r="AO12" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>3C</v>
+      </c>
+      <c r="AP12" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="116">
+        <v>3</v>
+      </c>
+      <c r="AR12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS12" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT12" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="120">
+        <f>B12+1</f>
+        <v>10</v>
+      </c>
+      <c r="C13" s="121" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="136"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
+      <c r="G13" s="126"/>
+      <c r="H13" s="126"/>
+      <c r="I13" s="126"/>
+      <c r="J13" s="126"/>
+      <c r="K13" s="126"/>
+      <c r="L13" s="126"/>
+      <c r="M13" s="126"/>
+      <c r="N13" s="126"/>
+      <c r="O13" s="126"/>
+      <c r="P13" s="126"/>
+      <c r="Q13" s="126"/>
+      <c r="R13" s="126"/>
+      <c r="S13" s="126"/>
+      <c r="T13" s="126"/>
+      <c r="U13" s="126"/>
+      <c r="V13" s="126"/>
+      <c r="W13" s="126"/>
+      <c r="X13" s="126"/>
+      <c r="Y13" s="126"/>
+      <c r="Z13" s="126"/>
+      <c r="AA13" s="126"/>
+      <c r="AB13" s="126"/>
+      <c r="AC13" s="126"/>
+      <c r="AD13" s="126"/>
+      <c r="AE13" s="126"/>
+      <c r="AF13" s="126"/>
+      <c r="AG13" s="126"/>
+      <c r="AH13" s="126"/>
+      <c r="AI13" s="126"/>
+      <c r="AJ13" s="136">
+        <v>12</v>
+      </c>
+      <c r="AK13" s="126">
+        <v>13</v>
+      </c>
+      <c r="AL13" s="126">
+        <v>14</v>
+      </c>
+      <c r="AM13" s="138">
+        <v>15</v>
+      </c>
+      <c r="AO13" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="AP13" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="116">
+        <v>3</v>
+      </c>
+      <c r="AR13" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT13" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="122">
+        <f>B13+1</f>
+        <v>11</v>
+      </c>
+      <c r="C14" s="119" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="136"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
+      <c r="H14" s="126"/>
+      <c r="I14" s="126"/>
+      <c r="J14" s="126"/>
+      <c r="K14" s="126"/>
+      <c r="L14" s="126"/>
+      <c r="M14" s="126"/>
+      <c r="N14" s="126"/>
+      <c r="O14" s="126"/>
+      <c r="P14" s="126"/>
+      <c r="Q14" s="126"/>
+      <c r="R14" s="126"/>
+      <c r="S14" s="126"/>
+      <c r="T14" s="126"/>
+      <c r="U14" s="126"/>
+      <c r="V14" s="126"/>
+      <c r="W14" s="126"/>
+      <c r="X14" s="126"/>
+      <c r="Y14" s="126"/>
+      <c r="Z14" s="126"/>
+      <c r="AA14" s="126"/>
+      <c r="AB14" s="126"/>
+      <c r="AC14" s="126"/>
+      <c r="AD14" s="126"/>
+      <c r="AE14" s="126"/>
+      <c r="AF14" s="126"/>
+      <c r="AG14" s="126"/>
+      <c r="AH14" s="126"/>
+      <c r="AI14" s="126"/>
+      <c r="AJ14" s="151">
+        <v>16</v>
+      </c>
+      <c r="AK14" s="152">
+        <v>17</v>
+      </c>
+      <c r="AL14" s="152">
+        <v>18</v>
+      </c>
+      <c r="AM14" s="153">
+        <v>19</v>
+      </c>
+      <c r="AO14" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>4C</v>
+      </c>
+      <c r="AP14" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="116">
+        <v>3</v>
+      </c>
+      <c r="AR14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT14" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="120">
+        <f>B14+1</f>
+        <v>12</v>
+      </c>
+      <c r="C15" s="121" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="148"/>
+      <c r="E15" s="149"/>
+      <c r="F15" s="149"/>
+      <c r="G15" s="149"/>
+      <c r="H15" s="149"/>
+      <c r="I15" s="149"/>
+      <c r="J15" s="149"/>
+      <c r="K15" s="149"/>
+      <c r="L15" s="149"/>
+      <c r="M15" s="149"/>
+      <c r="N15" s="149"/>
+      <c r="O15" s="149"/>
+      <c r="P15" s="149"/>
+      <c r="Q15" s="149"/>
+      <c r="R15" s="149"/>
+      <c r="S15" s="149"/>
+      <c r="T15" s="149"/>
+      <c r="U15" s="149"/>
+      <c r="V15" s="149"/>
+      <c r="W15" s="149"/>
+      <c r="X15" s="149"/>
+      <c r="Y15" s="149"/>
+      <c r="Z15" s="149"/>
+      <c r="AA15" s="149"/>
+      <c r="AB15" s="149"/>
+      <c r="AC15" s="149"/>
+      <c r="AD15" s="149"/>
+      <c r="AE15" s="149"/>
+      <c r="AF15" s="149"/>
+      <c r="AG15" s="149"/>
+      <c r="AH15" s="149"/>
+      <c r="AI15" s="150"/>
+      <c r="AJ15" s="208">
+        <v>20</v>
+      </c>
+      <c r="AO15" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="AP15" s="191">
+        <v>-1</v>
+      </c>
+      <c r="AQ15" s="192">
+        <v>-1</v>
+      </c>
+      <c r="AR15" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AS15" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AT15" s="114">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="122">
+        <f>B15+1</f>
+        <v>13</v>
+      </c>
+      <c r="C16" s="119" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="139"/>
+      <c r="E16" s="140"/>
+      <c r="F16" s="140"/>
+      <c r="G16" s="140"/>
+      <c r="H16" s="140"/>
+      <c r="I16" s="140"/>
+      <c r="J16" s="140"/>
+      <c r="K16" s="140"/>
+      <c r="L16" s="140"/>
+      <c r="M16" s="140"/>
+      <c r="N16" s="140"/>
+      <c r="O16" s="140"/>
+      <c r="P16" s="140"/>
+      <c r="Q16" s="140"/>
+      <c r="R16" s="140"/>
+      <c r="S16" s="140"/>
+      <c r="T16" s="140"/>
+      <c r="U16" s="140"/>
+      <c r="V16" s="140"/>
+      <c r="W16" s="140"/>
+      <c r="X16" s="140"/>
+      <c r="Y16" s="140"/>
+      <c r="Z16" s="140"/>
+      <c r="AA16" s="140"/>
+      <c r="AB16" s="140"/>
+      <c r="AC16" s="140"/>
+      <c r="AD16" s="140"/>
+      <c r="AE16" s="140"/>
+      <c r="AF16" s="140"/>
+      <c r="AG16" s="140"/>
+      <c r="AH16" s="140"/>
+      <c r="AI16" s="141"/>
+      <c r="AJ16" s="211">
+        <v>21</v>
+      </c>
+      <c r="AO16" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="AP16" s="191">
+        <v>-1</v>
+      </c>
+      <c r="AQ16" s="192">
+        <v>-1</v>
+      </c>
+      <c r="AR16" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AS16" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AT16" s="114">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="120">
+        <f>B16+1</f>
+        <v>14</v>
+      </c>
+      <c r="C17" s="121" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="144"/>
+      <c r="E17" s="145"/>
+      <c r="F17" s="145"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="145"/>
+      <c r="I17" s="145"/>
+      <c r="J17" s="145"/>
+      <c r="K17" s="145"/>
+      <c r="L17" s="145"/>
+      <c r="M17" s="145"/>
+      <c r="N17" s="145"/>
+      <c r="O17" s="145"/>
+      <c r="P17" s="145"/>
+      <c r="Q17" s="145"/>
+      <c r="R17" s="145"/>
+      <c r="S17" s="145"/>
+      <c r="T17" s="145"/>
+      <c r="U17" s="145"/>
+      <c r="V17" s="145"/>
+      <c r="W17" s="145"/>
+      <c r="X17" s="145"/>
+      <c r="Y17" s="145"/>
+      <c r="Z17" s="145"/>
+      <c r="AA17" s="145"/>
+      <c r="AB17" s="145"/>
+      <c r="AC17" s="145"/>
+      <c r="AD17" s="145"/>
+      <c r="AE17" s="145"/>
+      <c r="AF17" s="145"/>
+      <c r="AG17" s="145"/>
+      <c r="AH17" s="145"/>
+      <c r="AI17" s="145"/>
+      <c r="AJ17" s="195">
+        <v>22</v>
+      </c>
+      <c r="AK17" s="196">
+        <v>23</v>
+      </c>
+      <c r="AL17" s="196">
+        <v>24</v>
+      </c>
+      <c r="AM17" s="197">
+        <v>25</v>
+      </c>
+      <c r="AO17" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="AP17" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="116">
+        <v>3</v>
+      </c>
+      <c r="AR17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT17" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="122">
+        <f>B17+1</f>
+        <v>15</v>
+      </c>
+      <c r="C18" s="119" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="142"/>
+      <c r="E18" s="143"/>
+      <c r="F18" s="143"/>
+      <c r="G18" s="143"/>
+      <c r="H18" s="143"/>
+      <c r="I18" s="143"/>
+      <c r="J18" s="143"/>
+      <c r="K18" s="143"/>
+      <c r="L18" s="143"/>
+      <c r="M18" s="143"/>
+      <c r="N18" s="143"/>
+      <c r="O18" s="143"/>
+      <c r="P18" s="143"/>
+      <c r="Q18" s="143"/>
+      <c r="R18" s="143"/>
+      <c r="S18" s="143"/>
+      <c r="T18" s="143"/>
+      <c r="U18" s="143"/>
+      <c r="V18" s="143"/>
+      <c r="W18" s="143"/>
+      <c r="X18" s="143"/>
+      <c r="Y18" s="143"/>
+      <c r="Z18" s="143"/>
+      <c r="AA18" s="143"/>
+      <c r="AB18" s="143"/>
+      <c r="AC18" s="143"/>
+      <c r="AD18" s="143"/>
+      <c r="AE18" s="143"/>
+      <c r="AF18" s="143"/>
+      <c r="AG18" s="143"/>
+      <c r="AH18" s="143"/>
+      <c r="AI18" s="143"/>
+      <c r="AJ18" s="200">
+        <f>AJ17+4</f>
+        <v>26</v>
+      </c>
+      <c r="AK18" s="201">
+        <f>AK17+4</f>
+        <v>27</v>
+      </c>
+      <c r="AL18" s="201">
+        <f>AL17+4</f>
+        <v>28</v>
+      </c>
+      <c r="AM18" s="199">
+        <f>AM17+4</f>
+        <v>29</v>
+      </c>
+      <c r="AO18" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="AP18" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="116">
+        <v>3</v>
+      </c>
+      <c r="AR18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT18" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="120">
+        <f>B18+1</f>
+        <v>16</v>
+      </c>
+      <c r="C19" s="121" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="142"/>
+      <c r="E19" s="143"/>
+      <c r="F19" s="143"/>
+      <c r="G19" s="143"/>
+      <c r="H19" s="143"/>
+      <c r="I19" s="143"/>
+      <c r="J19" s="143"/>
+      <c r="K19" s="143"/>
+      <c r="L19" s="143"/>
+      <c r="M19" s="143"/>
+      <c r="N19" s="143"/>
+      <c r="O19" s="143"/>
+      <c r="P19" s="143"/>
+      <c r="Q19" s="143"/>
+      <c r="R19" s="143"/>
+      <c r="S19" s="143"/>
+      <c r="T19" s="143"/>
+      <c r="U19" s="143"/>
+      <c r="V19" s="143"/>
+      <c r="W19" s="143"/>
+      <c r="X19" s="143"/>
+      <c r="Y19" s="143"/>
+      <c r="Z19" s="143"/>
+      <c r="AA19" s="143"/>
+      <c r="AB19" s="143"/>
+      <c r="AC19" s="143"/>
+      <c r="AD19" s="143"/>
+      <c r="AE19" s="143"/>
+      <c r="AF19" s="143"/>
+      <c r="AG19" s="143"/>
+      <c r="AH19" s="143"/>
+      <c r="AI19" s="143"/>
+      <c r="AJ19" s="195">
+        <f>AJ18+4</f>
+        <v>30</v>
+      </c>
+      <c r="AK19" s="197">
+        <f>AK18+4</f>
+        <v>31</v>
+      </c>
+      <c r="AL19" s="212"/>
+      <c r="AM19" s="214"/>
+      <c r="AN19" s="115"/>
+      <c r="AO19" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="AP19" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="116">
+        <v>1</v>
+      </c>
+      <c r="AR19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT19" s="114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="122">
+        <f>B19+1</f>
+        <v>17</v>
+      </c>
+      <c r="C20" s="119" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="142"/>
+      <c r="E20" s="143"/>
+      <c r="F20" s="143"/>
+      <c r="G20" s="143"/>
+      <c r="H20" s="143"/>
+      <c r="I20" s="143"/>
+      <c r="J20" s="143"/>
+      <c r="K20" s="143"/>
+      <c r="L20" s="143"/>
+      <c r="M20" s="143"/>
+      <c r="N20" s="143"/>
+      <c r="O20" s="143"/>
+      <c r="P20" s="143"/>
+      <c r="Q20" s="143"/>
+      <c r="R20" s="143"/>
+      <c r="S20" s="143"/>
+      <c r="T20" s="143"/>
+      <c r="U20" s="143"/>
+      <c r="V20" s="143"/>
+      <c r="W20" s="143"/>
+      <c r="X20" s="143"/>
+      <c r="Y20" s="143"/>
+      <c r="Z20" s="143"/>
+      <c r="AA20" s="143"/>
+      <c r="AB20" s="143"/>
+      <c r="AC20" s="143"/>
+      <c r="AD20" s="143"/>
+      <c r="AE20" s="143"/>
+      <c r="AF20" s="143"/>
+      <c r="AG20" s="143"/>
+      <c r="AH20" s="143"/>
+      <c r="AI20" s="143"/>
+      <c r="AJ20" s="200">
+        <f>AJ19+2</f>
+        <v>32</v>
+      </c>
+      <c r="AK20" s="202">
+        <f>AK19+2</f>
+        <v>33</v>
+      </c>
+      <c r="AL20" s="212"/>
+      <c r="AM20" s="212"/>
+      <c r="AN20" s="115"/>
+      <c r="AO20" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>6C</v>
+      </c>
+      <c r="AP20" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="116">
+        <v>1</v>
+      </c>
+      <c r="AR20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT20" s="114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="120">
+        <f>B20+1</f>
+        <v>18</v>
+      </c>
+      <c r="C21" s="121" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="142"/>
+      <c r="E21" s="143"/>
+      <c r="F21" s="143"/>
+      <c r="G21" s="143"/>
+      <c r="H21" s="143"/>
+      <c r="I21" s="143"/>
+      <c r="J21" s="143"/>
+      <c r="K21" s="143"/>
+      <c r="L21" s="143"/>
+      <c r="M21" s="143"/>
+      <c r="N21" s="143"/>
+      <c r="O21" s="143"/>
+      <c r="P21" s="143"/>
+      <c r="Q21" s="143"/>
+      <c r="R21" s="143"/>
+      <c r="S21" s="143"/>
+      <c r="T21" s="143"/>
+      <c r="U21" s="143"/>
+      <c r="V21" s="143"/>
+      <c r="W21" s="143"/>
+      <c r="X21" s="143"/>
+      <c r="Y21" s="143"/>
+      <c r="Z21" s="143"/>
+      <c r="AA21" s="143"/>
+      <c r="AB21" s="143"/>
+      <c r="AC21" s="143"/>
+      <c r="AD21" s="143"/>
+      <c r="AE21" s="143"/>
+      <c r="AF21" s="143"/>
+      <c r="AG21" s="143"/>
+      <c r="AH21" s="143"/>
+      <c r="AI21" s="143"/>
+      <c r="AJ21" s="195">
+        <f>AJ20+2</f>
+        <v>34</v>
+      </c>
+      <c r="AK21" s="197">
+        <f>AK20+2</f>
+        <v>35</v>
+      </c>
+      <c r="AL21" s="212"/>
+      <c r="AM21" s="212"/>
+      <c r="AN21" s="115"/>
+      <c r="AO21" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="AP21" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="116">
+        <v>1</v>
+      </c>
+      <c r="AR21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT21" s="114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="122">
+        <f>B21+1</f>
+        <v>19</v>
+      </c>
+      <c r="C22" s="119" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="142"/>
+      <c r="E22" s="143"/>
+      <c r="F22" s="143"/>
+      <c r="G22" s="143"/>
+      <c r="H22" s="143"/>
+      <c r="I22" s="143"/>
+      <c r="J22" s="143"/>
+      <c r="K22" s="143"/>
+      <c r="L22" s="143"/>
+      <c r="M22" s="143"/>
+      <c r="N22" s="143"/>
+      <c r="O22" s="143"/>
+      <c r="P22" s="143"/>
+      <c r="Q22" s="143"/>
+      <c r="R22" s="143"/>
+      <c r="S22" s="143"/>
+      <c r="T22" s="143"/>
+      <c r="U22" s="143"/>
+      <c r="V22" s="143"/>
+      <c r="W22" s="143"/>
+      <c r="X22" s="143"/>
+      <c r="Y22" s="143"/>
+      <c r="Z22" s="143"/>
+      <c r="AA22" s="143"/>
+      <c r="AB22" s="143"/>
+      <c r="AC22" s="143"/>
+      <c r="AD22" s="143"/>
+      <c r="AE22" s="143"/>
+      <c r="AF22" s="143"/>
+      <c r="AG22" s="143"/>
+      <c r="AH22" s="143"/>
+      <c r="AI22" s="143"/>
+      <c r="AJ22" s="198">
+        <f>AJ21+2</f>
+        <v>36</v>
+      </c>
+      <c r="AK22" s="199">
+        <f>AK21+2</f>
+        <v>37</v>
+      </c>
+      <c r="AL22" s="212"/>
+      <c r="AM22" s="213"/>
+      <c r="AN22" s="115"/>
+      <c r="AO22" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="AP22" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ22" s="116">
+        <v>1</v>
+      </c>
+      <c r="AR22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS22" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT22" s="114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="120">
+        <f>B22+1</f>
+        <v>20</v>
+      </c>
+      <c r="C23" s="121" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="142"/>
+      <c r="E23" s="143"/>
+      <c r="F23" s="143"/>
+      <c r="G23" s="143"/>
+      <c r="H23" s="143"/>
+      <c r="I23" s="143"/>
+      <c r="J23" s="143"/>
+      <c r="K23" s="143"/>
+      <c r="L23" s="143"/>
+      <c r="M23" s="143"/>
+      <c r="N23" s="143"/>
+      <c r="O23" s="143"/>
+      <c r="P23" s="143"/>
+      <c r="Q23" s="143"/>
+      <c r="R23" s="143"/>
+      <c r="S23" s="143"/>
+      <c r="T23" s="143"/>
+      <c r="U23" s="143"/>
+      <c r="V23" s="143"/>
+      <c r="W23" s="143"/>
+      <c r="X23" s="143"/>
+      <c r="Y23" s="143"/>
+      <c r="Z23" s="143"/>
+      <c r="AA23" s="143"/>
+      <c r="AB23" s="143"/>
+      <c r="AC23" s="143"/>
+      <c r="AD23" s="143"/>
+      <c r="AE23" s="143"/>
+      <c r="AF23" s="143"/>
+      <c r="AG23" s="143"/>
+      <c r="AH23" s="143"/>
+      <c r="AI23" s="143"/>
+      <c r="AJ23" s="195">
+        <f>AJ22+2</f>
+        <v>38</v>
+      </c>
+      <c r="AK23" s="196">
+        <f>AJ23+1</f>
+        <v>39</v>
+      </c>
+      <c r="AL23" s="196">
+        <f>AK23+1</f>
+        <v>40</v>
+      </c>
+      <c r="AM23" s="199">
+        <f>AL23+1</f>
+        <v>41</v>
+      </c>
+      <c r="AO23" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="AP23" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ23" s="116">
+        <v>3</v>
+      </c>
+      <c r="AR23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS23" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT23" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="122">
+        <f>B23+1</f>
+        <v>21</v>
+      </c>
+      <c r="C24" s="119" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="146"/>
+      <c r="E24" s="147"/>
+      <c r="F24" s="147"/>
+      <c r="G24" s="147"/>
+      <c r="H24" s="147"/>
+      <c r="I24" s="147"/>
+      <c r="J24" s="147"/>
+      <c r="K24" s="147"/>
+      <c r="L24" s="147"/>
+      <c r="M24" s="147"/>
+      <c r="N24" s="147"/>
+      <c r="O24" s="147"/>
+      <c r="P24" s="147"/>
+      <c r="Q24" s="147"/>
+      <c r="R24" s="147"/>
+      <c r="S24" s="147"/>
+      <c r="T24" s="147"/>
+      <c r="U24" s="147"/>
+      <c r="V24" s="147"/>
+      <c r="W24" s="147"/>
+      <c r="X24" s="147"/>
+      <c r="Y24" s="147"/>
+      <c r="Z24" s="147"/>
+      <c r="AA24" s="147"/>
+      <c r="AB24" s="147"/>
+      <c r="AC24" s="147"/>
+      <c r="AD24" s="147"/>
+      <c r="AE24" s="147"/>
+      <c r="AF24" s="147"/>
+      <c r="AG24" s="147"/>
+      <c r="AH24" s="147"/>
+      <c r="AI24" s="147"/>
+      <c r="AJ24" s="200">
+        <f>AJ23+4</f>
+        <v>42</v>
+      </c>
+      <c r="AK24" s="201">
+        <f>AK23+4</f>
+        <v>43</v>
+      </c>
+      <c r="AL24" s="201">
+        <f>AL23+4</f>
+        <v>44</v>
+      </c>
+      <c r="AM24" s="202">
+        <f>AM23+4</f>
+        <v>45</v>
+      </c>
+      <c r="AO24" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="AP24" s="114">
+        <v>0</v>
+      </c>
+      <c r="AQ24" s="116">
+        <v>3</v>
+      </c>
+      <c r="AR24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS24" s="9">
+        <v>64</v>
+      </c>
+      <c r="AT24" s="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="120">
+        <f>B24+1</f>
+        <v>22</v>
+      </c>
+      <c r="C25" s="121" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="148"/>
+      <c r="E25" s="149"/>
+      <c r="F25" s="149"/>
+      <c r="G25" s="149"/>
+      <c r="H25" s="149"/>
+      <c r="I25" s="149"/>
+      <c r="J25" s="149"/>
+      <c r="K25" s="149"/>
+      <c r="L25" s="149"/>
+      <c r="M25" s="149"/>
+      <c r="N25" s="149"/>
+      <c r="O25" s="149"/>
+      <c r="P25" s="149"/>
+      <c r="Q25" s="149"/>
+      <c r="R25" s="149"/>
+      <c r="S25" s="149"/>
+      <c r="T25" s="149"/>
+      <c r="U25" s="149"/>
+      <c r="V25" s="149"/>
+      <c r="W25" s="149"/>
+      <c r="X25" s="149"/>
+      <c r="Y25" s="149"/>
+      <c r="Z25" s="149"/>
+      <c r="AA25" s="149"/>
+      <c r="AB25" s="149"/>
+      <c r="AC25" s="149"/>
+      <c r="AD25" s="149"/>
+      <c r="AE25" s="149"/>
+      <c r="AF25" s="149"/>
+      <c r="AG25" s="149"/>
+      <c r="AH25" s="149"/>
+      <c r="AI25" s="150"/>
+      <c r="AJ25" s="208">
+        <v>20</v>
+      </c>
+      <c r="AO25" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="AP25" s="191">
+        <v>-1</v>
+      </c>
+      <c r="AQ25" s="192">
+        <v>-1</v>
+      </c>
+      <c r="AR25" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AS25" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AT25" s="114">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="122">
+        <f>B25+1</f>
+        <v>23</v>
+      </c>
+      <c r="C26" s="119" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="139"/>
+      <c r="E26" s="140"/>
+      <c r="F26" s="140"/>
+      <c r="G26" s="140"/>
+      <c r="H26" s="140"/>
+      <c r="I26" s="140"/>
+      <c r="J26" s="140"/>
+      <c r="K26" s="140"/>
+      <c r="L26" s="140"/>
+      <c r="M26" s="140"/>
+      <c r="N26" s="140"/>
+      <c r="O26" s="140"/>
+      <c r="P26" s="140"/>
+      <c r="Q26" s="140"/>
+      <c r="R26" s="140"/>
+      <c r="S26" s="140"/>
+      <c r="T26" s="140"/>
+      <c r="U26" s="140"/>
+      <c r="V26" s="140"/>
+      <c r="W26" s="140"/>
+      <c r="X26" s="140"/>
+      <c r="Y26" s="140"/>
+      <c r="Z26" s="140"/>
+      <c r="AA26" s="140"/>
+      <c r="AB26" s="140"/>
+      <c r="AC26" s="140"/>
+      <c r="AD26" s="140"/>
+      <c r="AE26" s="140"/>
+      <c r="AF26" s="140"/>
+      <c r="AG26" s="140"/>
+      <c r="AH26" s="140"/>
+      <c r="AI26" s="141"/>
+      <c r="AJ26" s="211">
+        <v>21</v>
+      </c>
+      <c r="AO26" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="AP26" s="191">
+        <v>-1</v>
+      </c>
+      <c r="AQ26" s="192">
+        <v>-1</v>
+      </c>
+      <c r="AR26" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AS26" s="182">
+        <v>-1</v>
+      </c>
+      <c r="AT26" s="114">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="B27" s="69"/>
+      <c r="C27" s="70" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="2:46" x14ac:dyDescent="0.3">
+      <c r="AI28" s="181" t="str">
+        <f>DEC2HEX(MAX(AJ3:AM27)*512,4)</f>
+        <v>5A00</v>
+      </c>
+      <c r="AJ28" s="181"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="AI28:AJ28"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AP1:AQ1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update 6845 CRTC timing spreadsheet to reflect recent timing adjustments
</commit_message>
<xml_diff>
--- a/6845_crtc_timing.xlsx
+++ b/6845_crtc_timing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\iCloudDrive\Documents\Developer\BBC_Micro\Programs\Game_01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\BBC_Micro\Programs\game_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7601B7DB-33C7-4F82-A7DC-05BB19A242AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE47749-DD52-4855-841F-24FCAA9FDA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{E881977C-AD55-4380-9786-6EB6D25147A4}"/>
   </bookViews>
@@ -747,7 +747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -889,12 +889,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -931,7 +925,7 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -994,9 +988,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1027,13 +1018,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1054,13 +1042,13 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1111,7 +1099,7 @@
     <xf numFmtId="0" fontId="0" fillId="27" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1171,12 +1159,6 @@
     <xf numFmtId="11" fontId="0" fillId="24" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="25" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="24" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="4" fillId="25" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1192,22 +1174,13 @@
     <xf numFmtId="0" fontId="1" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1219,112 +1192,106 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6309,7 +6276,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9990A00-F3D8-4E56-9C95-A4A5E0390716}">
-  <dimension ref="A1:Q42"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
@@ -6324,45 +6291,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="K1" s="168" t="s">
+      <c r="K1" s="162" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="169" t="s">
+      <c r="L1" s="163" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="180" t="s">
+      <c r="A2" s="170" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="154" t="s">
+      <c r="C2" s="150" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="155" t="s">
+      <c r="D2" s="151" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="155" t="s">
+      <c r="E2" s="151" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="155" t="s">
+      <c r="F2" s="151" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="155" t="s">
+      <c r="G2" s="151" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="155" t="s">
+      <c r="H2" s="151" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="155" t="s">
+      <c r="I2" s="151" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="167" t="s">
+      <c r="J2" s="161" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="154" t="s">
+      <c r="K2" s="150" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="155" t="s">
+      <c r="L2" s="151" t="s">
         <v>75</v>
       </c>
       <c r="M2" s="3"/>
@@ -6372,1152 +6339,1094 @@
       <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="82">
+      <c r="C3" s="80">
         <v>0</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="84" t="s">
+      <c r="E3" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="84">
+      <c r="F3" s="82">
         <v>32</v>
       </c>
-      <c r="G3" s="85">
+      <c r="G3" s="83">
         <v>0</v>
       </c>
-      <c r="H3" s="86">
+      <c r="H3" s="84">
         <v>1</v>
       </c>
-      <c r="I3" s="80">
+      <c r="I3" s="78">
         <f>C3</f>
         <v>0</v>
       </c>
-      <c r="J3" s="80" t="str">
+      <c r="J3" s="78" t="str">
         <f>DEC2HEX(IF(G3=0,H3*F3*16,0),4)</f>
         <v>0200</v>
       </c>
-      <c r="K3" s="93" t="str" cm="1">
+      <c r="K3" s="91" t="str" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">IF(G3=0,DEC2HEX(HEX2DEC($A$3)),INDIRECT("K"&amp;(G3+3)))</f>
         <v>2C00</v>
       </c>
-      <c r="L3" s="156" t="str">
+      <c r="L3" s="152" t="str">
         <f ca="1">DEC2HEX(HEX2DEC(K3)+HEX2DEC(J3)-1)</f>
         <v>2DFF</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C4" s="157">
-        <f>C3+1</f>
+      <c r="C4" s="153">
+        <f t="shared" ref="C4:C41" si="0">C3+1</f>
         <v>1</v>
       </c>
-      <c r="D4" s="99" t="s">
+      <c r="D4" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="96" t="s">
+      <c r="E4" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="96">
+      <c r="F4" s="94">
         <v>32</v>
       </c>
-      <c r="G4" s="75">
+      <c r="G4" s="73">
         <v>0</v>
       </c>
-      <c r="H4" s="77">
+      <c r="H4" s="75">
         <v>1</v>
       </c>
-      <c r="I4" s="87">
+      <c r="I4" s="85">
         <f>I3+HEX2DEC(J3)/512</f>
         <v>1</v>
       </c>
-      <c r="J4" s="87" t="str">
-        <f t="shared" ref="J4:J26" si="0">DEC2HEX(IF(G4=0,H4*F4*16,0),4)</f>
+      <c r="J4" s="85" t="str">
+        <f t="shared" ref="J4:J26" si="1">DEC2HEX(IF(G4=0,H4*F4*16,0),4)</f>
         <v>0200</v>
       </c>
-      <c r="K4" s="91" t="str" cm="1">
+      <c r="K4" s="89" t="str" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">IF(G4=0,DEC2HEX(HEX2DEC($A$3)+I4*512,4),INDIRECT("K"&amp;(G4+3)))</f>
         <v>2E00</v>
       </c>
-      <c r="L4" s="158" t="str">
-        <f t="shared" ref="L4:L26" ca="1" si="1">DEC2HEX(HEX2DEC(K4)+HEX2DEC(J4)-1)</f>
+      <c r="L4" s="154" t="str">
+        <f t="shared" ref="L4:L26" ca="1" si="2">DEC2HEX(HEX2DEC(K4)+HEX2DEC(J4)-1)</f>
         <v>2FFF</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C5" s="159">
-        <f>C4+1</f>
+      <c r="C5" s="155">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="97">
+      <c r="F5" s="95">
         <v>32</v>
       </c>
-      <c r="G5" s="76">
+      <c r="G5" s="74">
         <v>0</v>
       </c>
-      <c r="H5" s="78">
+      <c r="H5" s="76">
         <v>1</v>
       </c>
-      <c r="I5" s="82">
-        <f t="shared" ref="I5:I26" si="2">I4+HEX2DEC(J4)/512</f>
+      <c r="I5" s="80">
+        <f t="shared" ref="I5:I26" si="3">I4+HEX2DEC(J4)/512</f>
         <v>2</v>
       </c>
-      <c r="J5" s="82" t="str">
-        <f t="shared" si="0"/>
+      <c r="J5" s="80" t="str">
+        <f t="shared" si="1"/>
         <v>0200</v>
       </c>
-      <c r="K5" s="94" t="str" cm="1">
+      <c r="K5" s="92" t="str" cm="1">
         <f t="array" aca="1" ref="K5" ca="1">IF(G5=0,DEC2HEX(HEX2DEC($A$3)+I5*512,4),INDIRECT("K"&amp;(G5+3)))</f>
         <v>3000</v>
       </c>
-      <c r="L5" s="160" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L5" s="156" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>31FF</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C6" s="161">
-        <f>C5+1</f>
+      <c r="C6" s="157">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="98" t="s">
+      <c r="E6" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="98">
+      <c r="F6" s="96">
         <v>32</v>
       </c>
-      <c r="G6" s="88">
+      <c r="G6" s="86">
         <v>0</v>
       </c>
-      <c r="H6" s="79">
+      <c r="H6" s="77">
         <v>1</v>
       </c>
-      <c r="I6" s="89">
-        <f t="shared" si="2"/>
+      <c r="I6" s="87">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="J6" s="89" t="str">
-        <f t="shared" si="0"/>
+      <c r="J6" s="87" t="str">
+        <f t="shared" si="1"/>
         <v>0200</v>
       </c>
-      <c r="K6" s="92" t="str" cm="1">
+      <c r="K6" s="90" t="str" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">IF(G6=0,DEC2HEX(HEX2DEC($A$3)+I6*512,4),INDIRECT("K"&amp;(G6+3)))</f>
         <v>3200</v>
       </c>
-      <c r="L6" s="162" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L6" s="158" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>33FF</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C7" s="80">
-        <f>C6+1</f>
+      <c r="C7" s="78">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D7" s="71" t="s">
+      <c r="D7" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="E7" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="84">
+      <c r="F7" s="82">
         <v>32</v>
       </c>
-      <c r="G7" s="85">
+      <c r="G7" s="83">
         <v>0</v>
       </c>
-      <c r="H7" s="86">
+      <c r="H7" s="84">
         <v>4</v>
       </c>
-      <c r="I7" s="80">
-        <f t="shared" si="2"/>
+      <c r="I7" s="78">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="J7" s="80" t="str">
-        <f t="shared" si="0"/>
+      <c r="J7" s="78" t="str">
+        <f t="shared" si="1"/>
         <v>0800</v>
       </c>
-      <c r="K7" s="95" t="str" cm="1">
+      <c r="K7" s="93" t="str" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">IF(G7=0,DEC2HEX(HEX2DEC($A$3)+I7*512,4),INDIRECT("K"&amp;(G7+3)))</f>
         <v>3400</v>
       </c>
-      <c r="L7" s="163" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L7" s="152" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>3BFF</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C8" s="89">
-        <f>C7+1</f>
+      <c r="C8" s="87">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D8" s="73" t="s">
+      <c r="D8" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="74" t="s">
+      <c r="E8" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="74">
+      <c r="F8" s="72">
         <v>32</v>
       </c>
-      <c r="G8" s="88">
+      <c r="G8" s="86">
         <v>0</v>
       </c>
-      <c r="H8" s="79">
+      <c r="H8" s="77">
         <v>4</v>
       </c>
-      <c r="I8" s="89">
-        <f t="shared" si="2"/>
+      <c r="I8" s="87">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="J8" s="89" t="str">
-        <f t="shared" si="0"/>
+      <c r="J8" s="87" t="str">
+        <f t="shared" si="1"/>
         <v>0800</v>
       </c>
-      <c r="K8" s="92" t="str" cm="1">
+      <c r="K8" s="90" t="str" cm="1">
         <f t="array" aca="1" ref="K8" ca="1">IF(G8=0,DEC2HEX(HEX2DEC($A$3)+I8*512,4),INDIRECT("K"&amp;(G8+3)))</f>
         <v>3C00</v>
       </c>
-      <c r="L8" s="164" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L8" s="158" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>43FF</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C9" s="80">
-        <f>C8+1</f>
+      <c r="C9" s="78">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="84" t="s">
+      <c r="E9" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="84">
+      <c r="F9" s="82">
         <v>32</v>
       </c>
-      <c r="G9" s="85">
+      <c r="G9" s="83">
         <v>0</v>
       </c>
-      <c r="H9" s="86">
+      <c r="H9" s="84">
         <v>4</v>
       </c>
-      <c r="I9" s="80">
-        <f t="shared" si="2"/>
+      <c r="I9" s="78">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="J9" s="80" t="str">
-        <f t="shared" si="0"/>
+      <c r="J9" s="78" t="str">
+        <f t="shared" si="1"/>
         <v>0800</v>
       </c>
-      <c r="K9" s="95" t="str" cm="1">
+      <c r="K9" s="93" t="str" cm="1">
         <f t="array" aca="1" ref="K9" ca="1">IF(G9=0,DEC2HEX(HEX2DEC($A$3)+I9*512,4),INDIRECT("K"&amp;(G9+3)))</f>
         <v>4400</v>
       </c>
-      <c r="L9" s="163" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L9" s="152" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>4BFF</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C10" s="89">
-        <f>C9+1</f>
+      <c r="C10" s="87">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="74" t="s">
+      <c r="E10" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="74">
+      <c r="F10" s="72">
         <v>32</v>
       </c>
-      <c r="G10" s="88">
+      <c r="G10" s="86">
         <v>0</v>
       </c>
-      <c r="H10" s="79">
+      <c r="H10" s="77">
         <v>4</v>
       </c>
-      <c r="I10" s="89">
-        <f t="shared" si="2"/>
+      <c r="I10" s="87">
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="J10" s="89" t="str">
-        <f t="shared" si="0"/>
+      <c r="J10" s="87" t="str">
+        <f t="shared" si="1"/>
         <v>0800</v>
       </c>
-      <c r="K10" s="92" t="str" cm="1">
+      <c r="K10" s="90" t="str" cm="1">
         <f t="array" aca="1" ref="K10" ca="1">IF(G10=0,DEC2HEX(HEX2DEC($A$3)+I10*512,4),INDIRECT("K"&amp;(G10+3)))</f>
         <v>4C00</v>
       </c>
-      <c r="L10" s="164" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L10" s="158" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>53FF</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C11" s="80">
-        <f>C10+1</f>
+      <c r="C11" s="78">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D11" s="71" t="s">
+      <c r="D11" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="84" t="s">
+      <c r="E11" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="84">
+      <c r="F11" s="82">
         <v>32</v>
       </c>
-      <c r="G11" s="85">
+      <c r="G11" s="83">
         <v>4</v>
       </c>
-      <c r="H11" s="86">
+      <c r="H11" s="84">
         <v>4</v>
       </c>
-      <c r="I11" s="80">
-        <f t="shared" si="2"/>
+      <c r="I11" s="78">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J11" s="80" t="str">
-        <f t="shared" si="0"/>
+      <c r="J11" s="78" t="str">
+        <f t="shared" si="1"/>
         <v>0000</v>
       </c>
-      <c r="K11" s="95" t="str" cm="1">
+      <c r="K11" s="93" t="str" cm="1">
         <f t="array" aca="1" ref="K11" ca="1">IF(G11=0,DEC2HEX(HEX2DEC($A$3)+I11*512,4),INDIRECT("K"&amp;(G11+3)))</f>
         <v>3400</v>
       </c>
-      <c r="L11" s="165" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L11" s="159" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>33FF</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C12" s="89">
-        <f>C11+1</f>
+      <c r="C12" s="87">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D12" s="73" t="s">
+      <c r="D12" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="74">
+      <c r="F12" s="72">
         <v>32</v>
       </c>
-      <c r="G12" s="88">
+      <c r="G12" s="86">
         <v>5</v>
       </c>
-      <c r="H12" s="79">
+      <c r="H12" s="77">
         <v>4</v>
       </c>
-      <c r="I12" s="89">
-        <f t="shared" si="2"/>
+      <c r="I12" s="87">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J12" s="89" t="str">
-        <f t="shared" si="0"/>
+      <c r="J12" s="87" t="str">
+        <f t="shared" si="1"/>
         <v>0000</v>
       </c>
-      <c r="K12" s="92" t="str" cm="1">
+      <c r="K12" s="90" t="str" cm="1">
         <f t="array" aca="1" ref="K12" ca="1">IF(G12=0,DEC2HEX(HEX2DEC($A$3)+I12*512,4),INDIRECT("K"&amp;(G12+3)))</f>
         <v>3C00</v>
       </c>
-      <c r="L12" s="166" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L12" s="160" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>3BFF</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C13" s="80">
-        <f>C12+1</f>
+      <c r="C13" s="78">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D13" s="71" t="s">
+      <c r="D13" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="84" t="s">
+      <c r="E13" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="84">
+      <c r="F13" s="82">
         <v>32</v>
       </c>
-      <c r="G13" s="85">
+      <c r="G13" s="83">
         <v>6</v>
       </c>
-      <c r="H13" s="86">
+      <c r="H13" s="84">
         <v>4</v>
       </c>
-      <c r="I13" s="80">
-        <f t="shared" si="2"/>
+      <c r="I13" s="78">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J13" s="80" t="str">
-        <f t="shared" si="0"/>
+      <c r="J13" s="78" t="str">
+        <f t="shared" si="1"/>
         <v>0000</v>
       </c>
-      <c r="K13" s="95" t="str" cm="1">
+      <c r="K13" s="93" t="str" cm="1">
         <f t="array" aca="1" ref="K13" ca="1">IF(G13=0,DEC2HEX(HEX2DEC($A$3)+I13*512,4),INDIRECT("K"&amp;(G13+3)))</f>
         <v>4400</v>
       </c>
-      <c r="L13" s="165" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L13" s="159" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>43FF</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C14" s="89">
-        <f>C13+1</f>
+      <c r="C14" s="87">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D14" s="73" t="s">
+      <c r="D14" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="74" t="s">
+      <c r="E14" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="74">
+      <c r="F14" s="72">
         <v>32</v>
       </c>
-      <c r="G14" s="88">
+      <c r="G14" s="86">
         <v>7</v>
       </c>
-      <c r="H14" s="79">
+      <c r="H14" s="77">
         <v>4</v>
       </c>
-      <c r="I14" s="89">
-        <f t="shared" si="2"/>
+      <c r="I14" s="87">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J14" s="89" t="str">
-        <f t="shared" si="0"/>
+      <c r="J14" s="87" t="str">
+        <f t="shared" si="1"/>
         <v>0000</v>
       </c>
-      <c r="K14" s="92" t="str" cm="1">
+      <c r="K14" s="90" t="str" cm="1">
         <f t="array" aca="1" ref="K14" ca="1">IF(G14=0,DEC2HEX(HEX2DEC($A$3)+I14*512,4),INDIRECT("K"&amp;(G14+3)))</f>
         <v>4C00</v>
       </c>
-      <c r="L14" s="166" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L14" s="160" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>4BFF</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C15" s="80">
-        <f>C14+1</f>
+      <c r="C15" s="78">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D15" s="71" t="s">
+      <c r="D15" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="84" t="s">
+      <c r="E15" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="84">
+      <c r="F15" s="82">
         <v>32</v>
       </c>
-      <c r="G15" s="85">
+      <c r="G15" s="83">
         <v>0</v>
       </c>
-      <c r="H15" s="86">
+      <c r="H15" s="84">
         <v>1</v>
       </c>
-      <c r="I15" s="80">
-        <f t="shared" si="2"/>
+      <c r="I15" s="78">
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="J15" s="80" t="str">
-        <f t="shared" si="0"/>
+      <c r="J15" s="78" t="str">
+        <f t="shared" si="1"/>
         <v>0200</v>
       </c>
-      <c r="K15" s="95" t="str" cm="1">
+      <c r="K15" s="93" t="str" cm="1">
         <f t="array" aca="1" ref="K15" ca="1">IF(G15=0,DEC2HEX(HEX2DEC($A$3)+I15*512,4),INDIRECT("K"&amp;(G15+3)))</f>
         <v>5400</v>
       </c>
-      <c r="L15" s="163" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L15" s="152" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>55FF</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C16" s="89">
-        <f>C15+1</f>
+      <c r="C16" s="87">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D16" s="73" t="s">
+      <c r="D16" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="74" t="s">
+      <c r="E16" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="74">
+      <c r="F16" s="72">
         <v>32</v>
       </c>
-      <c r="G16" s="88">
+      <c r="G16" s="86">
         <v>0</v>
       </c>
-      <c r="H16" s="79">
+      <c r="H16" s="77">
         <v>1</v>
       </c>
-      <c r="I16" s="89">
-        <f t="shared" si="2"/>
+      <c r="I16" s="87">
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="J16" s="89" t="str">
-        <f t="shared" si="0"/>
+      <c r="J16" s="87" t="str">
+        <f t="shared" si="1"/>
         <v>0200</v>
       </c>
-      <c r="K16" s="92" t="str" cm="1">
+      <c r="K16" s="90" t="str" cm="1">
         <f t="array" aca="1" ref="K16" ca="1">IF(G16=0,DEC2HEX(HEX2DEC($A$3)+I16*512,4),INDIRECT("K"&amp;(G16+3)))</f>
         <v>5600</v>
       </c>
-      <c r="L16" s="164" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L16" s="158" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>57FF</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C17" s="80">
-        <f>C16+1</f>
+      <c r="C17" s="78">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D17" s="71" t="s">
+      <c r="D17" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="84" t="s">
+      <c r="E17" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="84">
+      <c r="F17" s="82">
         <v>32</v>
       </c>
-      <c r="G17" s="85">
+      <c r="G17" s="83">
         <v>0</v>
       </c>
-      <c r="H17" s="86">
+      <c r="H17" s="84">
         <v>4</v>
       </c>
-      <c r="I17" s="80">
-        <f t="shared" si="2"/>
+      <c r="I17" s="78">
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="J17" s="80" t="str">
-        <f t="shared" si="0"/>
+      <c r="J17" s="78" t="str">
+        <f t="shared" si="1"/>
         <v>0800</v>
       </c>
-      <c r="K17" s="95" t="str" cm="1">
+      <c r="K17" s="93" t="str" cm="1">
         <f t="array" aca="1" ref="K17" ca="1">IF(G17=0,DEC2HEX(HEX2DEC($A$3)+I17*512,4),INDIRECT("K"&amp;(G17+3)))</f>
         <v>5800</v>
       </c>
-      <c r="L17" s="156" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L17" s="152" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>5FFF</v>
       </c>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C18" s="89">
-        <f>C17+1</f>
+      <c r="C18" s="87">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D18" s="73" t="s">
+      <c r="D18" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="74" t="s">
+      <c r="E18" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="74">
+      <c r="F18" s="72">
         <v>32</v>
       </c>
-      <c r="G18" s="88">
+      <c r="G18" s="86">
         <v>0</v>
       </c>
-      <c r="H18" s="79">
+      <c r="H18" s="77">
         <v>4</v>
       </c>
-      <c r="I18" s="89">
-        <f t="shared" si="2"/>
+      <c r="I18" s="87">
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="J18" s="89" t="str">
-        <f t="shared" si="0"/>
+      <c r="J18" s="87" t="str">
+        <f t="shared" si="1"/>
         <v>0800</v>
       </c>
-      <c r="K18" s="92" t="str" cm="1">
+      <c r="K18" s="90" t="str" cm="1">
         <f t="array" aca="1" ref="K18" ca="1">IF(G18=0,DEC2HEX(HEX2DEC($A$3)+I18*512,4),INDIRECT("K"&amp;(G18+3)))</f>
         <v>6000</v>
       </c>
-      <c r="L18" s="162" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L18" s="158" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>67FF</v>
       </c>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C19" s="80">
-        <f>C18+1</f>
+      <c r="C19" s="78">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="D19" s="71" t="s">
+      <c r="D19" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="84" t="s">
+      <c r="E19" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="84">
+      <c r="F19" s="82">
         <v>32</v>
       </c>
-      <c r="G19" s="85">
+      <c r="G19" s="83">
         <v>0</v>
       </c>
-      <c r="H19" s="86">
+      <c r="H19" s="84">
         <v>2</v>
       </c>
-      <c r="I19" s="80">
-        <f t="shared" si="2"/>
+      <c r="I19" s="78">
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="J19" s="80" t="str">
-        <f t="shared" si="0"/>
+      <c r="J19" s="78" t="str">
+        <f t="shared" si="1"/>
         <v>0400</v>
       </c>
-      <c r="K19" s="95" t="str" cm="1">
+      <c r="K19" s="93" t="str" cm="1">
         <f t="array" aca="1" ref="K19" ca="1">IF(G19=0,DEC2HEX(HEX2DEC($A$3)+I19*512,4),INDIRECT("K"&amp;(G19+3)))</f>
         <v>6800</v>
       </c>
-      <c r="L19" s="156" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L19" s="152" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>6BFF</v>
       </c>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C20" s="89">
-        <f>C19+1</f>
+      <c r="C20" s="87">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D20" s="73" t="s">
+      <c r="D20" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="74" t="s">
+      <c r="E20" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="74">
+      <c r="F20" s="72">
         <v>32</v>
       </c>
-      <c r="G20" s="88">
+      <c r="G20" s="86">
         <v>0</v>
       </c>
-      <c r="H20" s="79">
+      <c r="H20" s="77">
         <v>2</v>
       </c>
-      <c r="I20" s="89">
-        <f t="shared" si="2"/>
+      <c r="I20" s="87">
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="J20" s="89" t="str">
-        <f t="shared" si="0"/>
+      <c r="J20" s="87" t="str">
+        <f t="shared" si="1"/>
         <v>0400</v>
       </c>
-      <c r="K20" s="92" t="str" cm="1">
+      <c r="K20" s="90" t="str" cm="1">
         <f t="array" aca="1" ref="K20" ca="1">IF(G20=0,DEC2HEX(HEX2DEC($A$3)+I20*512,4),INDIRECT("K"&amp;(G20+3)))</f>
         <v>6C00</v>
       </c>
-      <c r="L20" s="166" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L20" s="160" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>6FFF</v>
       </c>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C21" s="80">
-        <f>C20+1</f>
+      <c r="C21" s="78">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D21" s="71" t="s">
+      <c r="D21" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="84" t="s">
+      <c r="E21" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="84">
+      <c r="F21" s="82">
         <v>32</v>
       </c>
-      <c r="G21" s="85">
+      <c r="G21" s="83">
         <v>16</v>
       </c>
-      <c r="H21" s="86">
+      <c r="H21" s="84">
         <v>2</v>
       </c>
-      <c r="I21" s="80">
-        <f t="shared" si="2"/>
+      <c r="I21" s="78">
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="J21" s="80" t="str">
-        <f t="shared" si="0"/>
+      <c r="J21" s="78" t="str">
+        <f t="shared" si="1"/>
         <v>0000</v>
       </c>
-      <c r="K21" s="95" t="str" cm="1">
+      <c r="K21" s="93" t="str" cm="1">
         <f t="array" aca="1" ref="K21" ca="1">IF(G21=0,DEC2HEX(HEX2DEC($A$3)+I21*512,4),INDIRECT("K"&amp;(G21+3)))</f>
         <v>6800</v>
       </c>
-      <c r="L21" s="165" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L21" s="159" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>67FF</v>
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C22" s="89">
-        <f>C21+1</f>
+      <c r="C22" s="87">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D22" s="73" t="s">
+      <c r="D22" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="74" t="s">
+      <c r="E22" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="74">
+      <c r="F22" s="72">
         <v>32</v>
       </c>
-      <c r="G22" s="88">
+      <c r="G22" s="86">
         <v>17</v>
       </c>
-      <c r="H22" s="79">
+      <c r="H22" s="77">
         <v>2</v>
       </c>
-      <c r="I22" s="89">
-        <f t="shared" si="2"/>
+      <c r="I22" s="87">
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="J22" s="89" t="str">
-        <f t="shared" si="0"/>
+      <c r="J22" s="87" t="str">
+        <f t="shared" si="1"/>
         <v>0000</v>
       </c>
-      <c r="K22" s="92" t="str" cm="1">
+      <c r="K22" s="90" t="str" cm="1">
         <f t="array" aca="1" ref="K22" ca="1">IF(G22=0,DEC2HEX(HEX2DEC($A$3)+I22*512,4),INDIRECT("K"&amp;(G22+3)))</f>
         <v>6C00</v>
       </c>
-      <c r="L22" s="166" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L22" s="160" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>6BFF</v>
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C23" s="80">
-        <f>C22+1</f>
+      <c r="C23" s="78">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D23" s="71" t="s">
+      <c r="D23" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="84" t="s">
+      <c r="E23" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="84">
+      <c r="F23" s="82">
         <v>32</v>
       </c>
-      <c r="G23" s="85">
+      <c r="G23" s="83">
         <v>0</v>
       </c>
-      <c r="H23" s="86">
+      <c r="H23" s="84">
         <v>4</v>
       </c>
-      <c r="I23" s="80">
-        <f t="shared" si="2"/>
+      <c r="I23" s="78">
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="J23" s="80" t="str">
-        <f t="shared" si="0"/>
+      <c r="J23" s="78" t="str">
+        <f t="shared" si="1"/>
         <v>0800</v>
       </c>
-      <c r="K23" s="95" t="str" cm="1">
+      <c r="K23" s="93" t="str" cm="1">
         <f t="array" aca="1" ref="K23" ca="1">IF(G23=0,DEC2HEX(HEX2DEC($A$3)+I23*512,4),INDIRECT("K"&amp;(G23+3)))</f>
         <v>7000</v>
       </c>
-      <c r="L23" s="165" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L23" s="159" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>77FF</v>
       </c>
     </row>
     <row r="24" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C24" s="89">
-        <f>C23+1</f>
+      <c r="C24" s="87">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="D24" s="73" t="s">
+      <c r="D24" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="74" t="s">
+      <c r="E24" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="74">
+      <c r="F24" s="72">
         <v>32</v>
       </c>
-      <c r="G24" s="88">
+      <c r="G24" s="86">
         <v>0</v>
       </c>
-      <c r="H24" s="79">
+      <c r="H24" s="77">
         <v>4</v>
       </c>
-      <c r="I24" s="89">
-        <f t="shared" si="2"/>
+      <c r="I24" s="87">
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="J24" s="89" t="str">
-        <f t="shared" si="0"/>
+      <c r="J24" s="87" t="str">
+        <f t="shared" si="1"/>
         <v>0800</v>
       </c>
-      <c r="K24" s="92" t="str" cm="1">
+      <c r="K24" s="90" t="str" cm="1">
         <f t="array" aca="1" ref="K24" ca="1">IF(G24=0,DEC2HEX(HEX2DEC($A$3)+I24*512,4),INDIRECT("K"&amp;(G24+3)))</f>
         <v>7800</v>
       </c>
-      <c r="L24" s="166" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L24" s="160" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>7FFF</v>
       </c>
     </row>
     <row r="25" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C25" s="80">
-        <f>C24+1</f>
+      <c r="C25" s="78">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="D25" s="71" t="s">
+      <c r="D25" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="84" t="s">
+      <c r="E25" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="84">
+      <c r="F25" s="82">
         <v>32</v>
       </c>
-      <c r="G25" s="85">
+      <c r="G25" s="83">
         <v>12</v>
       </c>
-      <c r="H25" s="86">
+      <c r="H25" s="84">
         <v>1</v>
       </c>
-      <c r="I25" s="80">
-        <f t="shared" si="2"/>
+      <c r="I25" s="78">
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="J25" s="80" t="str">
-        <f t="shared" si="0"/>
+      <c r="J25" s="78" t="str">
+        <f t="shared" si="1"/>
         <v>0000</v>
       </c>
-      <c r="K25" s="95" t="str" cm="1">
+      <c r="K25" s="93" t="str" cm="1">
         <f t="array" aca="1" ref="K25" ca="1">IF(G25=0,DEC2HEX(HEX2DEC($A$3)+I25*512,4),INDIRECT("K"&amp;(G25+3)))</f>
         <v>5400</v>
       </c>
-      <c r="L25" s="165" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L25" s="159" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>53FF</v>
       </c>
     </row>
     <row r="26" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C26" s="81">
-        <f>C25+1</f>
+      <c r="C26" s="79">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="D26" s="73" t="s">
+      <c r="D26" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="74" t="s">
+      <c r="E26" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="F26" s="74">
+      <c r="F26" s="72">
         <v>32</v>
       </c>
-      <c r="G26" s="88">
+      <c r="G26" s="86">
         <v>13</v>
       </c>
-      <c r="H26" s="79">
+      <c r="H26" s="77">
         <v>1</v>
       </c>
-      <c r="I26" s="89">
-        <f t="shared" si="2"/>
+      <c r="I26" s="87">
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="J26" s="89" t="str">
-        <f t="shared" si="0"/>
+      <c r="J26" s="87" t="str">
+        <f t="shared" si="1"/>
         <v>0000</v>
       </c>
-      <c r="K26" s="92" t="str" cm="1">
+      <c r="K26" s="90" t="str" cm="1">
         <f t="array" aca="1" ref="K26" ca="1">IF(G26=0,DEC2HEX(HEX2DEC($A$3)+I26*512,4),INDIRECT("K"&amp;(G26+3)))</f>
         <v>5600</v>
       </c>
-      <c r="L26" s="166" t="str">
-        <f t="shared" ca="1" si="1"/>
+      <c r="L26" s="160" t="str">
+        <f t="shared" ca="1" si="2"/>
         <v>55FF</v>
       </c>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C27" s="80">
-        <f>C26+1</f>
+      <c r="C27" s="78">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="D27" s="179" t="s">
+      <c r="D27" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="171"/>
-      <c r="F27" s="171"/>
-      <c r="G27" s="171"/>
-      <c r="H27" s="171"/>
-      <c r="I27" s="171"/>
-      <c r="J27" s="171"/>
-      <c r="K27" s="171"/>
-      <c r="L27" s="103"/>
+      <c r="E27" s="100"/>
+      <c r="F27" s="100"/>
+      <c r="G27" s="100"/>
+      <c r="H27" s="100"/>
+      <c r="I27" s="100"/>
+      <c r="J27" s="100"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="101"/>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C28" s="81">
-        <f>C27+1</f>
+      <c r="C28" s="79">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="D28" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="E28" s="104"/>
-      <c r="F28" s="104"/>
-      <c r="G28" s="104"/>
-      <c r="H28" s="104"/>
-      <c r="I28" s="104"/>
-      <c r="J28" s="172"/>
-      <c r="K28" s="104"/>
+      <c r="J28" s="10"/>
       <c r="L28" s="68"/>
     </row>
     <row r="29" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C29" s="82">
-        <f>C28+1</f>
+      <c r="C29" s="80">
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="D29" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="104"/>
-      <c r="F29" s="104"/>
-      <c r="G29" s="104"/>
-      <c r="H29" s="104"/>
-      <c r="I29" s="104"/>
-      <c r="J29" s="104"/>
-      <c r="K29" s="104"/>
       <c r="L29" s="68"/>
     </row>
     <row r="30" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C30" s="81">
-        <f>C29+1</f>
+      <c r="C30" s="79">
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="D30" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="104"/>
-      <c r="F30" s="104"/>
-      <c r="G30" s="104"/>
-      <c r="H30" s="104"/>
-      <c r="I30" s="104"/>
-      <c r="J30" s="104"/>
-      <c r="K30" s="104"/>
       <c r="L30" s="68"/>
     </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C31" s="82">
-        <f>C30+1</f>
+      <c r="C31" s="80">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="D31" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="104"/>
-      <c r="F31" s="104"/>
-      <c r="G31" s="104"/>
-      <c r="H31" s="104"/>
-      <c r="I31" s="104"/>
-      <c r="J31" s="104"/>
-      <c r="K31" s="104"/>
       <c r="L31" s="68"/>
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C32" s="81">
-        <f>C31+1</f>
+      <c r="C32" s="79">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="D32" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="104"/>
-      <c r="F32" s="104"/>
-      <c r="G32" s="104"/>
-      <c r="H32" s="104"/>
-      <c r="I32" s="104"/>
-      <c r="J32" s="104"/>
-      <c r="K32" s="104"/>
       <c r="L32" s="68"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C33" s="82">
-        <f>C32+1</f>
+      <c r="C33" s="80">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="D33" s="106" t="s">
+      <c r="D33" s="103" t="s">
         <v>63</v>
       </c>
-      <c r="E33" s="105"/>
-      <c r="F33" s="105"/>
-      <c r="G33" s="105"/>
-      <c r="H33" s="105"/>
-      <c r="I33" s="105"/>
-      <c r="J33" s="105"/>
-      <c r="K33" s="105"/>
-      <c r="L33" s="106"/>
+      <c r="E33" s="102"/>
+      <c r="F33" s="102"/>
+      <c r="G33" s="102"/>
+      <c r="H33" s="102"/>
+      <c r="I33" s="102"/>
+      <c r="J33" s="102"/>
+      <c r="K33" s="102"/>
+      <c r="L33" s="103"/>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C34" s="87">
-        <f>C33+1</f>
+      <c r="C34" s="85">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="D34" s="174" t="s">
+      <c r="D34" s="165" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="173"/>
-      <c r="F34" s="173"/>
-      <c r="G34" s="173"/>
-      <c r="H34" s="173"/>
-      <c r="I34" s="173"/>
-      <c r="J34" s="173"/>
-      <c r="K34" s="173"/>
-      <c r="L34" s="174"/>
+      <c r="E34" s="164"/>
+      <c r="F34" s="164"/>
+      <c r="G34" s="164"/>
+      <c r="H34" s="164"/>
+      <c r="I34" s="164"/>
+      <c r="J34" s="164"/>
+      <c r="K34" s="164"/>
+      <c r="L34" s="165"/>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C35" s="82">
-        <f>C34+1</f>
+      <c r="C35" s="80">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="D35" s="176" t="s">
+      <c r="D35" s="167" t="s">
         <v>92</v>
       </c>
-      <c r="E35" s="175"/>
-      <c r="F35" s="175"/>
-      <c r="G35" s="175"/>
-      <c r="H35" s="175"/>
-      <c r="I35" s="175"/>
-      <c r="J35" s="175"/>
-      <c r="K35" s="175"/>
-      <c r="L35" s="176"/>
+      <c r="E35" s="166"/>
+      <c r="F35" s="166"/>
+      <c r="G35" s="166"/>
+      <c r="H35" s="166"/>
+      <c r="I35" s="166"/>
+      <c r="J35" s="166"/>
+      <c r="K35" s="166"/>
+      <c r="L35" s="167"/>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C36" s="89">
-        <f>C35+1</f>
+      <c r="C36" s="87">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="D36" s="178" t="s">
+      <c r="D36" s="169" t="s">
         <v>92</v>
       </c>
-      <c r="E36" s="177"/>
-      <c r="F36" s="177"/>
-      <c r="G36" s="177"/>
-      <c r="H36" s="177"/>
-      <c r="I36" s="177"/>
-      <c r="J36" s="177"/>
-      <c r="K36" s="177"/>
-      <c r="L36" s="178"/>
+      <c r="E36" s="168"/>
+      <c r="F36" s="168"/>
+      <c r="G36" s="168"/>
+      <c r="H36" s="168"/>
+      <c r="I36" s="168"/>
+      <c r="J36" s="168"/>
+      <c r="K36" s="168"/>
+      <c r="L36" s="169"/>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C37" s="82">
-        <f>C36+1</f>
+      <c r="C37" s="80">
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="D37" s="103" t="s">
+      <c r="D37" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="E37" s="102"/>
-      <c r="F37" s="102"/>
-      <c r="G37" s="102"/>
-      <c r="H37" s="102"/>
-      <c r="I37" s="102"/>
-      <c r="J37" s="102"/>
-      <c r="K37" s="102"/>
-      <c r="L37" s="103"/>
+      <c r="E37" s="100"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="100"/>
+      <c r="H37" s="100"/>
+      <c r="I37" s="100"/>
+      <c r="J37" s="100"/>
+      <c r="K37" s="100"/>
+      <c r="L37" s="101"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C38" s="81">
-        <f>C37+1</f>
+      <c r="C38" s="79">
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="D38" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="104"/>
-      <c r="F38" s="104"/>
-      <c r="G38" s="104"/>
-      <c r="H38" s="104"/>
-      <c r="I38" s="104"/>
-      <c r="J38" s="104"/>
-      <c r="K38" s="104"/>
       <c r="L38" s="68"/>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C39" s="82">
-        <f>C38+1</f>
+      <c r="C39" s="80">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="D39" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="104"/>
-      <c r="F39" s="104"/>
-      <c r="G39" s="104"/>
-      <c r="H39" s="104"/>
-      <c r="I39" s="104"/>
-      <c r="J39" s="104"/>
-      <c r="K39" s="104"/>
       <c r="L39" s="68"/>
     </row>
     <row r="40" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C40" s="81">
-        <f>C39+1</f>
+      <c r="C40" s="79">
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="D40" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="104"/>
-      <c r="F40" s="104"/>
-      <c r="G40" s="104"/>
-      <c r="H40" s="104"/>
-      <c r="I40" s="104"/>
-      <c r="J40" s="104"/>
-      <c r="K40" s="104"/>
       <c r="L40" s="68"/>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C41" s="90">
-        <f>C40+1</f>
+      <c r="C41" s="88">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="D41" s="106" t="s">
+      <c r="D41" s="103" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="105"/>
-      <c r="F41" s="105"/>
-      <c r="G41" s="105"/>
-      <c r="H41" s="105"/>
-      <c r="I41" s="105"/>
-      <c r="J41" s="105"/>
-      <c r="K41" s="105"/>
-      <c r="L41" s="106"/>
-    </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C42" s="170"/>
+      <c r="E41" s="102"/>
+      <c r="F41" s="102"/>
+      <c r="G41" s="102"/>
+      <c r="H41" s="102"/>
+      <c r="I41" s="102"/>
+      <c r="J41" s="102"/>
+      <c r="K41" s="102"/>
+      <c r="L41" s="103"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7528,8 +7437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F481C70-9657-4394-93E6-4755D8687536}">
   <dimension ref="B1:AT28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AV16" sqref="AV16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7545,521 +7454,521 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="AO1" s="186" t="s">
+      <c r="AO1" s="173" t="s">
         <v>80</v>
       </c>
-      <c r="AP1" s="188" t="s">
+      <c r="AP1" s="202" t="s">
         <v>93</v>
       </c>
-      <c r="AQ1" s="189"/>
-      <c r="AR1" s="183" t="s">
+      <c r="AQ1" s="203"/>
+      <c r="AR1" s="200" t="s">
         <v>94</v>
       </c>
-      <c r="AS1" s="184"/>
-      <c r="AT1" s="193" t="s">
+      <c r="AS1" s="201"/>
+      <c r="AT1" s="175" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="2:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="204">
+      <c r="D2" s="189">
         <v>0</v>
       </c>
-      <c r="E2" s="204">
+      <c r="E2" s="189">
         <f>D2+1</f>
         <v>1</v>
       </c>
-      <c r="F2" s="204">
+      <c r="F2" s="189">
         <f t="shared" ref="F2:AI2" si="0">E2+1</f>
         <v>2</v>
       </c>
-      <c r="G2" s="204">
+      <c r="G2" s="189">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H2" s="204">
+      <c r="H2" s="189">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I2" s="204">
+      <c r="I2" s="189">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J2" s="204">
+      <c r="J2" s="189">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K2" s="204">
+      <c r="K2" s="189">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="L2" s="204">
+      <c r="L2" s="189">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M2" s="204">
+      <c r="M2" s="189">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="N2" s="204">
+      <c r="N2" s="189">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O2" s="204">
+      <c r="O2" s="189">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="P2" s="204">
+      <c r="P2" s="189">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="Q2" s="204">
+      <c r="Q2" s="189">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="R2" s="204">
+      <c r="R2" s="189">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="S2" s="204">
+      <c r="S2" s="189">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="T2" s="204">
+      <c r="T2" s="189">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="U2" s="204">
+      <c r="U2" s="189">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="V2" s="204">
+      <c r="V2" s="189">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="W2" s="204">
+      <c r="W2" s="189">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="X2" s="203">
+      <c r="X2" s="188">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="Y2" s="203">
+      <c r="Y2" s="188">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="Z2" s="203">
+      <c r="Z2" s="188">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="AA2" s="203">
+      <c r="AA2" s="188">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="AB2" s="203">
+      <c r="AB2" s="188">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AC2" s="203">
+      <c r="AC2" s="188">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AD2" s="203">
+      <c r="AD2" s="188">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AE2" s="203">
+      <c r="AE2" s="188">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AF2" s="204">
+      <c r="AF2" s="189">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AG2" s="204">
+      <c r="AG2" s="189">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AH2" s="204">
+      <c r="AH2" s="189">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AI2" s="204">
+      <c r="AI2" s="189">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AO2" s="185" t="s">
+      <c r="AO2" s="172" t="s">
         <v>75</v>
       </c>
-      <c r="AP2" s="194" t="s">
+      <c r="AP2" s="179" t="s">
         <v>95</v>
       </c>
-      <c r="AQ2" s="194" t="s">
+      <c r="AQ2" s="179" t="s">
         <v>96</v>
       </c>
-      <c r="AR2" s="187" t="s">
+      <c r="AR2" s="174" t="s">
         <v>95</v>
       </c>
-      <c r="AS2" s="185" t="s">
+      <c r="AS2" s="172" t="s">
         <v>96</v>
       </c>
-      <c r="AT2" s="190" t="s">
+      <c r="AT2" s="176" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="107">
+      <c r="B3" s="104">
         <v>0</v>
       </c>
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="105" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="114" t="s">
+      <c r="D3" s="111" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="110" t="s">
+      <c r="E3" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="110" t="s">
+      <c r="F3" s="107" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="110"/>
-      <c r="J3" s="110" t="s">
+      <c r="G3" s="107"/>
+      <c r="J3" s="107" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="110" t="s">
+      <c r="K3" s="107" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="110" t="s">
+      <c r="L3" s="107" t="s">
         <v>84</v>
       </c>
-      <c r="M3" s="110" t="s">
+      <c r="M3" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="110" t="s">
+      <c r="N3" s="107" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="110" t="s">
+      <c r="O3" s="107" t="s">
         <v>90</v>
       </c>
-      <c r="P3" s="110">
+      <c r="P3" s="107">
         <v>0</v>
       </c>
-      <c r="Q3" s="110">
+      <c r="Q3" s="107">
         <v>0</v>
       </c>
-      <c r="R3" s="110">
+      <c r="R3" s="107">
         <v>0</v>
       </c>
-      <c r="S3" s="110">
+      <c r="S3" s="107">
         <v>0</v>
       </c>
-      <c r="T3" s="110">
+      <c r="T3" s="107">
         <v>0</v>
       </c>
-      <c r="U3" s="110">
+      <c r="U3" s="107">
         <v>0</v>
       </c>
-      <c r="V3" s="110"/>
-      <c r="W3" s="110"/>
-      <c r="X3" s="205"/>
-      <c r="Y3" s="206"/>
-      <c r="Z3" s="206"/>
-      <c r="AA3" s="206"/>
-      <c r="AB3" s="206"/>
-      <c r="AC3" s="206"/>
-      <c r="AD3" s="206"/>
-      <c r="AE3" s="207"/>
-      <c r="AF3" s="110" t="s">
+      <c r="V3" s="107"/>
+      <c r="W3" s="107"/>
+      <c r="X3" s="190"/>
+      <c r="Y3" s="191"/>
+      <c r="Z3" s="191"/>
+      <c r="AA3" s="191"/>
+      <c r="AB3" s="191"/>
+      <c r="AC3" s="191"/>
+      <c r="AD3" s="191"/>
+      <c r="AE3" s="192"/>
+      <c r="AF3" s="107" t="s">
         <v>83</v>
       </c>
-      <c r="AG3" s="110" t="s">
+      <c r="AG3" s="107" t="s">
         <v>85</v>
       </c>
-      <c r="AH3" s="110" t="s">
+      <c r="AH3" s="107" t="s">
         <v>86</v>
       </c>
-      <c r="AI3" s="111" t="s">
+      <c r="AI3" s="108" t="s">
         <v>87</v>
       </c>
-      <c r="AJ3" s="208">
+      <c r="AJ3" s="193">
         <v>0</v>
       </c>
-      <c r="AO3" s="116" t="str">
+      <c r="AO3" s="112" t="str">
         <f>DEC2HEX(AJ3*2+44,2)</f>
         <v>2C</v>
       </c>
-      <c r="AP3" s="191">
+      <c r="AP3" s="177">
         <v>-1</v>
       </c>
-      <c r="AQ3" s="192">
+      <c r="AQ3" s="178">
         <v>-1</v>
       </c>
-      <c r="AR3" s="182">
+      <c r="AR3" s="171">
         <v>-1</v>
       </c>
-      <c r="AS3" s="182">
+      <c r="AS3" s="171">
         <v>-1</v>
       </c>
-      <c r="AT3" s="109">
+      <c r="AT3" s="106">
         <v>-1</v>
       </c>
     </row>
     <row r="4" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="112">
-        <f>B3+1</f>
+      <c r="B4" s="109">
+        <f t="shared" ref="B4:B26" si="1">B3+1</f>
         <v>1</v>
       </c>
-      <c r="C4" s="113" t="s">
+      <c r="C4" s="110" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="130"/>
-      <c r="E4" s="131"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="131"/>
-      <c r="J4" s="131"/>
-      <c r="K4" s="131"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="132"/>
-      <c r="N4" s="132"/>
-      <c r="O4" s="131"/>
-      <c r="P4" s="131"/>
-      <c r="Q4" s="131"/>
-      <c r="R4" s="131"/>
-      <c r="S4" s="132"/>
-      <c r="T4" s="132"/>
-      <c r="U4" s="131"/>
-      <c r="V4" s="131"/>
-      <c r="W4" s="131"/>
-      <c r="X4" s="131"/>
-      <c r="Y4" s="132"/>
-      <c r="Z4" s="132"/>
-      <c r="AA4" s="131"/>
-      <c r="AB4" s="131"/>
-      <c r="AC4" s="131"/>
-      <c r="AD4" s="131"/>
-      <c r="AE4" s="132"/>
-      <c r="AF4" s="132"/>
-      <c r="AG4" s="131"/>
-      <c r="AH4" s="131"/>
-      <c r="AI4" s="133"/>
-      <c r="AJ4" s="209">
+      <c r="D4" s="126"/>
+      <c r="E4" s="127"/>
+      <c r="F4" s="127"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="127"/>
+      <c r="M4" s="128"/>
+      <c r="N4" s="128"/>
+      <c r="O4" s="127"/>
+      <c r="P4" s="127"/>
+      <c r="Q4" s="127"/>
+      <c r="R4" s="127"/>
+      <c r="S4" s="128"/>
+      <c r="T4" s="128"/>
+      <c r="U4" s="127"/>
+      <c r="V4" s="127"/>
+      <c r="W4" s="127"/>
+      <c r="X4" s="127"/>
+      <c r="Y4" s="128"/>
+      <c r="Z4" s="128"/>
+      <c r="AA4" s="127"/>
+      <c r="AB4" s="127"/>
+      <c r="AC4" s="127"/>
+      <c r="AD4" s="127"/>
+      <c r="AE4" s="128"/>
+      <c r="AF4" s="128"/>
+      <c r="AG4" s="127"/>
+      <c r="AH4" s="127"/>
+      <c r="AI4" s="129"/>
+      <c r="AJ4" s="194">
         <v>1</v>
       </c>
-      <c r="AO4" s="116" t="str">
-        <f t="shared" ref="AO4:AO26" si="1">DEC2HEX(AJ4*2+44,2)</f>
+      <c r="AO4" s="112" t="str">
+        <f t="shared" ref="AO4:AO26" si="2">DEC2HEX(AJ4*2+44,2)</f>
         <v>2E</v>
       </c>
-      <c r="AP4" s="191">
+      <c r="AP4" s="177">
         <v>-1</v>
       </c>
-      <c r="AQ4" s="192">
+      <c r="AQ4" s="178">
         <v>-1</v>
       </c>
-      <c r="AR4" s="182">
+      <c r="AR4" s="171">
         <v>-1</v>
       </c>
-      <c r="AS4" s="182">
+      <c r="AS4" s="171">
         <v>-1</v>
       </c>
-      <c r="AT4" s="114">
+      <c r="AT4" s="111">
         <v>-1</v>
       </c>
     </row>
     <row r="5" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="117">
-        <f>B4+1</f>
+      <c r="B5" s="113">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="C5" s="108" t="s">
+      <c r="C5" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="123"/>
-      <c r="E5" s="124"/>
-      <c r="F5" s="124"/>
-      <c r="G5" s="134"/>
-      <c r="H5" s="137"/>
-      <c r="I5" s="124"/>
-      <c r="J5" s="124"/>
-      <c r="K5" s="124"/>
-      <c r="L5" s="124"/>
-      <c r="M5" s="134"/>
-      <c r="N5" s="137"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="124"/>
-      <c r="Q5" s="124"/>
-      <c r="R5" s="124"/>
-      <c r="S5" s="134"/>
-      <c r="T5" s="137"/>
-      <c r="U5" s="124"/>
-      <c r="V5" s="124"/>
-      <c r="W5" s="124"/>
-      <c r="X5" s="124"/>
-      <c r="Y5" s="134"/>
-      <c r="Z5" s="137"/>
-      <c r="AA5" s="124"/>
-      <c r="AB5" s="124"/>
-      <c r="AC5" s="124"/>
-      <c r="AD5" s="124"/>
-      <c r="AE5" s="134"/>
-      <c r="AF5" s="137"/>
-      <c r="AG5" s="124"/>
-      <c r="AH5" s="124"/>
-      <c r="AI5" s="125"/>
-      <c r="AJ5" s="210">
+      <c r="D5" s="119"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="120"/>
+      <c r="J5" s="120"/>
+      <c r="K5" s="120"/>
+      <c r="L5" s="120"/>
+      <c r="M5" s="130"/>
+      <c r="N5" s="133"/>
+      <c r="O5" s="120"/>
+      <c r="P5" s="120"/>
+      <c r="Q5" s="120"/>
+      <c r="R5" s="120"/>
+      <c r="S5" s="130"/>
+      <c r="T5" s="133"/>
+      <c r="U5" s="120"/>
+      <c r="V5" s="120"/>
+      <c r="W5" s="120"/>
+      <c r="X5" s="120"/>
+      <c r="Y5" s="130"/>
+      <c r="Z5" s="133"/>
+      <c r="AA5" s="120"/>
+      <c r="AB5" s="120"/>
+      <c r="AC5" s="120"/>
+      <c r="AD5" s="120"/>
+      <c r="AE5" s="130"/>
+      <c r="AF5" s="133"/>
+      <c r="AG5" s="120"/>
+      <c r="AH5" s="120"/>
+      <c r="AI5" s="121"/>
+      <c r="AJ5" s="194">
         <v>2</v>
       </c>
-      <c r="AO5" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO5" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="AP5" s="191">
+      <c r="AP5" s="177">
         <v>-1</v>
       </c>
-      <c r="AQ5" s="192">
+      <c r="AQ5" s="178">
         <v>-1</v>
       </c>
-      <c r="AR5" s="182">
+      <c r="AR5" s="171">
         <v>-1</v>
       </c>
-      <c r="AS5" s="182">
+      <c r="AS5" s="171">
         <v>-1</v>
       </c>
-      <c r="AT5" s="114">
+      <c r="AT5" s="111">
         <v>-1</v>
       </c>
     </row>
     <row r="6" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="118">
-        <f>B5+1</f>
+      <c r="B6" s="114">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C6" s="119" t="s">
+      <c r="C6" s="115" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="127"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="138"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="128"/>
-      <c r="L6" s="128"/>
-      <c r="M6" s="136"/>
-      <c r="N6" s="138"/>
-      <c r="O6" s="128"/>
-      <c r="P6" s="128"/>
-      <c r="Q6" s="128"/>
-      <c r="R6" s="128"/>
-      <c r="S6" s="136"/>
-      <c r="T6" s="138"/>
-      <c r="U6" s="128"/>
-      <c r="V6" s="128"/>
-      <c r="W6" s="128"/>
-      <c r="X6" s="128"/>
-      <c r="Y6" s="136"/>
-      <c r="Z6" s="138"/>
-      <c r="AA6" s="128"/>
-      <c r="AB6" s="128"/>
-      <c r="AC6" s="128"/>
-      <c r="AD6" s="128"/>
-      <c r="AE6" s="136"/>
-      <c r="AF6" s="138"/>
-      <c r="AG6" s="128"/>
-      <c r="AH6" s="128"/>
-      <c r="AI6" s="129"/>
-      <c r="AJ6" s="211">
+      <c r="D6" s="123"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="124"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="134"/>
+      <c r="O6" s="124"/>
+      <c r="P6" s="124"/>
+      <c r="Q6" s="124"/>
+      <c r="R6" s="124"/>
+      <c r="S6" s="132"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="124"/>
+      <c r="V6" s="124"/>
+      <c r="W6" s="124"/>
+      <c r="X6" s="124"/>
+      <c r="Y6" s="132"/>
+      <c r="Z6" s="134"/>
+      <c r="AA6" s="124"/>
+      <c r="AB6" s="124"/>
+      <c r="AC6" s="124"/>
+      <c r="AD6" s="124"/>
+      <c r="AE6" s="132"/>
+      <c r="AF6" s="134"/>
+      <c r="AG6" s="124"/>
+      <c r="AH6" s="124"/>
+      <c r="AI6" s="125"/>
+      <c r="AJ6" s="195">
         <v>3</v>
       </c>
-      <c r="AO6" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO6" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="AP6" s="191">
+      <c r="AP6" s="177">
         <v>-1</v>
       </c>
-      <c r="AQ6" s="192">
+      <c r="AQ6" s="178">
         <v>-1</v>
       </c>
-      <c r="AR6" s="182">
+      <c r="AR6" s="171">
         <v>-1</v>
       </c>
-      <c r="AS6" s="182">
+      <c r="AS6" s="171">
         <v>-1</v>
       </c>
-      <c r="AT6" s="114">
+      <c r="AT6" s="111">
         <v>-1</v>
       </c>
     </row>
     <row r="7" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="120">
-        <f>B6+1</f>
+      <c r="B7" s="116">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C7" s="121" t="s">
+      <c r="C7" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="136"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="126"/>
-      <c r="G7" s="126"/>
-      <c r="H7" s="126"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="126"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="126"/>
-      <c r="N7" s="126"/>
-      <c r="O7" s="126"/>
-      <c r="P7" s="126"/>
-      <c r="Q7" s="126"/>
-      <c r="R7" s="126"/>
-      <c r="S7" s="126"/>
-      <c r="T7" s="126"/>
-      <c r="U7" s="126"/>
-      <c r="V7" s="126"/>
-      <c r="W7" s="126"/>
-      <c r="X7" s="126"/>
-      <c r="Y7" s="126"/>
-      <c r="Z7" s="126"/>
-      <c r="AA7" s="126"/>
-      <c r="AB7" s="126"/>
-      <c r="AC7" s="126"/>
-      <c r="AD7" s="126"/>
-      <c r="AE7" s="126"/>
-      <c r="AF7" s="126"/>
-      <c r="AG7" s="126"/>
-      <c r="AH7" s="126"/>
-      <c r="AI7" s="126"/>
-      <c r="AJ7" s="134">
+      <c r="D7" s="132"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="122"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="122"/>
+      <c r="K7" s="122"/>
+      <c r="L7" s="122"/>
+      <c r="M7" s="122"/>
+      <c r="N7" s="122"/>
+      <c r="O7" s="122"/>
+      <c r="P7" s="122"/>
+      <c r="Q7" s="122"/>
+      <c r="R7" s="122"/>
+      <c r="S7" s="122"/>
+      <c r="T7" s="122"/>
+      <c r="U7" s="122"/>
+      <c r="V7" s="122"/>
+      <c r="W7" s="122"/>
+      <c r="X7" s="122"/>
+      <c r="Y7" s="122"/>
+      <c r="Z7" s="122"/>
+      <c r="AA7" s="122"/>
+      <c r="AB7" s="122"/>
+      <c r="AC7" s="122"/>
+      <c r="AD7" s="122"/>
+      <c r="AE7" s="122"/>
+      <c r="AF7" s="122"/>
+      <c r="AG7" s="122"/>
+      <c r="AH7" s="122"/>
+      <c r="AI7" s="122"/>
+      <c r="AJ7" s="130">
         <v>4</v>
       </c>
-      <c r="AK7" s="135">
+      <c r="AK7" s="131">
         <v>5</v>
       </c>
-      <c r="AL7" s="135">
+      <c r="AL7" s="131">
         <v>6</v>
       </c>
-      <c r="AM7" s="137">
+      <c r="AM7" s="133">
         <v>7</v>
       </c>
-      <c r="AO7" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO7" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="AP7" s="114">
+      <c r="AP7" s="111">
         <v>0</v>
       </c>
-      <c r="AQ7" s="116">
+      <c r="AQ7" s="112">
         <v>3</v>
       </c>
       <c r="AR7" s="9">
@@ -8068,70 +7977,70 @@
       <c r="AS7" s="9">
         <v>64</v>
       </c>
-      <c r="AT7" s="114">
+      <c r="AT7" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="122">
-        <f>B7+1</f>
+      <c r="B8" s="118">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C8" s="119" t="s">
+      <c r="C8" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="136"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="126"/>
-      <c r="G8" s="126"/>
-      <c r="H8" s="126"/>
-      <c r="I8" s="126"/>
-      <c r="J8" s="126"/>
-      <c r="K8" s="126"/>
-      <c r="L8" s="126"/>
-      <c r="M8" s="126"/>
-      <c r="N8" s="126"/>
-      <c r="O8" s="126"/>
-      <c r="P8" s="126"/>
-      <c r="Q8" s="126"/>
-      <c r="R8" s="126"/>
-      <c r="S8" s="126"/>
-      <c r="T8" s="126"/>
-      <c r="U8" s="126"/>
-      <c r="V8" s="126"/>
-      <c r="W8" s="126"/>
-      <c r="X8" s="126"/>
-      <c r="Y8" s="126"/>
-      <c r="Z8" s="126"/>
-      <c r="AA8" s="126"/>
-      <c r="AB8" s="126"/>
-      <c r="AC8" s="126"/>
-      <c r="AD8" s="126"/>
-      <c r="AE8" s="126"/>
-      <c r="AF8" s="126"/>
-      <c r="AG8" s="126"/>
-      <c r="AH8" s="126"/>
-      <c r="AI8" s="126"/>
-      <c r="AJ8" s="151">
+      <c r="D8" s="132"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="122"/>
+      <c r="H8" s="122"/>
+      <c r="I8" s="122"/>
+      <c r="J8" s="122"/>
+      <c r="K8" s="122"/>
+      <c r="L8" s="122"/>
+      <c r="M8" s="122"/>
+      <c r="N8" s="122"/>
+      <c r="O8" s="122"/>
+      <c r="P8" s="122"/>
+      <c r="Q8" s="122"/>
+      <c r="R8" s="122"/>
+      <c r="S8" s="122"/>
+      <c r="T8" s="122"/>
+      <c r="U8" s="122"/>
+      <c r="V8" s="122"/>
+      <c r="W8" s="122"/>
+      <c r="X8" s="122"/>
+      <c r="Y8" s="122"/>
+      <c r="Z8" s="122"/>
+      <c r="AA8" s="122"/>
+      <c r="AB8" s="122"/>
+      <c r="AC8" s="122"/>
+      <c r="AD8" s="122"/>
+      <c r="AE8" s="122"/>
+      <c r="AF8" s="122"/>
+      <c r="AG8" s="122"/>
+      <c r="AH8" s="122"/>
+      <c r="AI8" s="122"/>
+      <c r="AJ8" s="147">
         <v>8</v>
       </c>
-      <c r="AK8" s="152">
+      <c r="AK8" s="148">
         <v>9</v>
       </c>
-      <c r="AL8" s="152">
+      <c r="AL8" s="148">
         <v>10</v>
       </c>
-      <c r="AM8" s="153">
+      <c r="AM8" s="149">
         <v>11</v>
       </c>
-      <c r="AO8" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO8" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>3C</v>
       </c>
-      <c r="AP8" s="114">
+      <c r="AP8" s="111">
         <v>0</v>
       </c>
-      <c r="AQ8" s="116">
+      <c r="AQ8" s="112">
         <v>3</v>
       </c>
       <c r="AR8" s="9">
@@ -8140,70 +8049,70 @@
       <c r="AS8" s="9">
         <v>64</v>
       </c>
-      <c r="AT8" s="114">
+      <c r="AT8" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="120">
-        <f>B8+1</f>
+      <c r="B9" s="116">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C9" s="121" t="s">
+      <c r="C9" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="136"/>
-      <c r="E9" s="126"/>
-      <c r="F9" s="126"/>
-      <c r="G9" s="126"/>
-      <c r="H9" s="126"/>
-      <c r="I9" s="126"/>
-      <c r="J9" s="126"/>
-      <c r="K9" s="126"/>
-      <c r="L9" s="126"/>
-      <c r="M9" s="126"/>
-      <c r="N9" s="126"/>
-      <c r="O9" s="126"/>
-      <c r="P9" s="126"/>
-      <c r="Q9" s="126"/>
-      <c r="R9" s="126"/>
-      <c r="S9" s="126"/>
-      <c r="T9" s="126"/>
-      <c r="U9" s="126"/>
-      <c r="V9" s="126"/>
-      <c r="W9" s="126"/>
-      <c r="X9" s="126"/>
-      <c r="Y9" s="126"/>
-      <c r="Z9" s="126"/>
-      <c r="AA9" s="126"/>
-      <c r="AB9" s="126"/>
-      <c r="AC9" s="126"/>
-      <c r="AD9" s="126"/>
-      <c r="AE9" s="126"/>
-      <c r="AF9" s="126"/>
-      <c r="AG9" s="126"/>
-      <c r="AH9" s="126"/>
-      <c r="AI9" s="126"/>
-      <c r="AJ9" s="134">
+      <c r="D9" s="132"/>
+      <c r="E9" s="122"/>
+      <c r="F9" s="122"/>
+      <c r="G9" s="122"/>
+      <c r="H9" s="122"/>
+      <c r="I9" s="122"/>
+      <c r="J9" s="122"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="122"/>
+      <c r="M9" s="122"/>
+      <c r="N9" s="122"/>
+      <c r="O9" s="122"/>
+      <c r="P9" s="122"/>
+      <c r="Q9" s="122"/>
+      <c r="R9" s="122"/>
+      <c r="S9" s="122"/>
+      <c r="T9" s="122"/>
+      <c r="U9" s="122"/>
+      <c r="V9" s="122"/>
+      <c r="W9" s="122"/>
+      <c r="X9" s="122"/>
+      <c r="Y9" s="122"/>
+      <c r="Z9" s="122"/>
+      <c r="AA9" s="122"/>
+      <c r="AB9" s="122"/>
+      <c r="AC9" s="122"/>
+      <c r="AD9" s="122"/>
+      <c r="AE9" s="122"/>
+      <c r="AF9" s="122"/>
+      <c r="AG9" s="122"/>
+      <c r="AH9" s="122"/>
+      <c r="AI9" s="122"/>
+      <c r="AJ9" s="130">
         <v>12</v>
       </c>
-      <c r="AK9" s="135">
+      <c r="AK9" s="131">
         <v>13</v>
       </c>
-      <c r="AL9" s="135">
+      <c r="AL9" s="131">
         <v>14</v>
       </c>
-      <c r="AM9" s="137">
+      <c r="AM9" s="133">
         <v>15</v>
       </c>
-      <c r="AO9" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO9" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="AP9" s="114">
+      <c r="AP9" s="111">
         <v>0</v>
       </c>
-      <c r="AQ9" s="116">
+      <c r="AQ9" s="112">
         <v>3</v>
       </c>
       <c r="AR9" s="9">
@@ -8212,70 +8121,70 @@
       <c r="AS9" s="9">
         <v>64</v>
       </c>
-      <c r="AT9" s="114">
+      <c r="AT9" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="122">
-        <f>B9+1</f>
+      <c r="B10" s="118">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C10" s="119" t="s">
+      <c r="C10" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="136"/>
-      <c r="E10" s="126"/>
-      <c r="F10" s="126"/>
-      <c r="G10" s="126"/>
-      <c r="H10" s="126"/>
-      <c r="I10" s="126"/>
-      <c r="J10" s="126"/>
-      <c r="K10" s="126"/>
-      <c r="L10" s="126"/>
-      <c r="M10" s="126"/>
-      <c r="N10" s="126"/>
-      <c r="O10" s="126"/>
-      <c r="P10" s="126"/>
-      <c r="Q10" s="126"/>
-      <c r="R10" s="126"/>
-      <c r="S10" s="126"/>
-      <c r="T10" s="126"/>
-      <c r="U10" s="126"/>
-      <c r="V10" s="126"/>
-      <c r="W10" s="126"/>
-      <c r="X10" s="126"/>
-      <c r="Y10" s="126"/>
-      <c r="Z10" s="126"/>
-      <c r="AA10" s="126"/>
-      <c r="AB10" s="126"/>
-      <c r="AC10" s="126"/>
-      <c r="AD10" s="126"/>
-      <c r="AE10" s="126"/>
-      <c r="AF10" s="126"/>
-      <c r="AG10" s="126"/>
-      <c r="AH10" s="126"/>
-      <c r="AI10" s="126"/>
-      <c r="AJ10" s="151">
+      <c r="D10" s="132"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="122"/>
+      <c r="I10" s="122"/>
+      <c r="J10" s="122"/>
+      <c r="K10" s="122"/>
+      <c r="L10" s="122"/>
+      <c r="M10" s="122"/>
+      <c r="N10" s="122"/>
+      <c r="O10" s="122"/>
+      <c r="P10" s="122"/>
+      <c r="Q10" s="122"/>
+      <c r="R10" s="122"/>
+      <c r="S10" s="122"/>
+      <c r="T10" s="122"/>
+      <c r="U10" s="122"/>
+      <c r="V10" s="122"/>
+      <c r="W10" s="122"/>
+      <c r="X10" s="122"/>
+      <c r="Y10" s="122"/>
+      <c r="Z10" s="122"/>
+      <c r="AA10" s="122"/>
+      <c r="AB10" s="122"/>
+      <c r="AC10" s="122"/>
+      <c r="AD10" s="122"/>
+      <c r="AE10" s="122"/>
+      <c r="AF10" s="122"/>
+      <c r="AG10" s="122"/>
+      <c r="AH10" s="122"/>
+      <c r="AI10" s="122"/>
+      <c r="AJ10" s="147">
         <v>16</v>
       </c>
-      <c r="AK10" s="152">
+      <c r="AK10" s="148">
         <v>17</v>
       </c>
-      <c r="AL10" s="152">
+      <c r="AL10" s="148">
         <v>18</v>
       </c>
-      <c r="AM10" s="153">
+      <c r="AM10" s="149">
         <v>19</v>
       </c>
-      <c r="AO10" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO10" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>4C</v>
       </c>
-      <c r="AP10" s="114">
+      <c r="AP10" s="111">
         <v>0</v>
       </c>
-      <c r="AQ10" s="116">
+      <c r="AQ10" s="112">
         <v>3</v>
       </c>
       <c r="AR10" s="9">
@@ -8284,70 +8193,70 @@
       <c r="AS10" s="9">
         <v>64</v>
       </c>
-      <c r="AT10" s="114">
+      <c r="AT10" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="120">
-        <f>B10+1</f>
+      <c r="B11" s="116">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C11" s="121" t="s">
+      <c r="C11" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="136"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="126"/>
-      <c r="G11" s="126"/>
-      <c r="H11" s="126"/>
-      <c r="I11" s="126"/>
-      <c r="J11" s="126"/>
-      <c r="K11" s="126"/>
-      <c r="L11" s="126"/>
-      <c r="M11" s="126"/>
-      <c r="N11" s="126"/>
-      <c r="O11" s="126"/>
-      <c r="P11" s="126"/>
-      <c r="Q11" s="126"/>
-      <c r="R11" s="126"/>
-      <c r="S11" s="126"/>
-      <c r="T11" s="126"/>
-      <c r="U11" s="126"/>
-      <c r="V11" s="126"/>
-      <c r="W11" s="126"/>
-      <c r="X11" s="126"/>
-      <c r="Y11" s="126"/>
-      <c r="Z11" s="126"/>
-      <c r="AA11" s="126"/>
-      <c r="AB11" s="126"/>
-      <c r="AC11" s="126"/>
-      <c r="AD11" s="126"/>
-      <c r="AE11" s="126"/>
-      <c r="AF11" s="126"/>
-      <c r="AG11" s="126"/>
-      <c r="AH11" s="126"/>
-      <c r="AI11" s="126"/>
-      <c r="AJ11" s="134">
+      <c r="D11" s="132"/>
+      <c r="E11" s="122"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="122"/>
+      <c r="H11" s="122"/>
+      <c r="I11" s="122"/>
+      <c r="J11" s="122"/>
+      <c r="K11" s="122"/>
+      <c r="L11" s="122"/>
+      <c r="M11" s="122"/>
+      <c r="N11" s="122"/>
+      <c r="O11" s="122"/>
+      <c r="P11" s="122"/>
+      <c r="Q11" s="122"/>
+      <c r="R11" s="122"/>
+      <c r="S11" s="122"/>
+      <c r="T11" s="122"/>
+      <c r="U11" s="122"/>
+      <c r="V11" s="122"/>
+      <c r="W11" s="122"/>
+      <c r="X11" s="122"/>
+      <c r="Y11" s="122"/>
+      <c r="Z11" s="122"/>
+      <c r="AA11" s="122"/>
+      <c r="AB11" s="122"/>
+      <c r="AC11" s="122"/>
+      <c r="AD11" s="122"/>
+      <c r="AE11" s="122"/>
+      <c r="AF11" s="122"/>
+      <c r="AG11" s="122"/>
+      <c r="AH11" s="122"/>
+      <c r="AI11" s="122"/>
+      <c r="AJ11" s="130">
         <v>4</v>
       </c>
-      <c r="AK11" s="135">
+      <c r="AK11" s="131">
         <v>5</v>
       </c>
-      <c r="AL11" s="135">
+      <c r="AL11" s="131">
         <v>6</v>
       </c>
-      <c r="AM11" s="137">
+      <c r="AM11" s="133">
         <v>7</v>
       </c>
-      <c r="AO11" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO11" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="AP11" s="114">
+      <c r="AP11" s="111">
         <v>0</v>
       </c>
-      <c r="AQ11" s="116">
+      <c r="AQ11" s="112">
         <v>3</v>
       </c>
       <c r="AR11" s="9">
@@ -8356,70 +8265,70 @@
       <c r="AS11" s="9">
         <v>64</v>
       </c>
-      <c r="AT11" s="114">
+      <c r="AT11" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="122">
-        <f>B11+1</f>
+      <c r="B12" s="118">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C12" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="136"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="126"/>
-      <c r="H12" s="126"/>
-      <c r="I12" s="126"/>
-      <c r="J12" s="126"/>
-      <c r="K12" s="126"/>
-      <c r="L12" s="126"/>
-      <c r="M12" s="126"/>
-      <c r="N12" s="126"/>
-      <c r="O12" s="126"/>
-      <c r="P12" s="126"/>
-      <c r="Q12" s="126"/>
-      <c r="R12" s="126"/>
-      <c r="S12" s="126"/>
-      <c r="T12" s="126"/>
-      <c r="U12" s="126"/>
-      <c r="V12" s="126"/>
-      <c r="W12" s="126"/>
-      <c r="X12" s="126"/>
-      <c r="Y12" s="126"/>
-      <c r="Z12" s="126"/>
-      <c r="AA12" s="126"/>
-      <c r="AB12" s="126"/>
-      <c r="AC12" s="126"/>
-      <c r="AD12" s="126"/>
-      <c r="AE12" s="126"/>
-      <c r="AF12" s="126"/>
-      <c r="AG12" s="126"/>
-      <c r="AH12" s="126"/>
-      <c r="AI12" s="126"/>
-      <c r="AJ12" s="151">
+      <c r="D12" s="132"/>
+      <c r="E12" s="122"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="122"/>
+      <c r="J12" s="122"/>
+      <c r="K12" s="122"/>
+      <c r="L12" s="122"/>
+      <c r="M12" s="122"/>
+      <c r="N12" s="122"/>
+      <c r="O12" s="122"/>
+      <c r="P12" s="122"/>
+      <c r="Q12" s="122"/>
+      <c r="R12" s="122"/>
+      <c r="S12" s="122"/>
+      <c r="T12" s="122"/>
+      <c r="U12" s="122"/>
+      <c r="V12" s="122"/>
+      <c r="W12" s="122"/>
+      <c r="X12" s="122"/>
+      <c r="Y12" s="122"/>
+      <c r="Z12" s="122"/>
+      <c r="AA12" s="122"/>
+      <c r="AB12" s="122"/>
+      <c r="AC12" s="122"/>
+      <c r="AD12" s="122"/>
+      <c r="AE12" s="122"/>
+      <c r="AF12" s="122"/>
+      <c r="AG12" s="122"/>
+      <c r="AH12" s="122"/>
+      <c r="AI12" s="122"/>
+      <c r="AJ12" s="147">
         <v>8</v>
       </c>
-      <c r="AK12" s="152">
+      <c r="AK12" s="148">
         <v>9</v>
       </c>
-      <c r="AL12" s="152">
+      <c r="AL12" s="148">
         <v>10</v>
       </c>
-      <c r="AM12" s="153">
+      <c r="AM12" s="149">
         <v>11</v>
       </c>
-      <c r="AO12" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO12" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>3C</v>
       </c>
-      <c r="AP12" s="114">
+      <c r="AP12" s="111">
         <v>0</v>
       </c>
-      <c r="AQ12" s="116">
+      <c r="AQ12" s="112">
         <v>3</v>
       </c>
       <c r="AR12" s="9">
@@ -8428,70 +8337,70 @@
       <c r="AS12" s="9">
         <v>64</v>
       </c>
-      <c r="AT12" s="114">
+      <c r="AT12" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="120">
-        <f>B12+1</f>
+      <c r="B13" s="116">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="C13" s="121" t="s">
+      <c r="C13" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="136"/>
-      <c r="E13" s="126"/>
-      <c r="F13" s="126"/>
-      <c r="G13" s="126"/>
-      <c r="H13" s="126"/>
-      <c r="I13" s="126"/>
-      <c r="J13" s="126"/>
-      <c r="K13" s="126"/>
-      <c r="L13" s="126"/>
-      <c r="M13" s="126"/>
-      <c r="N13" s="126"/>
-      <c r="O13" s="126"/>
-      <c r="P13" s="126"/>
-      <c r="Q13" s="126"/>
-      <c r="R13" s="126"/>
-      <c r="S13" s="126"/>
-      <c r="T13" s="126"/>
-      <c r="U13" s="126"/>
-      <c r="V13" s="126"/>
-      <c r="W13" s="126"/>
-      <c r="X13" s="126"/>
-      <c r="Y13" s="126"/>
-      <c r="Z13" s="126"/>
-      <c r="AA13" s="126"/>
-      <c r="AB13" s="126"/>
-      <c r="AC13" s="126"/>
-      <c r="AD13" s="126"/>
-      <c r="AE13" s="126"/>
-      <c r="AF13" s="126"/>
-      <c r="AG13" s="126"/>
-      <c r="AH13" s="126"/>
-      <c r="AI13" s="126"/>
-      <c r="AJ13" s="136">
+      <c r="D13" s="132"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="122"/>
+      <c r="I13" s="122"/>
+      <c r="J13" s="122"/>
+      <c r="K13" s="122"/>
+      <c r="L13" s="122"/>
+      <c r="M13" s="122"/>
+      <c r="N13" s="122"/>
+      <c r="O13" s="122"/>
+      <c r="P13" s="122"/>
+      <c r="Q13" s="122"/>
+      <c r="R13" s="122"/>
+      <c r="S13" s="122"/>
+      <c r="T13" s="122"/>
+      <c r="U13" s="122"/>
+      <c r="V13" s="122"/>
+      <c r="W13" s="122"/>
+      <c r="X13" s="122"/>
+      <c r="Y13" s="122"/>
+      <c r="Z13" s="122"/>
+      <c r="AA13" s="122"/>
+      <c r="AB13" s="122"/>
+      <c r="AC13" s="122"/>
+      <c r="AD13" s="122"/>
+      <c r="AE13" s="122"/>
+      <c r="AF13" s="122"/>
+      <c r="AG13" s="122"/>
+      <c r="AH13" s="122"/>
+      <c r="AI13" s="122"/>
+      <c r="AJ13" s="132">
         <v>12</v>
       </c>
-      <c r="AK13" s="126">
+      <c r="AK13" s="122">
         <v>13</v>
       </c>
-      <c r="AL13" s="126">
+      <c r="AL13" s="122">
         <v>14</v>
       </c>
-      <c r="AM13" s="138">
+      <c r="AM13" s="134">
         <v>15</v>
       </c>
-      <c r="AO13" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO13" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="AP13" s="114">
+      <c r="AP13" s="111">
         <v>0</v>
       </c>
-      <c r="AQ13" s="116">
+      <c r="AQ13" s="112">
         <v>3</v>
       </c>
       <c r="AR13" s="9">
@@ -8500,70 +8409,70 @@
       <c r="AS13" s="9">
         <v>64</v>
       </c>
-      <c r="AT13" s="114">
+      <c r="AT13" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="122">
-        <f>B13+1</f>
+      <c r="B14" s="118">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C14" s="119" t="s">
+      <c r="C14" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="136"/>
-      <c r="E14" s="126"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
-      <c r="H14" s="126"/>
-      <c r="I14" s="126"/>
-      <c r="J14" s="126"/>
-      <c r="K14" s="126"/>
-      <c r="L14" s="126"/>
-      <c r="M14" s="126"/>
-      <c r="N14" s="126"/>
-      <c r="O14" s="126"/>
-      <c r="P14" s="126"/>
-      <c r="Q14" s="126"/>
-      <c r="R14" s="126"/>
-      <c r="S14" s="126"/>
-      <c r="T14" s="126"/>
-      <c r="U14" s="126"/>
-      <c r="V14" s="126"/>
-      <c r="W14" s="126"/>
-      <c r="X14" s="126"/>
-      <c r="Y14" s="126"/>
-      <c r="Z14" s="126"/>
-      <c r="AA14" s="126"/>
-      <c r="AB14" s="126"/>
-      <c r="AC14" s="126"/>
-      <c r="AD14" s="126"/>
-      <c r="AE14" s="126"/>
-      <c r="AF14" s="126"/>
-      <c r="AG14" s="126"/>
-      <c r="AH14" s="126"/>
-      <c r="AI14" s="126"/>
-      <c r="AJ14" s="151">
+      <c r="D14" s="132"/>
+      <c r="E14" s="122"/>
+      <c r="F14" s="122"/>
+      <c r="G14" s="122"/>
+      <c r="H14" s="122"/>
+      <c r="I14" s="122"/>
+      <c r="J14" s="122"/>
+      <c r="K14" s="122"/>
+      <c r="L14" s="122"/>
+      <c r="M14" s="122"/>
+      <c r="N14" s="122"/>
+      <c r="O14" s="122"/>
+      <c r="P14" s="122"/>
+      <c r="Q14" s="122"/>
+      <c r="R14" s="122"/>
+      <c r="S14" s="122"/>
+      <c r="T14" s="122"/>
+      <c r="U14" s="122"/>
+      <c r="V14" s="122"/>
+      <c r="W14" s="122"/>
+      <c r="X14" s="122"/>
+      <c r="Y14" s="122"/>
+      <c r="Z14" s="122"/>
+      <c r="AA14" s="122"/>
+      <c r="AB14" s="122"/>
+      <c r="AC14" s="122"/>
+      <c r="AD14" s="122"/>
+      <c r="AE14" s="122"/>
+      <c r="AF14" s="122"/>
+      <c r="AG14" s="122"/>
+      <c r="AH14" s="122"/>
+      <c r="AI14" s="122"/>
+      <c r="AJ14" s="147">
         <v>16</v>
       </c>
-      <c r="AK14" s="152">
+      <c r="AK14" s="148">
         <v>17</v>
       </c>
-      <c r="AL14" s="152">
+      <c r="AL14" s="148">
         <v>18</v>
       </c>
-      <c r="AM14" s="153">
+      <c r="AM14" s="149">
         <v>19</v>
       </c>
-      <c r="AO14" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO14" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>4C</v>
       </c>
-      <c r="AP14" s="114">
+      <c r="AP14" s="111">
         <v>0</v>
       </c>
-      <c r="AQ14" s="116">
+      <c r="AQ14" s="112">
         <v>3</v>
       </c>
       <c r="AR14" s="9">
@@ -8572,196 +8481,196 @@
       <c r="AS14" s="9">
         <v>64</v>
       </c>
-      <c r="AT14" s="114">
+      <c r="AT14" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="120">
-        <f>B14+1</f>
+      <c r="B15" s="116">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="C15" s="121" t="s">
+      <c r="C15" s="117" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="148"/>
-      <c r="E15" s="149"/>
-      <c r="F15" s="149"/>
-      <c r="G15" s="149"/>
-      <c r="H15" s="149"/>
-      <c r="I15" s="149"/>
-      <c r="J15" s="149"/>
-      <c r="K15" s="149"/>
-      <c r="L15" s="149"/>
-      <c r="M15" s="149"/>
-      <c r="N15" s="149"/>
-      <c r="O15" s="149"/>
-      <c r="P15" s="149"/>
-      <c r="Q15" s="149"/>
-      <c r="R15" s="149"/>
-      <c r="S15" s="149"/>
-      <c r="T15" s="149"/>
-      <c r="U15" s="149"/>
-      <c r="V15" s="149"/>
-      <c r="W15" s="149"/>
-      <c r="X15" s="149"/>
-      <c r="Y15" s="149"/>
-      <c r="Z15" s="149"/>
-      <c r="AA15" s="149"/>
-      <c r="AB15" s="149"/>
-      <c r="AC15" s="149"/>
-      <c r="AD15" s="149"/>
-      <c r="AE15" s="149"/>
-      <c r="AF15" s="149"/>
-      <c r="AG15" s="149"/>
-      <c r="AH15" s="149"/>
-      <c r="AI15" s="150"/>
-      <c r="AJ15" s="208">
+      <c r="D15" s="144"/>
+      <c r="E15" s="145"/>
+      <c r="F15" s="145"/>
+      <c r="G15" s="145"/>
+      <c r="H15" s="145"/>
+      <c r="I15" s="145"/>
+      <c r="J15" s="145"/>
+      <c r="K15" s="145"/>
+      <c r="L15" s="145"/>
+      <c r="M15" s="145"/>
+      <c r="N15" s="145"/>
+      <c r="O15" s="145"/>
+      <c r="P15" s="145"/>
+      <c r="Q15" s="145"/>
+      <c r="R15" s="145"/>
+      <c r="S15" s="145"/>
+      <c r="T15" s="145"/>
+      <c r="U15" s="145"/>
+      <c r="V15" s="145"/>
+      <c r="W15" s="145"/>
+      <c r="X15" s="145"/>
+      <c r="Y15" s="145"/>
+      <c r="Z15" s="145"/>
+      <c r="AA15" s="145"/>
+      <c r="AB15" s="145"/>
+      <c r="AC15" s="145"/>
+      <c r="AD15" s="145"/>
+      <c r="AE15" s="145"/>
+      <c r="AF15" s="145"/>
+      <c r="AG15" s="145"/>
+      <c r="AH15" s="145"/>
+      <c r="AI15" s="146"/>
+      <c r="AJ15" s="193">
         <v>20</v>
       </c>
-      <c r="AO15" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO15" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="AP15" s="191">
+      <c r="AP15" s="177">
         <v>-1</v>
       </c>
-      <c r="AQ15" s="192">
+      <c r="AQ15" s="178">
         <v>-1</v>
       </c>
-      <c r="AR15" s="182">
+      <c r="AR15" s="171">
         <v>-1</v>
       </c>
-      <c r="AS15" s="182">
+      <c r="AS15" s="171">
         <v>-1</v>
       </c>
-      <c r="AT15" s="114">
+      <c r="AT15" s="111">
         <v>-1</v>
       </c>
     </row>
     <row r="16" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="122">
-        <f>B15+1</f>
+      <c r="B16" s="118">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="C16" s="119" t="s">
+      <c r="C16" s="115" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="139"/>
-      <c r="E16" s="140"/>
-      <c r="F16" s="140"/>
-      <c r="G16" s="140"/>
-      <c r="H16" s="140"/>
-      <c r="I16" s="140"/>
-      <c r="J16" s="140"/>
-      <c r="K16" s="140"/>
-      <c r="L16" s="140"/>
-      <c r="M16" s="140"/>
-      <c r="N16" s="140"/>
-      <c r="O16" s="140"/>
-      <c r="P16" s="140"/>
-      <c r="Q16" s="140"/>
-      <c r="R16" s="140"/>
-      <c r="S16" s="140"/>
-      <c r="T16" s="140"/>
-      <c r="U16" s="140"/>
-      <c r="V16" s="140"/>
-      <c r="W16" s="140"/>
-      <c r="X16" s="140"/>
-      <c r="Y16" s="140"/>
-      <c r="Z16" s="140"/>
-      <c r="AA16" s="140"/>
-      <c r="AB16" s="140"/>
-      <c r="AC16" s="140"/>
-      <c r="AD16" s="140"/>
-      <c r="AE16" s="140"/>
-      <c r="AF16" s="140"/>
-      <c r="AG16" s="140"/>
-      <c r="AH16" s="140"/>
-      <c r="AI16" s="141"/>
-      <c r="AJ16" s="211">
+      <c r="D16" s="135"/>
+      <c r="E16" s="136"/>
+      <c r="F16" s="136"/>
+      <c r="G16" s="136"/>
+      <c r="H16" s="136"/>
+      <c r="I16" s="136"/>
+      <c r="J16" s="136"/>
+      <c r="K16" s="136"/>
+      <c r="L16" s="136"/>
+      <c r="M16" s="136"/>
+      <c r="N16" s="136"/>
+      <c r="O16" s="136"/>
+      <c r="P16" s="136"/>
+      <c r="Q16" s="136"/>
+      <c r="R16" s="136"/>
+      <c r="S16" s="136"/>
+      <c r="T16" s="136"/>
+      <c r="U16" s="136"/>
+      <c r="V16" s="136"/>
+      <c r="W16" s="136"/>
+      <c r="X16" s="136"/>
+      <c r="Y16" s="136"/>
+      <c r="Z16" s="136"/>
+      <c r="AA16" s="136"/>
+      <c r="AB16" s="136"/>
+      <c r="AC16" s="136"/>
+      <c r="AD16" s="136"/>
+      <c r="AE16" s="136"/>
+      <c r="AF16" s="136"/>
+      <c r="AG16" s="136"/>
+      <c r="AH16" s="136"/>
+      <c r="AI16" s="137"/>
+      <c r="AJ16" s="195">
         <v>21</v>
       </c>
-      <c r="AO16" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO16" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
-      <c r="AP16" s="191">
+      <c r="AP16" s="177">
         <v>-1</v>
       </c>
-      <c r="AQ16" s="192">
+      <c r="AQ16" s="178">
         <v>-1</v>
       </c>
-      <c r="AR16" s="182">
+      <c r="AR16" s="171">
         <v>-1</v>
       </c>
-      <c r="AS16" s="182">
+      <c r="AS16" s="171">
         <v>-1</v>
       </c>
-      <c r="AT16" s="114">
+      <c r="AT16" s="111">
         <v>-1</v>
       </c>
     </row>
     <row r="17" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="120">
-        <f>B16+1</f>
+      <c r="B17" s="116">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="C17" s="121" t="s">
+      <c r="C17" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="144"/>
-      <c r="E17" s="145"/>
-      <c r="F17" s="145"/>
-      <c r="G17" s="145"/>
-      <c r="H17" s="145"/>
-      <c r="I17" s="145"/>
-      <c r="J17" s="145"/>
-      <c r="K17" s="145"/>
-      <c r="L17" s="145"/>
-      <c r="M17" s="145"/>
-      <c r="N17" s="145"/>
-      <c r="O17" s="145"/>
-      <c r="P17" s="145"/>
-      <c r="Q17" s="145"/>
-      <c r="R17" s="145"/>
-      <c r="S17" s="145"/>
-      <c r="T17" s="145"/>
-      <c r="U17" s="145"/>
-      <c r="V17" s="145"/>
-      <c r="W17" s="145"/>
-      <c r="X17" s="145"/>
-      <c r="Y17" s="145"/>
-      <c r="Z17" s="145"/>
-      <c r="AA17" s="145"/>
-      <c r="AB17" s="145"/>
-      <c r="AC17" s="145"/>
-      <c r="AD17" s="145"/>
-      <c r="AE17" s="145"/>
-      <c r="AF17" s="145"/>
-      <c r="AG17" s="145"/>
-      <c r="AH17" s="145"/>
-      <c r="AI17" s="145"/>
-      <c r="AJ17" s="195">
+      <c r="D17" s="140"/>
+      <c r="E17" s="141"/>
+      <c r="F17" s="141"/>
+      <c r="G17" s="141"/>
+      <c r="H17" s="141"/>
+      <c r="I17" s="141"/>
+      <c r="J17" s="141"/>
+      <c r="K17" s="141"/>
+      <c r="L17" s="141"/>
+      <c r="M17" s="141"/>
+      <c r="N17" s="141"/>
+      <c r="O17" s="141"/>
+      <c r="P17" s="141"/>
+      <c r="Q17" s="141"/>
+      <c r="R17" s="141"/>
+      <c r="S17" s="141"/>
+      <c r="T17" s="141"/>
+      <c r="U17" s="141"/>
+      <c r="V17" s="141"/>
+      <c r="W17" s="141"/>
+      <c r="X17" s="141"/>
+      <c r="Y17" s="141"/>
+      <c r="Z17" s="141"/>
+      <c r="AA17" s="141"/>
+      <c r="AB17" s="141"/>
+      <c r="AC17" s="141"/>
+      <c r="AD17" s="141"/>
+      <c r="AE17" s="141"/>
+      <c r="AF17" s="141"/>
+      <c r="AG17" s="141"/>
+      <c r="AH17" s="141"/>
+      <c r="AI17" s="141"/>
+      <c r="AJ17" s="180">
         <v>22</v>
       </c>
-      <c r="AK17" s="196">
+      <c r="AK17" s="181">
         <v>23</v>
       </c>
-      <c r="AL17" s="196">
+      <c r="AL17" s="181">
         <v>24</v>
       </c>
-      <c r="AM17" s="197">
+      <c r="AM17" s="182">
         <v>25</v>
       </c>
-      <c r="AO17" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO17" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
-      <c r="AP17" s="114">
+      <c r="AP17" s="111">
         <v>0</v>
       </c>
-      <c r="AQ17" s="116">
+      <c r="AQ17" s="112">
         <v>3</v>
       </c>
       <c r="AR17" s="9">
@@ -8770,74 +8679,74 @@
       <c r="AS17" s="9">
         <v>64</v>
       </c>
-      <c r="AT17" s="114">
+      <c r="AT17" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="122">
-        <f>B17+1</f>
+      <c r="B18" s="118">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="C18" s="119" t="s">
+      <c r="C18" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="142"/>
-      <c r="E18" s="143"/>
-      <c r="F18" s="143"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="143"/>
-      <c r="I18" s="143"/>
-      <c r="J18" s="143"/>
-      <c r="K18" s="143"/>
-      <c r="L18" s="143"/>
-      <c r="M18" s="143"/>
-      <c r="N18" s="143"/>
-      <c r="O18" s="143"/>
-      <c r="P18" s="143"/>
-      <c r="Q18" s="143"/>
-      <c r="R18" s="143"/>
-      <c r="S18" s="143"/>
-      <c r="T18" s="143"/>
-      <c r="U18" s="143"/>
-      <c r="V18" s="143"/>
-      <c r="W18" s="143"/>
-      <c r="X18" s="143"/>
-      <c r="Y18" s="143"/>
-      <c r="Z18" s="143"/>
-      <c r="AA18" s="143"/>
-      <c r="AB18" s="143"/>
-      <c r="AC18" s="143"/>
-      <c r="AD18" s="143"/>
-      <c r="AE18" s="143"/>
-      <c r="AF18" s="143"/>
-      <c r="AG18" s="143"/>
-      <c r="AH18" s="143"/>
-      <c r="AI18" s="143"/>
-      <c r="AJ18" s="200">
+      <c r="D18" s="138"/>
+      <c r="E18" s="139"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="139"/>
+      <c r="H18" s="139"/>
+      <c r="I18" s="139"/>
+      <c r="J18" s="139"/>
+      <c r="K18" s="139"/>
+      <c r="L18" s="139"/>
+      <c r="M18" s="139"/>
+      <c r="N18" s="139"/>
+      <c r="O18" s="139"/>
+      <c r="P18" s="139"/>
+      <c r="Q18" s="139"/>
+      <c r="R18" s="139"/>
+      <c r="S18" s="139"/>
+      <c r="T18" s="139"/>
+      <c r="U18" s="139"/>
+      <c r="V18" s="139"/>
+      <c r="W18" s="139"/>
+      <c r="X18" s="139"/>
+      <c r="Y18" s="139"/>
+      <c r="Z18" s="139"/>
+      <c r="AA18" s="139"/>
+      <c r="AB18" s="139"/>
+      <c r="AC18" s="139"/>
+      <c r="AD18" s="139"/>
+      <c r="AE18" s="139"/>
+      <c r="AF18" s="139"/>
+      <c r="AG18" s="139"/>
+      <c r="AH18" s="139"/>
+      <c r="AI18" s="139"/>
+      <c r="AJ18" s="185">
         <f>AJ17+4</f>
         <v>26</v>
       </c>
-      <c r="AK18" s="201">
+      <c r="AK18" s="186">
         <f>AK17+4</f>
         <v>27</v>
       </c>
-      <c r="AL18" s="201">
+      <c r="AL18" s="186">
         <f>AL17+4</f>
         <v>28</v>
       </c>
-      <c r="AM18" s="199">
+      <c r="AM18" s="184">
         <f>AM17+4</f>
         <v>29</v>
       </c>
-      <c r="AO18" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO18" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="AP18" s="114">
+      <c r="AP18" s="111">
         <v>0</v>
       </c>
-      <c r="AQ18" s="116">
+      <c r="AQ18" s="112">
         <v>3</v>
       </c>
       <c r="AR18" s="9">
@@ -8846,69 +8755,68 @@
       <c r="AS18" s="9">
         <v>64</v>
       </c>
-      <c r="AT18" s="114">
+      <c r="AT18" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="120">
-        <f>B18+1</f>
+      <c r="B19" s="116">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="C19" s="121" t="s">
+      <c r="C19" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="142"/>
-      <c r="E19" s="143"/>
-      <c r="F19" s="143"/>
-      <c r="G19" s="143"/>
-      <c r="H19" s="143"/>
-      <c r="I19" s="143"/>
-      <c r="J19" s="143"/>
-      <c r="K19" s="143"/>
-      <c r="L19" s="143"/>
-      <c r="M19" s="143"/>
-      <c r="N19" s="143"/>
-      <c r="O19" s="143"/>
-      <c r="P19" s="143"/>
-      <c r="Q19" s="143"/>
-      <c r="R19" s="143"/>
-      <c r="S19" s="143"/>
-      <c r="T19" s="143"/>
-      <c r="U19" s="143"/>
-      <c r="V19" s="143"/>
-      <c r="W19" s="143"/>
-      <c r="X19" s="143"/>
-      <c r="Y19" s="143"/>
-      <c r="Z19" s="143"/>
-      <c r="AA19" s="143"/>
-      <c r="AB19" s="143"/>
-      <c r="AC19" s="143"/>
-      <c r="AD19" s="143"/>
-      <c r="AE19" s="143"/>
-      <c r="AF19" s="143"/>
-      <c r="AG19" s="143"/>
-      <c r="AH19" s="143"/>
-      <c r="AI19" s="143"/>
-      <c r="AJ19" s="195">
+      <c r="D19" s="138"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="139"/>
+      <c r="G19" s="139"/>
+      <c r="H19" s="139"/>
+      <c r="I19" s="139"/>
+      <c r="J19" s="139"/>
+      <c r="K19" s="139"/>
+      <c r="L19" s="139"/>
+      <c r="M19" s="139"/>
+      <c r="N19" s="139"/>
+      <c r="O19" s="139"/>
+      <c r="P19" s="139"/>
+      <c r="Q19" s="139"/>
+      <c r="R19" s="139"/>
+      <c r="S19" s="139"/>
+      <c r="T19" s="139"/>
+      <c r="U19" s="139"/>
+      <c r="V19" s="139"/>
+      <c r="W19" s="139"/>
+      <c r="X19" s="139"/>
+      <c r="Y19" s="139"/>
+      <c r="Z19" s="139"/>
+      <c r="AA19" s="139"/>
+      <c r="AB19" s="139"/>
+      <c r="AC19" s="139"/>
+      <c r="AD19" s="139"/>
+      <c r="AE19" s="139"/>
+      <c r="AF19" s="139"/>
+      <c r="AG19" s="139"/>
+      <c r="AH19" s="139"/>
+      <c r="AI19" s="139"/>
+      <c r="AJ19" s="180">
         <f>AJ18+4</f>
         <v>30</v>
       </c>
-      <c r="AK19" s="197">
+      <c r="AK19" s="182">
         <f>AK18+4</f>
         <v>31</v>
       </c>
-      <c r="AL19" s="212"/>
-      <c r="AM19" s="214"/>
-      <c r="AN19" s="115"/>
-      <c r="AO19" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AL19" s="196"/>
+      <c r="AM19" s="198"/>
+      <c r="AO19" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="AP19" s="114">
+      <c r="AP19" s="111">
         <v>0</v>
       </c>
-      <c r="AQ19" s="116">
+      <c r="AQ19" s="112">
         <v>1</v>
       </c>
       <c r="AR19" s="9">
@@ -8917,69 +8825,68 @@
       <c r="AS19" s="9">
         <v>64</v>
       </c>
-      <c r="AT19" s="114">
+      <c r="AT19" s="111">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="122">
-        <f>B19+1</f>
+      <c r="B20" s="118">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="C20" s="119" t="s">
+      <c r="C20" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="142"/>
-      <c r="E20" s="143"/>
-      <c r="F20" s="143"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="143"/>
-      <c r="I20" s="143"/>
-      <c r="J20" s="143"/>
-      <c r="K20" s="143"/>
-      <c r="L20" s="143"/>
-      <c r="M20" s="143"/>
-      <c r="N20" s="143"/>
-      <c r="O20" s="143"/>
-      <c r="P20" s="143"/>
-      <c r="Q20" s="143"/>
-      <c r="R20" s="143"/>
-      <c r="S20" s="143"/>
-      <c r="T20" s="143"/>
-      <c r="U20" s="143"/>
-      <c r="V20" s="143"/>
-      <c r="W20" s="143"/>
-      <c r="X20" s="143"/>
-      <c r="Y20" s="143"/>
-      <c r="Z20" s="143"/>
-      <c r="AA20" s="143"/>
-      <c r="AB20" s="143"/>
-      <c r="AC20" s="143"/>
-      <c r="AD20" s="143"/>
-      <c r="AE20" s="143"/>
-      <c r="AF20" s="143"/>
-      <c r="AG20" s="143"/>
-      <c r="AH20" s="143"/>
-      <c r="AI20" s="143"/>
-      <c r="AJ20" s="200">
-        <f>AJ19+2</f>
+      <c r="D20" s="138"/>
+      <c r="E20" s="139"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="139"/>
+      <c r="H20" s="139"/>
+      <c r="I20" s="139"/>
+      <c r="J20" s="139"/>
+      <c r="K20" s="139"/>
+      <c r="L20" s="139"/>
+      <c r="M20" s="139"/>
+      <c r="N20" s="139"/>
+      <c r="O20" s="139"/>
+      <c r="P20" s="139"/>
+      <c r="Q20" s="139"/>
+      <c r="R20" s="139"/>
+      <c r="S20" s="139"/>
+      <c r="T20" s="139"/>
+      <c r="U20" s="139"/>
+      <c r="V20" s="139"/>
+      <c r="W20" s="139"/>
+      <c r="X20" s="139"/>
+      <c r="Y20" s="139"/>
+      <c r="Z20" s="139"/>
+      <c r="AA20" s="139"/>
+      <c r="AB20" s="139"/>
+      <c r="AC20" s="139"/>
+      <c r="AD20" s="139"/>
+      <c r="AE20" s="139"/>
+      <c r="AF20" s="139"/>
+      <c r="AG20" s="139"/>
+      <c r="AH20" s="139"/>
+      <c r="AI20" s="139"/>
+      <c r="AJ20" s="185">
+        <f t="shared" ref="AJ20:AK22" si="3">AJ19+2</f>
         <v>32</v>
       </c>
-      <c r="AK20" s="202">
-        <f>AK19+2</f>
+      <c r="AK20" s="187">
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="AL20" s="212"/>
-      <c r="AM20" s="212"/>
-      <c r="AN20" s="115"/>
-      <c r="AO20" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AL20" s="196"/>
+      <c r="AM20" s="196"/>
+      <c r="AO20" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>6C</v>
       </c>
-      <c r="AP20" s="114">
+      <c r="AP20" s="111">
         <v>0</v>
       </c>
-      <c r="AQ20" s="116">
+      <c r="AQ20" s="112">
         <v>1</v>
       </c>
       <c r="AR20" s="9">
@@ -8988,69 +8895,66 @@
       <c r="AS20" s="9">
         <v>64</v>
       </c>
-      <c r="AT20" s="114">
+      <c r="AT20" s="111">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="120">
-        <f>B20+1</f>
+      <c r="B21" s="116">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="C21" s="121" t="s">
+      <c r="C21" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="142"/>
-      <c r="E21" s="143"/>
-      <c r="F21" s="143"/>
-      <c r="G21" s="143"/>
-      <c r="H21" s="143"/>
-      <c r="I21" s="143"/>
-      <c r="J21" s="143"/>
-      <c r="K21" s="143"/>
-      <c r="L21" s="143"/>
-      <c r="M21" s="143"/>
-      <c r="N21" s="143"/>
-      <c r="O21" s="143"/>
-      <c r="P21" s="143"/>
-      <c r="Q21" s="143"/>
-      <c r="R21" s="143"/>
-      <c r="S21" s="143"/>
-      <c r="T21" s="143"/>
-      <c r="U21" s="143"/>
-      <c r="V21" s="143"/>
-      <c r="W21" s="143"/>
-      <c r="X21" s="143"/>
-      <c r="Y21" s="143"/>
-      <c r="Z21" s="143"/>
-      <c r="AA21" s="143"/>
-      <c r="AB21" s="143"/>
-      <c r="AC21" s="143"/>
-      <c r="AD21" s="143"/>
-      <c r="AE21" s="143"/>
-      <c r="AF21" s="143"/>
-      <c r="AG21" s="143"/>
-      <c r="AH21" s="143"/>
-      <c r="AI21" s="143"/>
-      <c r="AJ21" s="195">
-        <f>AJ20+2</f>
-        <v>34</v>
-      </c>
-      <c r="AK21" s="197">
-        <f>AK20+2</f>
-        <v>35</v>
-      </c>
-      <c r="AL21" s="212"/>
-      <c r="AM21" s="212"/>
-      <c r="AN21" s="115"/>
-      <c r="AO21" s="116" t="str">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="AP21" s="114">
+      <c r="D21" s="138"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="139"/>
+      <c r="G21" s="139"/>
+      <c r="H21" s="139"/>
+      <c r="I21" s="139"/>
+      <c r="J21" s="139"/>
+      <c r="K21" s="139"/>
+      <c r="L21" s="139"/>
+      <c r="M21" s="139"/>
+      <c r="N21" s="139"/>
+      <c r="O21" s="139"/>
+      <c r="P21" s="139"/>
+      <c r="Q21" s="139"/>
+      <c r="R21" s="139"/>
+      <c r="S21" s="139"/>
+      <c r="T21" s="139"/>
+      <c r="U21" s="139"/>
+      <c r="V21" s="139"/>
+      <c r="W21" s="139"/>
+      <c r="X21" s="139"/>
+      <c r="Y21" s="139"/>
+      <c r="Z21" s="139"/>
+      <c r="AA21" s="139"/>
+      <c r="AB21" s="139"/>
+      <c r="AC21" s="139"/>
+      <c r="AD21" s="139"/>
+      <c r="AE21" s="139"/>
+      <c r="AF21" s="139"/>
+      <c r="AG21" s="139"/>
+      <c r="AH21" s="139"/>
+      <c r="AI21" s="139"/>
+      <c r="AJ21" s="180">
+        <v>30</v>
+      </c>
+      <c r="AK21" s="182">
+        <v>31</v>
+      </c>
+      <c r="AL21" s="196"/>
+      <c r="AM21" s="196"/>
+      <c r="AO21" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="AP21" s="111">
         <v>0</v>
       </c>
-      <c r="AQ21" s="116">
+      <c r="AQ21" s="112">
         <v>1</v>
       </c>
       <c r="AR21" s="9">
@@ -9059,69 +8963,68 @@
       <c r="AS21" s="9">
         <v>64</v>
       </c>
-      <c r="AT21" s="114">
+      <c r="AT21" s="111">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="122">
-        <f>B21+1</f>
+      <c r="B22" s="118">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="C22" s="119" t="s">
+      <c r="C22" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="142"/>
-      <c r="E22" s="143"/>
-      <c r="F22" s="143"/>
-      <c r="G22" s="143"/>
-      <c r="H22" s="143"/>
-      <c r="I22" s="143"/>
-      <c r="J22" s="143"/>
-      <c r="K22" s="143"/>
-      <c r="L22" s="143"/>
-      <c r="M22" s="143"/>
-      <c r="N22" s="143"/>
-      <c r="O22" s="143"/>
-      <c r="P22" s="143"/>
-      <c r="Q22" s="143"/>
-      <c r="R22" s="143"/>
-      <c r="S22" s="143"/>
-      <c r="T22" s="143"/>
-      <c r="U22" s="143"/>
-      <c r="V22" s="143"/>
-      <c r="W22" s="143"/>
-      <c r="X22" s="143"/>
-      <c r="Y22" s="143"/>
-      <c r="Z22" s="143"/>
-      <c r="AA22" s="143"/>
-      <c r="AB22" s="143"/>
-      <c r="AC22" s="143"/>
-      <c r="AD22" s="143"/>
-      <c r="AE22" s="143"/>
-      <c r="AF22" s="143"/>
-      <c r="AG22" s="143"/>
-      <c r="AH22" s="143"/>
-      <c r="AI22" s="143"/>
-      <c r="AJ22" s="198">
-        <f>AJ21+2</f>
-        <v>36</v>
-      </c>
-      <c r="AK22" s="199">
-        <f>AK21+2</f>
-        <v>37</v>
-      </c>
-      <c r="AL22" s="212"/>
-      <c r="AM22" s="213"/>
-      <c r="AN22" s="115"/>
-      <c r="AO22" s="116" t="str">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="AP22" s="114">
+      <c r="D22" s="138"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="139"/>
+      <c r="I22" s="139"/>
+      <c r="J22" s="139"/>
+      <c r="K22" s="139"/>
+      <c r="L22" s="139"/>
+      <c r="M22" s="139"/>
+      <c r="N22" s="139"/>
+      <c r="O22" s="139"/>
+      <c r="P22" s="139"/>
+      <c r="Q22" s="139"/>
+      <c r="R22" s="139"/>
+      <c r="S22" s="139"/>
+      <c r="T22" s="139"/>
+      <c r="U22" s="139"/>
+      <c r="V22" s="139"/>
+      <c r="W22" s="139"/>
+      <c r="X22" s="139"/>
+      <c r="Y22" s="139"/>
+      <c r="Z22" s="139"/>
+      <c r="AA22" s="139"/>
+      <c r="AB22" s="139"/>
+      <c r="AC22" s="139"/>
+      <c r="AD22" s="139"/>
+      <c r="AE22" s="139"/>
+      <c r="AF22" s="139"/>
+      <c r="AG22" s="139"/>
+      <c r="AH22" s="139"/>
+      <c r="AI22" s="139"/>
+      <c r="AJ22" s="183">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="AK22" s="184">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="AL22" s="196"/>
+      <c r="AM22" s="197"/>
+      <c r="AO22" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>6C</v>
+      </c>
+      <c r="AP22" s="111">
         <v>0</v>
       </c>
-      <c r="AQ22" s="116">
+      <c r="AQ22" s="112">
         <v>1</v>
       </c>
       <c r="AR22" s="9">
@@ -9130,74 +9033,74 @@
       <c r="AS22" s="9">
         <v>64</v>
       </c>
-      <c r="AT22" s="114">
+      <c r="AT22" s="111">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="120">
-        <f>B22+1</f>
+      <c r="B23" s="116">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="C23" s="121" t="s">
+      <c r="C23" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="142"/>
-      <c r="E23" s="143"/>
-      <c r="F23" s="143"/>
-      <c r="G23" s="143"/>
-      <c r="H23" s="143"/>
-      <c r="I23" s="143"/>
-      <c r="J23" s="143"/>
-      <c r="K23" s="143"/>
-      <c r="L23" s="143"/>
-      <c r="M23" s="143"/>
-      <c r="N23" s="143"/>
-      <c r="O23" s="143"/>
-      <c r="P23" s="143"/>
-      <c r="Q23" s="143"/>
-      <c r="R23" s="143"/>
-      <c r="S23" s="143"/>
-      <c r="T23" s="143"/>
-      <c r="U23" s="143"/>
-      <c r="V23" s="143"/>
-      <c r="W23" s="143"/>
-      <c r="X23" s="143"/>
-      <c r="Y23" s="143"/>
-      <c r="Z23" s="143"/>
-      <c r="AA23" s="143"/>
-      <c r="AB23" s="143"/>
-      <c r="AC23" s="143"/>
-      <c r="AD23" s="143"/>
-      <c r="AE23" s="143"/>
-      <c r="AF23" s="143"/>
-      <c r="AG23" s="143"/>
-      <c r="AH23" s="143"/>
-      <c r="AI23" s="143"/>
-      <c r="AJ23" s="195">
+      <c r="D23" s="138"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="139"/>
+      <c r="G23" s="139"/>
+      <c r="H23" s="139"/>
+      <c r="I23" s="139"/>
+      <c r="J23" s="139"/>
+      <c r="K23" s="139"/>
+      <c r="L23" s="139"/>
+      <c r="M23" s="139"/>
+      <c r="N23" s="139"/>
+      <c r="O23" s="139"/>
+      <c r="P23" s="139"/>
+      <c r="Q23" s="139"/>
+      <c r="R23" s="139"/>
+      <c r="S23" s="139"/>
+      <c r="T23" s="139"/>
+      <c r="U23" s="139"/>
+      <c r="V23" s="139"/>
+      <c r="W23" s="139"/>
+      <c r="X23" s="139"/>
+      <c r="Y23" s="139"/>
+      <c r="Z23" s="139"/>
+      <c r="AA23" s="139"/>
+      <c r="AB23" s="139"/>
+      <c r="AC23" s="139"/>
+      <c r="AD23" s="139"/>
+      <c r="AE23" s="139"/>
+      <c r="AF23" s="139"/>
+      <c r="AG23" s="139"/>
+      <c r="AH23" s="139"/>
+      <c r="AI23" s="139"/>
+      <c r="AJ23" s="180">
         <f>AJ22+2</f>
-        <v>38</v>
-      </c>
-      <c r="AK23" s="196">
+        <v>34</v>
+      </c>
+      <c r="AK23" s="181">
         <f>AJ23+1</f>
-        <v>39</v>
-      </c>
-      <c r="AL23" s="196">
+        <v>35</v>
+      </c>
+      <c r="AL23" s="181">
         <f>AK23+1</f>
-        <v>40</v>
-      </c>
-      <c r="AM23" s="199">
+        <v>36</v>
+      </c>
+      <c r="AM23" s="184">
         <f>AL23+1</f>
-        <v>41</v>
-      </c>
-      <c r="AO23" s="116" t="str">
-        <f t="shared" si="1"/>
-        <v>78</v>
-      </c>
-      <c r="AP23" s="114">
+        <v>37</v>
+      </c>
+      <c r="AO23" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="AP23" s="111">
         <v>0</v>
       </c>
-      <c r="AQ23" s="116">
+      <c r="AQ23" s="112">
         <v>3</v>
       </c>
       <c r="AR23" s="9">
@@ -9206,74 +9109,74 @@
       <c r="AS23" s="9">
         <v>64</v>
       </c>
-      <c r="AT23" s="114">
+      <c r="AT23" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="122">
-        <f>B23+1</f>
+      <c r="B24" s="118">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="C24" s="119" t="s">
+      <c r="C24" s="115" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="146"/>
-      <c r="E24" s="147"/>
-      <c r="F24" s="147"/>
-      <c r="G24" s="147"/>
-      <c r="H24" s="147"/>
-      <c r="I24" s="147"/>
-      <c r="J24" s="147"/>
-      <c r="K24" s="147"/>
-      <c r="L24" s="147"/>
-      <c r="M24" s="147"/>
-      <c r="N24" s="147"/>
-      <c r="O24" s="147"/>
-      <c r="P24" s="147"/>
-      <c r="Q24" s="147"/>
-      <c r="R24" s="147"/>
-      <c r="S24" s="147"/>
-      <c r="T24" s="147"/>
-      <c r="U24" s="147"/>
-      <c r="V24" s="147"/>
-      <c r="W24" s="147"/>
-      <c r="X24" s="147"/>
-      <c r="Y24" s="147"/>
-      <c r="Z24" s="147"/>
-      <c r="AA24" s="147"/>
-      <c r="AB24" s="147"/>
-      <c r="AC24" s="147"/>
-      <c r="AD24" s="147"/>
-      <c r="AE24" s="147"/>
-      <c r="AF24" s="147"/>
-      <c r="AG24" s="147"/>
-      <c r="AH24" s="147"/>
-      <c r="AI24" s="147"/>
-      <c r="AJ24" s="200">
+      <c r="D24" s="142"/>
+      <c r="E24" s="143"/>
+      <c r="F24" s="143"/>
+      <c r="G24" s="143"/>
+      <c r="H24" s="143"/>
+      <c r="I24" s="143"/>
+      <c r="J24" s="143"/>
+      <c r="K24" s="143"/>
+      <c r="L24" s="143"/>
+      <c r="M24" s="143"/>
+      <c r="N24" s="143"/>
+      <c r="O24" s="143"/>
+      <c r="P24" s="143"/>
+      <c r="Q24" s="143"/>
+      <c r="R24" s="143"/>
+      <c r="S24" s="143"/>
+      <c r="T24" s="143"/>
+      <c r="U24" s="143"/>
+      <c r="V24" s="143"/>
+      <c r="W24" s="143"/>
+      <c r="X24" s="143"/>
+      <c r="Y24" s="143"/>
+      <c r="Z24" s="143"/>
+      <c r="AA24" s="143"/>
+      <c r="AB24" s="143"/>
+      <c r="AC24" s="143"/>
+      <c r="AD24" s="143"/>
+      <c r="AE24" s="143"/>
+      <c r="AF24" s="143"/>
+      <c r="AG24" s="143"/>
+      <c r="AH24" s="143"/>
+      <c r="AI24" s="143"/>
+      <c r="AJ24" s="185">
         <f>AJ23+4</f>
-        <v>42</v>
-      </c>
-      <c r="AK24" s="201">
+        <v>38</v>
+      </c>
+      <c r="AK24" s="186">
         <f>AK23+4</f>
-        <v>43</v>
-      </c>
-      <c r="AL24" s="201">
+        <v>39</v>
+      </c>
+      <c r="AL24" s="186">
         <f>AL23+4</f>
-        <v>44</v>
-      </c>
-      <c r="AM24" s="202">
+        <v>40</v>
+      </c>
+      <c r="AM24" s="187">
         <f>AM23+4</f>
-        <v>45</v>
-      </c>
-      <c r="AO24" s="116" t="str">
-        <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="AP24" s="114">
+        <v>41</v>
+      </c>
+      <c r="AO24" s="112" t="str">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="AP24" s="111">
         <v>0</v>
       </c>
-      <c r="AQ24" s="116">
+      <c r="AQ24" s="112">
         <v>3</v>
       </c>
       <c r="AR24" s="9">
@@ -9282,148 +9185,148 @@
       <c r="AS24" s="9">
         <v>64</v>
       </c>
-      <c r="AT24" s="114">
+      <c r="AT24" s="111">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="120">
-        <f>B24+1</f>
+      <c r="B25" s="116">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="C25" s="121" t="s">
+      <c r="C25" s="117" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="148"/>
-      <c r="E25" s="149"/>
-      <c r="F25" s="149"/>
-      <c r="G25" s="149"/>
-      <c r="H25" s="149"/>
-      <c r="I25" s="149"/>
-      <c r="J25" s="149"/>
-      <c r="K25" s="149"/>
-      <c r="L25" s="149"/>
-      <c r="M25" s="149"/>
-      <c r="N25" s="149"/>
-      <c r="O25" s="149"/>
-      <c r="P25" s="149"/>
-      <c r="Q25" s="149"/>
-      <c r="R25" s="149"/>
-      <c r="S25" s="149"/>
-      <c r="T25" s="149"/>
-      <c r="U25" s="149"/>
-      <c r="V25" s="149"/>
-      <c r="W25" s="149"/>
-      <c r="X25" s="149"/>
-      <c r="Y25" s="149"/>
-      <c r="Z25" s="149"/>
-      <c r="AA25" s="149"/>
-      <c r="AB25" s="149"/>
-      <c r="AC25" s="149"/>
-      <c r="AD25" s="149"/>
-      <c r="AE25" s="149"/>
-      <c r="AF25" s="149"/>
-      <c r="AG25" s="149"/>
-      <c r="AH25" s="149"/>
-      <c r="AI25" s="150"/>
-      <c r="AJ25" s="208">
+      <c r="D25" s="144"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
+      <c r="H25" s="145"/>
+      <c r="I25" s="145"/>
+      <c r="J25" s="145"/>
+      <c r="K25" s="145"/>
+      <c r="L25" s="145"/>
+      <c r="M25" s="145"/>
+      <c r="N25" s="145"/>
+      <c r="O25" s="145"/>
+      <c r="P25" s="145"/>
+      <c r="Q25" s="145"/>
+      <c r="R25" s="145"/>
+      <c r="S25" s="145"/>
+      <c r="T25" s="145"/>
+      <c r="U25" s="145"/>
+      <c r="V25" s="145"/>
+      <c r="W25" s="145"/>
+      <c r="X25" s="145"/>
+      <c r="Y25" s="145"/>
+      <c r="Z25" s="145"/>
+      <c r="AA25" s="145"/>
+      <c r="AB25" s="145"/>
+      <c r="AC25" s="145"/>
+      <c r="AD25" s="145"/>
+      <c r="AE25" s="145"/>
+      <c r="AF25" s="145"/>
+      <c r="AG25" s="145"/>
+      <c r="AH25" s="145"/>
+      <c r="AI25" s="146"/>
+      <c r="AJ25" s="193">
         <v>20</v>
       </c>
-      <c r="AO25" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO25" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="AP25" s="191">
+      <c r="AP25" s="177">
         <v>-1</v>
       </c>
-      <c r="AQ25" s="192">
+      <c r="AQ25" s="178">
         <v>-1</v>
       </c>
-      <c r="AR25" s="182">
+      <c r="AR25" s="171">
         <v>-1</v>
       </c>
-      <c r="AS25" s="182">
+      <c r="AS25" s="171">
         <v>-1</v>
       </c>
-      <c r="AT25" s="114">
+      <c r="AT25" s="111">
         <v>-1</v>
       </c>
     </row>
     <row r="26" spans="2:46" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="122">
-        <f>B25+1</f>
+      <c r="B26" s="118">
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="C26" s="119" t="s">
+      <c r="C26" s="115" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="139"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140"/>
-      <c r="G26" s="140"/>
-      <c r="H26" s="140"/>
-      <c r="I26" s="140"/>
-      <c r="J26" s="140"/>
-      <c r="K26" s="140"/>
-      <c r="L26" s="140"/>
-      <c r="M26" s="140"/>
-      <c r="N26" s="140"/>
-      <c r="O26" s="140"/>
-      <c r="P26" s="140"/>
-      <c r="Q26" s="140"/>
-      <c r="R26" s="140"/>
-      <c r="S26" s="140"/>
-      <c r="T26" s="140"/>
-      <c r="U26" s="140"/>
-      <c r="V26" s="140"/>
-      <c r="W26" s="140"/>
-      <c r="X26" s="140"/>
-      <c r="Y26" s="140"/>
-      <c r="Z26" s="140"/>
-      <c r="AA26" s="140"/>
-      <c r="AB26" s="140"/>
-      <c r="AC26" s="140"/>
-      <c r="AD26" s="140"/>
-      <c r="AE26" s="140"/>
-      <c r="AF26" s="140"/>
-      <c r="AG26" s="140"/>
-      <c r="AH26" s="140"/>
-      <c r="AI26" s="141"/>
-      <c r="AJ26" s="211">
+      <c r="D26" s="135"/>
+      <c r="E26" s="136"/>
+      <c r="F26" s="136"/>
+      <c r="G26" s="136"/>
+      <c r="H26" s="136"/>
+      <c r="I26" s="136"/>
+      <c r="J26" s="136"/>
+      <c r="K26" s="136"/>
+      <c r="L26" s="136"/>
+      <c r="M26" s="136"/>
+      <c r="N26" s="136"/>
+      <c r="O26" s="136"/>
+      <c r="P26" s="136"/>
+      <c r="Q26" s="136"/>
+      <c r="R26" s="136"/>
+      <c r="S26" s="136"/>
+      <c r="T26" s="136"/>
+      <c r="U26" s="136"/>
+      <c r="V26" s="136"/>
+      <c r="W26" s="136"/>
+      <c r="X26" s="136"/>
+      <c r="Y26" s="136"/>
+      <c r="Z26" s="136"/>
+      <c r="AA26" s="136"/>
+      <c r="AB26" s="136"/>
+      <c r="AC26" s="136"/>
+      <c r="AD26" s="136"/>
+      <c r="AE26" s="136"/>
+      <c r="AF26" s="136"/>
+      <c r="AG26" s="136"/>
+      <c r="AH26" s="136"/>
+      <c r="AI26" s="137"/>
+      <c r="AJ26" s="195">
         <v>21</v>
       </c>
-      <c r="AO26" s="116" t="str">
-        <f t="shared" si="1"/>
+      <c r="AO26" s="112" t="str">
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
-      <c r="AP26" s="191">
+      <c r="AP26" s="177">
         <v>-1</v>
       </c>
-      <c r="AQ26" s="192">
+      <c r="AQ26" s="178">
         <v>-1</v>
       </c>
-      <c r="AR26" s="182">
+      <c r="AR26" s="171">
         <v>-1</v>
       </c>
-      <c r="AS26" s="182">
+      <c r="AS26" s="171">
         <v>-1</v>
       </c>
-      <c r="AT26" s="114">
+      <c r="AT26" s="111">
         <v>-1</v>
       </c>
     </row>
     <row r="27" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="B27" s="69"/>
-      <c r="C27" s="70" t="s">
+      <c r="B27" s="68"/>
+      <c r="C27" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="28" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="AI28" s="181" t="str">
+      <c r="AI28" s="199" t="str">
         <f>DEC2HEX(MAX(AJ3:AM27)*512,4)</f>
-        <v>5A00</v>
-      </c>
-      <c r="AJ28" s="181"/>
+        <v>5200</v>
+      </c>
+      <c r="AJ28" s="199"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Update 6845 CRTC timing spreadsheet with revised timing values
</commit_message>
<xml_diff>
--- a/6845_crtc_timing.xlsx
+++ b/6845_crtc_timing.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\BBC_Micro\Programs\game_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6029A5-F70D-4D1A-9A48-1AE9C3F18517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1226CE0F-3CD1-402B-9ABD-8EDE2BF02050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{E881977C-AD55-4380-9786-6EB6D25147A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{E881977C-AD55-4380-9786-6EB6D25147A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="118">
   <si>
     <t>6845 CRTC Vertical Rupture Worksheet</t>
   </si>
@@ -353,6 +354,69 @@
   <si>
     <t>Speed</t>
   </si>
+  <si>
+    <t>Sprites</t>
+  </si>
+  <si>
+    <t>AND #00010001b</t>
+  </si>
+  <si>
+    <t>AND #11101110</t>
+  </si>
+  <si>
+    <t>Lookup Table Method</t>
+  </si>
+  <si>
+    <t>Conventional Method</t>
+  </si>
+  <si>
+    <t>Method to shift sprite data 1 pixel to the right</t>
+  </si>
+  <si>
+    <t>LDA pixel_data_table, X</t>
+  </si>
+  <si>
+    <t>LDA pixel_data_0</t>
+  </si>
+  <si>
+    <t>LDX pixel_data_0</t>
+  </si>
+  <si>
+    <t>LDX pixel_data_1</t>
+  </si>
+  <si>
+    <t>ORA pixel_0</t>
+  </si>
+  <si>
+    <t>LDA pixel_data_table + 256, X</t>
+  </si>
+  <si>
+    <t>STA pixel_0</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Cycles</t>
+  </si>
+  <si>
+    <t>4*</t>
+  </si>
+  <si>
+    <t>ASL A</t>
+  </si>
+  <si>
+    <t>LSR A</t>
+  </si>
+  <si>
+    <t>ADC pixel_0</t>
+  </si>
+  <si>
+    <t>LDA pixel_data_1</t>
+  </si>
+  <si>
+    <t>CLC</t>
+  </si>
 </sst>
 </file>
 
@@ -361,7 +425,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,6 +458,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -744,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1327,6 +1400,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1340,6 +1416,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2901,7 +2981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC23565D-C8C0-41CF-B4FA-F791AA87DEFC}">
   <dimension ref="A1:BN41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -3705,7 +3785,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="169" t="str">
-        <f t="shared" ref="C4:L19" si="5">DEC2HEX($B4*512+C$2,4)</f>
+        <f t="shared" ref="C4:F19" si="5">DEC2HEX($B4*512+C$2,4)</f>
         <v>0200</v>
       </c>
       <c r="D4" s="170" t="str">
@@ -14971,7 +15051,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F481C70-9657-4394-93E6-4755D8687536}">
   <dimension ref="B1:AT28"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AK3" sqref="AK3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -14989,14 +15071,14 @@
       <c r="AO1" s="133" t="s">
         <v>79</v>
       </c>
-      <c r="AP1" s="199" t="s">
+      <c r="AP1" s="200" t="s">
         <v>92</v>
       </c>
-      <c r="AQ1" s="200"/>
-      <c r="AR1" s="197" t="s">
+      <c r="AQ1" s="201"/>
+      <c r="AR1" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="AS1" s="198"/>
+      <c r="AS1" s="199"/>
       <c r="AT1" s="135" t="s">
         <v>55</v>
       </c>
@@ -16854,11 +16936,11 @@
       </c>
     </row>
     <row r="28" spans="2:46" x14ac:dyDescent="0.3">
-      <c r="AI28" s="196" t="str">
+      <c r="AI28" s="197" t="str">
         <f>DEC2HEX(MAX(AJ3:AM27)*512,4)</f>
         <v>5200</v>
       </c>
-      <c r="AJ28" s="196"/>
+      <c r="AJ28" s="197"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -16868,4 +16950,609 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{744C020C-2F75-4BCA-8E76-D71B94C1C041}">
+  <dimension ref="A1:O28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="12" width="3.33203125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N2" s="202" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N4" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N5" s="2"/>
+      <c r="O5" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D6" s="21">
+        <v>3</v>
+      </c>
+      <c r="E6" s="21">
+        <v>2</v>
+      </c>
+      <c r="F6" s="21">
+        <v>1</v>
+      </c>
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="196">
+        <v>3</v>
+      </c>
+      <c r="I6" s="196">
+        <v>2</v>
+      </c>
+      <c r="J6" s="196">
+        <v>1</v>
+      </c>
+      <c r="K6" s="196">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>104</v>
+      </c>
+      <c r="O6" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D7" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" s="21">
+        <v>0</v>
+      </c>
+      <c r="H7" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="J7" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="K7" s="196">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>98</v>
+      </c>
+      <c r="O7" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D8" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="21">
+        <v>0</v>
+      </c>
+      <c r="G8" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="J8" s="196">
+        <v>0</v>
+      </c>
+      <c r="K8" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="N8" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D9" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="21">
+        <v>0</v>
+      </c>
+      <c r="F9" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="196">
+        <v>0</v>
+      </c>
+      <c r="J9" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="K9" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="N9" t="s">
+        <v>113</v>
+      </c>
+      <c r="O9" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D10" s="21">
+        <v>0</v>
+      </c>
+      <c r="E10" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="H10" s="196">
+        <v>0</v>
+      </c>
+      <c r="I10" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="J10" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="N10" t="s">
+        <v>113</v>
+      </c>
+      <c r="O10" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
+      <c r="E11" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="H11" s="196">
+        <v>0</v>
+      </c>
+      <c r="I11" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="J11" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="K11" s="203" t="s">
+        <v>110</v>
+      </c>
+      <c r="N11" t="s">
+        <v>109</v>
+      </c>
+      <c r="O11" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D12" s="21">
+        <v>3</v>
+      </c>
+      <c r="E12" s="21">
+        <v>2</v>
+      </c>
+      <c r="F12" s="21">
+        <v>1</v>
+      </c>
+      <c r="G12" s="21">
+        <v>0</v>
+      </c>
+      <c r="H12" s="196">
+        <v>3</v>
+      </c>
+      <c r="I12" s="196">
+        <v>2</v>
+      </c>
+      <c r="J12" s="196">
+        <v>1</v>
+      </c>
+      <c r="K12" s="196">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>116</v>
+      </c>
+      <c r="O12" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D13" s="21">
+        <v>3</v>
+      </c>
+      <c r="E13" s="21">
+        <v>2</v>
+      </c>
+      <c r="F13" s="21">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="H13" s="196">
+        <v>3</v>
+      </c>
+      <c r="I13" s="196">
+        <v>2</v>
+      </c>
+      <c r="J13" s="196">
+        <v>1</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="N13" t="s">
+        <v>99</v>
+      </c>
+      <c r="O13" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D14" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="21">
+        <v>3</v>
+      </c>
+      <c r="F14" s="21">
+        <v>2</v>
+      </c>
+      <c r="G14" s="21">
+        <v>1</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="I14" s="196">
+        <v>3</v>
+      </c>
+      <c r="J14" s="196">
+        <v>2</v>
+      </c>
+      <c r="K14" s="196">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>114</v>
+      </c>
+      <c r="O14" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D15" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="21">
+        <v>3</v>
+      </c>
+      <c r="F15" s="21">
+        <v>2</v>
+      </c>
+      <c r="G15" s="21">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" s="196">
+        <v>3</v>
+      </c>
+      <c r="J15" s="196">
+        <v>2</v>
+      </c>
+      <c r="K15" s="196">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
+        <v>117</v>
+      </c>
+      <c r="O15" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D16" s="21">
+        <v>0</v>
+      </c>
+      <c r="E16" s="21">
+        <v>3</v>
+      </c>
+      <c r="F16" s="21">
+        <v>2</v>
+      </c>
+      <c r="G16" s="21">
+        <v>1</v>
+      </c>
+      <c r="H16" s="196">
+        <v>0</v>
+      </c>
+      <c r="I16" s="196">
+        <v>3</v>
+      </c>
+      <c r="J16" s="196">
+        <v>2</v>
+      </c>
+      <c r="K16" s="196">
+        <v>1</v>
+      </c>
+      <c r="N16" t="s">
+        <v>115</v>
+      </c>
+      <c r="O16" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="O17" s="9">
+        <f>SUM(O6:O16)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="N20" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D22" s="21">
+        <v>3</v>
+      </c>
+      <c r="E22" s="21">
+        <v>2</v>
+      </c>
+      <c r="F22" s="21">
+        <v>1</v>
+      </c>
+      <c r="G22" s="21">
+        <v>0</v>
+      </c>
+      <c r="H22" s="196">
+        <v>3</v>
+      </c>
+      <c r="I22" s="196">
+        <v>2</v>
+      </c>
+      <c r="J22" s="196">
+        <v>1</v>
+      </c>
+      <c r="K22" s="196">
+        <v>0</v>
+      </c>
+      <c r="N22" t="s">
+        <v>105</v>
+      </c>
+      <c r="O22" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D23" s="21">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="H23" s="196">
+        <v>0</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="N23" t="s">
+        <v>108</v>
+      </c>
+      <c r="O23" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D24" s="21">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="H24" s="196">
+        <v>0</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="N24" t="s">
+        <v>109</v>
+      </c>
+      <c r="O24" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D25" s="21">
+        <v>3</v>
+      </c>
+      <c r="E25" s="21">
+        <v>2</v>
+      </c>
+      <c r="F25" s="21">
+        <v>1</v>
+      </c>
+      <c r="G25" s="21">
+        <v>0</v>
+      </c>
+      <c r="H25" s="196">
+        <v>3</v>
+      </c>
+      <c r="I25" s="196">
+        <v>2</v>
+      </c>
+      <c r="J25" s="196">
+        <v>1</v>
+      </c>
+      <c r="K25" s="196">
+        <v>0</v>
+      </c>
+      <c r="N25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O25" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D26" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="21">
+        <v>3</v>
+      </c>
+      <c r="F26" s="21">
+        <v>2</v>
+      </c>
+      <c r="G26" s="21">
+        <v>1</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="I26" s="196">
+        <v>3</v>
+      </c>
+      <c r="J26" s="196">
+        <v>2</v>
+      </c>
+      <c r="K26" s="196">
+        <v>1</v>
+      </c>
+      <c r="N26" t="s">
+        <v>103</v>
+      </c>
+      <c r="O26" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="D27" s="21">
+        <v>0</v>
+      </c>
+      <c r="E27" s="21">
+        <v>3</v>
+      </c>
+      <c r="F27" s="21">
+        <v>2</v>
+      </c>
+      <c r="G27" s="21">
+        <v>1</v>
+      </c>
+      <c r="H27" s="196">
+        <v>0</v>
+      </c>
+      <c r="I27" s="196">
+        <v>3</v>
+      </c>
+      <c r="J27" s="196">
+        <v>2</v>
+      </c>
+      <c r="K27" s="196">
+        <v>1</v>
+      </c>
+      <c r="N27" t="s">
+        <v>107</v>
+      </c>
+      <c r="O27" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="O28" s="9">
+        <f>SUM(O22:O27)</f>
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>